<commit_message>
-change openpushcall nash from 0-8 to 0-11 -bug fixes
</commit_message>
<xml_diff>
--- a/pAd/bin/Debug/Data/SPINRANGES.xlsx
+++ b/pAd/bin/Debug/Data/SPINRANGES.xlsx
@@ -2587,44 +2587,11 @@
     <xf numFmtId="49" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="11" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2641,16 +2608,61 @@
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="10" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2659,22 +2671,10 @@
     <xf numFmtId="0" fontId="10" fillId="22" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3051,8 +3051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DS744"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BO83" sqref="BO83"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC62" sqref="AC62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3062,70 +3062,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="21.1" x14ac:dyDescent="0.35">
-      <c r="A1" s="303"/>
-      <c r="B1" s="303"/>
-      <c r="C1" s="303"/>
-      <c r="D1" s="303"/>
-      <c r="E1" s="303"/>
-      <c r="F1" s="303"/>
-      <c r="G1" s="303"/>
-      <c r="H1" s="303"/>
-      <c r="I1" s="303"/>
-      <c r="J1" s="303"/>
-      <c r="K1" s="303"/>
-      <c r="L1" s="303"/>
-      <c r="M1" s="303"/>
-      <c r="N1" s="303"/>
-      <c r="O1" s="303"/>
-      <c r="P1" s="303"/>
-      <c r="Q1" s="303"/>
-      <c r="R1" s="303"/>
-      <c r="S1" s="303"/>
-      <c r="T1" s="303"/>
-      <c r="U1" s="303"/>
-      <c r="V1" s="303"/>
-      <c r="W1" s="303"/>
-      <c r="X1" s="303"/>
-      <c r="Y1" s="303"/>
-      <c r="Z1" s="303"/>
-      <c r="AA1" s="303"/>
-      <c r="AB1" s="303"/>
-      <c r="AC1" s="303"/>
-      <c r="AD1" s="303"/>
+      <c r="A1" s="298"/>
+      <c r="B1" s="298"/>
+      <c r="C1" s="298"/>
+      <c r="D1" s="298"/>
+      <c r="E1" s="298"/>
+      <c r="F1" s="298"/>
+      <c r="G1" s="298"/>
+      <c r="H1" s="298"/>
+      <c r="I1" s="298"/>
+      <c r="J1" s="298"/>
+      <c r="K1" s="298"/>
+      <c r="L1" s="298"/>
+      <c r="M1" s="298"/>
+      <c r="N1" s="298"/>
+      <c r="O1" s="298"/>
+      <c r="P1" s="298"/>
+      <c r="Q1" s="298"/>
+      <c r="R1" s="298"/>
+      <c r="S1" s="298"/>
+      <c r="T1" s="298"/>
+      <c r="U1" s="298"/>
+      <c r="V1" s="298"/>
+      <c r="W1" s="298"/>
+      <c r="X1" s="298"/>
+      <c r="Y1" s="298"/>
+      <c r="Z1" s="298"/>
+      <c r="AA1" s="298"/>
+      <c r="AB1" s="298"/>
+      <c r="AC1" s="298"/>
+      <c r="AD1" s="298"/>
     </row>
     <row r="17" spans="1:94" ht="20.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="303" t="s">
+      <c r="A17" s="298" t="s">
         <v>137</v>
       </c>
-      <c r="B17" s="303"/>
-      <c r="C17" s="303"/>
-      <c r="D17" s="303"/>
-      <c r="E17" s="303"/>
-      <c r="F17" s="303"/>
-      <c r="G17" s="303"/>
-      <c r="H17" s="303"/>
-      <c r="I17" s="303"/>
-      <c r="J17" s="303"/>
-      <c r="K17" s="303"/>
-      <c r="L17" s="303"/>
-      <c r="M17" s="303"/>
-      <c r="N17" s="303"/>
-      <c r="O17" s="303"/>
-      <c r="P17" s="303"/>
-      <c r="Q17" s="303"/>
-      <c r="R17" s="303"/>
-      <c r="S17" s="303"/>
-      <c r="T17" s="303"/>
-      <c r="U17" s="303"/>
-      <c r="V17" s="303"/>
-      <c r="W17" s="303"/>
-      <c r="X17" s="303"/>
-      <c r="Y17" s="303"/>
-      <c r="Z17" s="303"/>
-      <c r="AA17" s="303"/>
-      <c r="AB17" s="303"/>
-      <c r="AC17" s="303"/>
-      <c r="AD17" s="303"/>
+      <c r="B17" s="298"/>
+      <c r="C17" s="298"/>
+      <c r="D17" s="298"/>
+      <c r="E17" s="298"/>
+      <c r="F17" s="298"/>
+      <c r="G17" s="298"/>
+      <c r="H17" s="298"/>
+      <c r="I17" s="298"/>
+      <c r="J17" s="298"/>
+      <c r="K17" s="298"/>
+      <c r="L17" s="298"/>
+      <c r="M17" s="298"/>
+      <c r="N17" s="298"/>
+      <c r="O17" s="298"/>
+      <c r="P17" s="298"/>
+      <c r="Q17" s="298"/>
+      <c r="R17" s="298"/>
+      <c r="S17" s="298"/>
+      <c r="T17" s="298"/>
+      <c r="U17" s="298"/>
+      <c r="V17" s="298"/>
+      <c r="W17" s="298"/>
+      <c r="X17" s="298"/>
+      <c r="Y17" s="298"/>
+      <c r="Z17" s="298"/>
+      <c r="AA17" s="298"/>
+      <c r="AB17" s="298"/>
+      <c r="AC17" s="298"/>
+      <c r="AD17" s="298"/>
       <c r="AE17" s="66"/>
       <c r="AF17" s="66"/>
       <c r="AG17" s="66"/>
@@ -3192,70 +3192,70 @@
       <c r="CP17" s="66"/>
     </row>
     <row r="18" spans="1:94" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="317" t="s">
+      <c r="A18" s="314" t="s">
         <v>245</v>
       </c>
-      <c r="B18" s="317"/>
-      <c r="C18" s="317"/>
-      <c r="D18" s="317"/>
-      <c r="E18" s="317"/>
-      <c r="F18" s="317"/>
-      <c r="G18" s="317"/>
-      <c r="H18" s="317"/>
-      <c r="I18" s="317"/>
-      <c r="J18" s="317"/>
-      <c r="K18" s="317"/>
-      <c r="L18" s="317"/>
-      <c r="M18" s="317"/>
-      <c r="N18" s="317"/>
-      <c r="P18" s="317" t="s">
+      <c r="B18" s="314"/>
+      <c r="C18" s="314"/>
+      <c r="D18" s="314"/>
+      <c r="E18" s="314"/>
+      <c r="F18" s="314"/>
+      <c r="G18" s="314"/>
+      <c r="H18" s="314"/>
+      <c r="I18" s="314"/>
+      <c r="J18" s="314"/>
+      <c r="K18" s="314"/>
+      <c r="L18" s="314"/>
+      <c r="M18" s="314"/>
+      <c r="N18" s="314"/>
+      <c r="P18" s="314" t="s">
         <v>246</v>
       </c>
-      <c r="Q18" s="317"/>
-      <c r="R18" s="317"/>
-      <c r="S18" s="317"/>
-      <c r="T18" s="317"/>
-      <c r="U18" s="317"/>
-      <c r="V18" s="317"/>
-      <c r="W18" s="317"/>
-      <c r="X18" s="317"/>
-      <c r="Y18" s="317"/>
-      <c r="Z18" s="317"/>
-      <c r="AA18" s="317"/>
-      <c r="AB18" s="317"/>
-      <c r="AC18" s="317"/>
-      <c r="AE18" s="319" t="s">
+      <c r="Q18" s="314"/>
+      <c r="R18" s="314"/>
+      <c r="S18" s="314"/>
+      <c r="T18" s="314"/>
+      <c r="U18" s="314"/>
+      <c r="V18" s="314"/>
+      <c r="W18" s="314"/>
+      <c r="X18" s="314"/>
+      <c r="Y18" s="314"/>
+      <c r="Z18" s="314"/>
+      <c r="AA18" s="314"/>
+      <c r="AB18" s="314"/>
+      <c r="AC18" s="314"/>
+      <c r="AE18" s="305" t="s">
         <v>247</v>
       </c>
-      <c r="AF18" s="319"/>
-      <c r="AG18" s="319"/>
-      <c r="AH18" s="319"/>
-      <c r="AI18" s="319"/>
-      <c r="AJ18" s="319"/>
-      <c r="AK18" s="319"/>
-      <c r="AL18" s="319"/>
-      <c r="AM18" s="319"/>
-      <c r="AN18" s="319"/>
-      <c r="AO18" s="319"/>
-      <c r="AP18" s="319"/>
-      <c r="AQ18" s="319"/>
-      <c r="AR18" s="319"/>
-      <c r="AT18" s="304" t="s">
+      <c r="AF18" s="305"/>
+      <c r="AG18" s="305"/>
+      <c r="AH18" s="305"/>
+      <c r="AI18" s="305"/>
+      <c r="AJ18" s="305"/>
+      <c r="AK18" s="305"/>
+      <c r="AL18" s="305"/>
+      <c r="AM18" s="305"/>
+      <c r="AN18" s="305"/>
+      <c r="AO18" s="305"/>
+      <c r="AP18" s="305"/>
+      <c r="AQ18" s="305"/>
+      <c r="AR18" s="305"/>
+      <c r="AT18" s="313" t="s">
         <v>248</v>
       </c>
-      <c r="AU18" s="304"/>
-      <c r="AV18" s="304"/>
-      <c r="AW18" s="304"/>
-      <c r="AX18" s="304"/>
-      <c r="AY18" s="304"/>
-      <c r="AZ18" s="304"/>
-      <c r="BA18" s="304"/>
-      <c r="BB18" s="304"/>
-      <c r="BC18" s="304"/>
-      <c r="BD18" s="304"/>
-      <c r="BE18" s="304"/>
-      <c r="BF18" s="304"/>
-      <c r="BG18" s="304"/>
+      <c r="AU18" s="313"/>
+      <c r="AV18" s="313"/>
+      <c r="AW18" s="313"/>
+      <c r="AX18" s="313"/>
+      <c r="AY18" s="313"/>
+      <c r="AZ18" s="313"/>
+      <c r="BA18" s="313"/>
+      <c r="BB18" s="313"/>
+      <c r="BC18" s="313"/>
+      <c r="BD18" s="313"/>
+      <c r="BE18" s="313"/>
+      <c r="BF18" s="313"/>
+      <c r="BG18" s="313"/>
     </row>
     <row r="19" spans="1:94" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
@@ -5631,38 +5631,38 @@
     </row>
     <row r="33" spans="16:59" ht="14.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="16:59" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P34" s="317" t="s">
+      <c r="P34" s="314" t="s">
         <v>250</v>
       </c>
-      <c r="Q34" s="317"/>
-      <c r="R34" s="317"/>
-      <c r="S34" s="317"/>
-      <c r="T34" s="317"/>
-      <c r="U34" s="317"/>
-      <c r="V34" s="317"/>
-      <c r="W34" s="317"/>
-      <c r="X34" s="317"/>
-      <c r="Y34" s="317"/>
-      <c r="Z34" s="317"/>
-      <c r="AA34" s="317"/>
-      <c r="AB34" s="317"/>
-      <c r="AC34" s="317"/>
-      <c r="AE34" s="319" t="s">
+      <c r="Q34" s="314"/>
+      <c r="R34" s="314"/>
+      <c r="S34" s="314"/>
+      <c r="T34" s="314"/>
+      <c r="U34" s="314"/>
+      <c r="V34" s="314"/>
+      <c r="W34" s="314"/>
+      <c r="X34" s="314"/>
+      <c r="Y34" s="314"/>
+      <c r="Z34" s="314"/>
+      <c r="AA34" s="314"/>
+      <c r="AB34" s="314"/>
+      <c r="AC34" s="314"/>
+      <c r="AE34" s="305" t="s">
         <v>249</v>
       </c>
-      <c r="AF34" s="319"/>
-      <c r="AG34" s="319"/>
-      <c r="AH34" s="319"/>
-      <c r="AI34" s="319"/>
-      <c r="AJ34" s="319"/>
-      <c r="AK34" s="319"/>
-      <c r="AL34" s="319"/>
-      <c r="AM34" s="319"/>
-      <c r="AN34" s="319"/>
-      <c r="AO34" s="319"/>
-      <c r="AP34" s="319"/>
-      <c r="AQ34" s="319"/>
-      <c r="AR34" s="319"/>
+      <c r="AF34" s="305"/>
+      <c r="AG34" s="305"/>
+      <c r="AH34" s="305"/>
+      <c r="AI34" s="305"/>
+      <c r="AJ34" s="305"/>
+      <c r="AK34" s="305"/>
+      <c r="AL34" s="305"/>
+      <c r="AM34" s="305"/>
+      <c r="AN34" s="305"/>
+      <c r="AO34" s="305"/>
+      <c r="AP34" s="305"/>
+      <c r="AQ34" s="305"/>
+      <c r="AR34" s="305"/>
       <c r="AT34" s="318" t="s">
         <v>138</v>
       </c>
@@ -7545,111 +7545,111 @@
       <c r="BW50" s="66"/>
     </row>
     <row r="51" spans="1:75" ht="14.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P51" s="323" t="s">
+      <c r="P51" s="315" t="s">
         <v>283</v>
       </c>
-      <c r="Q51" s="323"/>
-      <c r="R51" s="323"/>
-      <c r="S51" s="323"/>
-      <c r="T51" s="323"/>
-      <c r="U51" s="323"/>
-      <c r="V51" s="323"/>
-      <c r="W51" s="323"/>
-      <c r="X51" s="323"/>
-      <c r="Y51" s="323"/>
-      <c r="Z51" s="323"/>
-      <c r="AA51" s="323"/>
-      <c r="AB51" s="323"/>
-      <c r="AC51" s="323"/>
-      <c r="AD51" s="323"/>
-      <c r="AE51" s="323"/>
-      <c r="AF51" s="323"/>
-      <c r="AG51" s="323"/>
-      <c r="AH51" s="323"/>
-      <c r="AI51" s="323"/>
-      <c r="AJ51" s="323"/>
-      <c r="AK51" s="323"/>
-      <c r="AL51" s="323"/>
-      <c r="AM51" s="323"/>
-      <c r="AN51" s="323"/>
-      <c r="AO51" s="323"/>
-      <c r="AP51" s="323"/>
-      <c r="AQ51" s="323"/>
-      <c r="AR51" s="323"/>
-      <c r="AS51" s="323"/>
-      <c r="AT51" s="323"/>
-      <c r="AU51" s="323"/>
-      <c r="AV51" s="323"/>
-      <c r="AW51" s="323"/>
-      <c r="AX51" s="323"/>
+      <c r="Q51" s="315"/>
+      <c r="R51" s="315"/>
+      <c r="S51" s="315"/>
+      <c r="T51" s="315"/>
+      <c r="U51" s="315"/>
+      <c r="V51" s="315"/>
+      <c r="W51" s="315"/>
+      <c r="X51" s="315"/>
+      <c r="Y51" s="315"/>
+      <c r="Z51" s="315"/>
+      <c r="AA51" s="315"/>
+      <c r="AB51" s="315"/>
+      <c r="AC51" s="315"/>
+      <c r="AD51" s="315"/>
+      <c r="AE51" s="315"/>
+      <c r="AF51" s="315"/>
+      <c r="AG51" s="315"/>
+      <c r="AH51" s="315"/>
+      <c r="AI51" s="315"/>
+      <c r="AJ51" s="315"/>
+      <c r="AK51" s="315"/>
+      <c r="AL51" s="315"/>
+      <c r="AM51" s="315"/>
+      <c r="AN51" s="315"/>
+      <c r="AO51" s="315"/>
+      <c r="AP51" s="315"/>
+      <c r="AQ51" s="315"/>
+      <c r="AR51" s="315"/>
+      <c r="AS51" s="315"/>
+      <c r="AT51" s="315"/>
+      <c r="AU51" s="315"/>
+      <c r="AV51" s="315"/>
+      <c r="AW51" s="315"/>
+      <c r="AX51" s="315"/>
     </row>
     <row r="52" spans="1:75" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="316" t="s">
+      <c r="A52" s="306" t="s">
         <v>197</v>
       </c>
-      <c r="B52" s="316"/>
-      <c r="C52" s="316"/>
-      <c r="D52" s="316"/>
-      <c r="E52" s="316"/>
-      <c r="F52" s="316"/>
-      <c r="G52" s="316"/>
-      <c r="H52" s="316"/>
-      <c r="I52" s="316"/>
-      <c r="J52" s="316"/>
-      <c r="K52" s="316"/>
-      <c r="L52" s="316"/>
-      <c r="M52" s="316"/>
-      <c r="N52" s="316"/>
-      <c r="P52" s="327" t="s">
+      <c r="B52" s="306"/>
+      <c r="C52" s="306"/>
+      <c r="D52" s="306"/>
+      <c r="E52" s="306"/>
+      <c r="F52" s="306"/>
+      <c r="G52" s="306"/>
+      <c r="H52" s="306"/>
+      <c r="I52" s="306"/>
+      <c r="J52" s="306"/>
+      <c r="K52" s="306"/>
+      <c r="L52" s="306"/>
+      <c r="M52" s="306"/>
+      <c r="N52" s="306"/>
+      <c r="P52" s="309" t="s">
         <v>200</v>
       </c>
-      <c r="Q52" s="327"/>
-      <c r="R52" s="327"/>
-      <c r="S52" s="327"/>
-      <c r="T52" s="327"/>
-      <c r="U52" s="327"/>
-      <c r="V52" s="327"/>
-      <c r="W52" s="327"/>
-      <c r="X52" s="327"/>
-      <c r="Y52" s="327"/>
-      <c r="Z52" s="327"/>
-      <c r="AA52" s="327"/>
-      <c r="AB52" s="327"/>
-      <c r="AC52" s="327"/>
+      <c r="Q52" s="309"/>
+      <c r="R52" s="309"/>
+      <c r="S52" s="309"/>
+      <c r="T52" s="309"/>
+      <c r="U52" s="309"/>
+      <c r="V52" s="309"/>
+      <c r="W52" s="309"/>
+      <c r="X52" s="309"/>
+      <c r="Y52" s="309"/>
+      <c r="Z52" s="309"/>
+      <c r="AA52" s="309"/>
+      <c r="AB52" s="309"/>
+      <c r="AC52" s="309"/>
       <c r="AD52" s="107"/>
-      <c r="AE52" s="327" t="s">
+      <c r="AE52" s="309" t="s">
         <v>201</v>
       </c>
-      <c r="AF52" s="327"/>
-      <c r="AG52" s="327"/>
-      <c r="AH52" s="327"/>
-      <c r="AI52" s="327"/>
-      <c r="AJ52" s="327"/>
-      <c r="AK52" s="327"/>
-      <c r="AL52" s="327"/>
-      <c r="AM52" s="327"/>
-      <c r="AN52" s="327"/>
-      <c r="AO52" s="327"/>
-      <c r="AP52" s="327"/>
-      <c r="AQ52" s="327"/>
-      <c r="AR52" s="327"/>
+      <c r="AF52" s="309"/>
+      <c r="AG52" s="309"/>
+      <c r="AH52" s="309"/>
+      <c r="AI52" s="309"/>
+      <c r="AJ52" s="309"/>
+      <c r="AK52" s="309"/>
+      <c r="AL52" s="309"/>
+      <c r="AM52" s="309"/>
+      <c r="AN52" s="309"/>
+      <c r="AO52" s="309"/>
+      <c r="AP52" s="309"/>
+      <c r="AQ52" s="309"/>
+      <c r="AR52" s="309"/>
       <c r="AS52" s="108"/>
-      <c r="AT52" s="327" t="s">
+      <c r="AT52" s="309" t="s">
         <v>202</v>
       </c>
-      <c r="AU52" s="327"/>
-      <c r="AV52" s="327"/>
-      <c r="AW52" s="327"/>
-      <c r="AX52" s="327"/>
-      <c r="AY52" s="327"/>
-      <c r="AZ52" s="327"/>
-      <c r="BA52" s="327"/>
-      <c r="BB52" s="327"/>
-      <c r="BC52" s="327"/>
-      <c r="BD52" s="327"/>
-      <c r="BE52" s="327"/>
-      <c r="BF52" s="327"/>
-      <c r="BG52" s="327"/>
+      <c r="AU52" s="309"/>
+      <c r="AV52" s="309"/>
+      <c r="AW52" s="309"/>
+      <c r="AX52" s="309"/>
+      <c r="AY52" s="309"/>
+      <c r="AZ52" s="309"/>
+      <c r="BA52" s="309"/>
+      <c r="BB52" s="309"/>
+      <c r="BC52" s="309"/>
+      <c r="BD52" s="309"/>
+      <c r="BE52" s="309"/>
+      <c r="BF52" s="309"/>
+      <c r="BG52" s="309"/>
     </row>
     <row r="53" spans="1:75" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
@@ -7814,22 +7814,22 @@
       <c r="BG53" s="4">
         <v>2</v>
       </c>
-      <c r="BI53" s="304" t="s">
+      <c r="BI53" s="313" t="s">
         <v>164</v>
       </c>
-      <c r="BJ53" s="304"/>
-      <c r="BK53" s="304"/>
-      <c r="BL53" s="304"/>
-      <c r="BM53" s="304"/>
-      <c r="BN53" s="304"/>
-      <c r="BO53" s="304"/>
-      <c r="BP53" s="304"/>
-      <c r="BQ53" s="304"/>
-      <c r="BR53" s="304"/>
-      <c r="BS53" s="304"/>
-      <c r="BT53" s="304"/>
-      <c r="BU53" s="304"/>
-      <c r="BV53" s="304"/>
+      <c r="BJ53" s="313"/>
+      <c r="BK53" s="313"/>
+      <c r="BL53" s="313"/>
+      <c r="BM53" s="313"/>
+      <c r="BN53" s="313"/>
+      <c r="BO53" s="313"/>
+      <c r="BP53" s="313"/>
+      <c r="BQ53" s="313"/>
+      <c r="BR53" s="313"/>
+      <c r="BS53" s="313"/>
+      <c r="BT53" s="313"/>
+      <c r="BU53" s="313"/>
+      <c r="BV53" s="313"/>
     </row>
     <row r="54" spans="1:75" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
@@ -10607,31 +10607,31 @@
       </c>
     </row>
     <row r="67" spans="1:89" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="311" t="s">
+      <c r="A67" s="300" t="s">
         <v>192</v>
       </c>
-      <c r="B67" s="311"/>
-      <c r="C67" s="311"/>
-      <c r="D67" s="312" t="s">
+      <c r="B67" s="300"/>
+      <c r="C67" s="300"/>
+      <c r="D67" s="301" t="s">
         <v>193</v>
       </c>
-      <c r="E67" s="312"/>
-      <c r="F67" s="312"/>
-      <c r="G67" s="313" t="s">
+      <c r="E67" s="301"/>
+      <c r="F67" s="301"/>
+      <c r="G67" s="302" t="s">
         <v>194</v>
       </c>
-      <c r="H67" s="313"/>
-      <c r="I67" s="313"/>
-      <c r="J67" s="314" t="s">
+      <c r="H67" s="302"/>
+      <c r="I67" s="302"/>
+      <c r="J67" s="303" t="s">
         <v>195</v>
       </c>
-      <c r="K67" s="314"/>
-      <c r="L67" s="314"/>
-      <c r="M67" s="315" t="s">
+      <c r="K67" s="303"/>
+      <c r="L67" s="303"/>
+      <c r="M67" s="304" t="s">
         <v>196</v>
       </c>
-      <c r="N67" s="315"/>
-      <c r="O67" s="315"/>
+      <c r="N67" s="304"/>
+      <c r="O67" s="304"/>
       <c r="BI67" s="12" t="s">
         <v>92</v>
       </c>
@@ -10676,153 +10676,153 @@
       </c>
     </row>
     <row r="68" spans="1:89" ht="14.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="BI68" s="311"/>
-      <c r="BJ68" s="311"/>
-      <c r="BK68" s="311"/>
-      <c r="BL68" s="312"/>
-      <c r="BM68" s="312"/>
-      <c r="BN68" s="312"/>
-      <c r="BO68" s="313"/>
-      <c r="BP68" s="313"/>
-      <c r="BQ68" s="313"/>
-      <c r="BR68" s="314"/>
-      <c r="BS68" s="314"/>
-      <c r="BT68" s="314"/>
-      <c r="BU68" s="315"/>
-      <c r="BV68" s="315"/>
-      <c r="BW68" s="315"/>
+      <c r="BI68" s="300"/>
+      <c r="BJ68" s="300"/>
+      <c r="BK68" s="300"/>
+      <c r="BL68" s="301"/>
+      <c r="BM68" s="301"/>
+      <c r="BN68" s="301"/>
+      <c r="BO68" s="302"/>
+      <c r="BP68" s="302"/>
+      <c r="BQ68" s="302"/>
+      <c r="BR68" s="303"/>
+      <c r="BS68" s="303"/>
+      <c r="BT68" s="303"/>
+      <c r="BU68" s="304"/>
+      <c r="BV68" s="304"/>
+      <c r="BW68" s="304"/>
     </row>
     <row r="69" spans="1:89" ht="20.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="303" t="s">
+      <c r="A69" s="298" t="s">
         <v>163</v>
       </c>
-      <c r="B69" s="303"/>
-      <c r="C69" s="303"/>
-      <c r="D69" s="303"/>
-      <c r="E69" s="303"/>
-      <c r="F69" s="303"/>
-      <c r="G69" s="303"/>
-      <c r="H69" s="303"/>
-      <c r="I69" s="303"/>
-      <c r="J69" s="303"/>
-      <c r="K69" s="303"/>
-      <c r="L69" s="303"/>
-      <c r="M69" s="303"/>
-      <c r="N69" s="303"/>
-      <c r="O69" s="303"/>
-      <c r="P69" s="303"/>
-      <c r="Q69" s="303"/>
-      <c r="R69" s="303"/>
-      <c r="S69" s="303"/>
-      <c r="T69" s="303"/>
-      <c r="U69" s="303"/>
-      <c r="V69" s="303"/>
-      <c r="W69" s="303"/>
-      <c r="X69" s="303"/>
-      <c r="Y69" s="303"/>
-      <c r="Z69" s="303"/>
-      <c r="AA69" s="303"/>
-      <c r="AB69" s="303"/>
-      <c r="AC69" s="303"/>
-      <c r="AD69" s="303"/>
+      <c r="B69" s="298"/>
+      <c r="C69" s="298"/>
+      <c r="D69" s="298"/>
+      <c r="E69" s="298"/>
+      <c r="F69" s="298"/>
+      <c r="G69" s="298"/>
+      <c r="H69" s="298"/>
+      <c r="I69" s="298"/>
+      <c r="J69" s="298"/>
+      <c r="K69" s="298"/>
+      <c r="L69" s="298"/>
+      <c r="M69" s="298"/>
+      <c r="N69" s="298"/>
+      <c r="O69" s="298"/>
+      <c r="P69" s="298"/>
+      <c r="Q69" s="298"/>
+      <c r="R69" s="298"/>
+      <c r="S69" s="298"/>
+      <c r="T69" s="298"/>
+      <c r="U69" s="298"/>
+      <c r="V69" s="298"/>
+      <c r="W69" s="298"/>
+      <c r="X69" s="298"/>
+      <c r="Y69" s="298"/>
+      <c r="Z69" s="298"/>
+      <c r="AA69" s="298"/>
+      <c r="AB69" s="298"/>
+      <c r="AC69" s="298"/>
+      <c r="AD69" s="298"/>
     </row>
     <row r="70" spans="1:89" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="316" t="s">
+      <c r="A70" s="306" t="s">
         <v>257</v>
       </c>
-      <c r="B70" s="316"/>
-      <c r="C70" s="316"/>
-      <c r="D70" s="316"/>
-      <c r="E70" s="316"/>
-      <c r="F70" s="316"/>
-      <c r="G70" s="316"/>
-      <c r="H70" s="316"/>
-      <c r="I70" s="316"/>
-      <c r="J70" s="316"/>
-      <c r="K70" s="316"/>
-      <c r="L70" s="316"/>
-      <c r="M70" s="316"/>
-      <c r="N70" s="316"/>
-      <c r="P70" s="304" t="s">
+      <c r="B70" s="306"/>
+      <c r="C70" s="306"/>
+      <c r="D70" s="306"/>
+      <c r="E70" s="306"/>
+      <c r="F70" s="306"/>
+      <c r="G70" s="306"/>
+      <c r="H70" s="306"/>
+      <c r="I70" s="306"/>
+      <c r="J70" s="306"/>
+      <c r="K70" s="306"/>
+      <c r="L70" s="306"/>
+      <c r="M70" s="306"/>
+      <c r="N70" s="306"/>
+      <c r="P70" s="313" t="s">
         <v>258</v>
       </c>
-      <c r="Q70" s="304"/>
-      <c r="R70" s="304"/>
-      <c r="S70" s="304"/>
-      <c r="T70" s="304"/>
-      <c r="U70" s="304"/>
-      <c r="V70" s="304"/>
-      <c r="W70" s="304"/>
-      <c r="X70" s="304"/>
-      <c r="Y70" s="304"/>
-      <c r="Z70" s="304"/>
-      <c r="AA70" s="304"/>
-      <c r="AB70" s="304"/>
-      <c r="AC70" s="304"/>
-      <c r="AE70" s="316" t="s">
+      <c r="Q70" s="313"/>
+      <c r="R70" s="313"/>
+      <c r="S70" s="313"/>
+      <c r="T70" s="313"/>
+      <c r="U70" s="313"/>
+      <c r="V70" s="313"/>
+      <c r="W70" s="313"/>
+      <c r="X70" s="313"/>
+      <c r="Y70" s="313"/>
+      <c r="Z70" s="313"/>
+      <c r="AA70" s="313"/>
+      <c r="AB70" s="313"/>
+      <c r="AC70" s="313"/>
+      <c r="AE70" s="306" t="s">
         <v>259</v>
       </c>
-      <c r="AF70" s="316"/>
-      <c r="AG70" s="316"/>
-      <c r="AH70" s="316"/>
-      <c r="AI70" s="316"/>
-      <c r="AJ70" s="316"/>
-      <c r="AK70" s="316"/>
-      <c r="AL70" s="316"/>
-      <c r="AM70" s="316"/>
-      <c r="AN70" s="316"/>
-      <c r="AO70" s="316"/>
-      <c r="AP70" s="316"/>
-      <c r="AQ70" s="316"/>
-      <c r="AR70" s="316"/>
-      <c r="AT70" s="316" t="s">
+      <c r="AF70" s="306"/>
+      <c r="AG70" s="306"/>
+      <c r="AH70" s="306"/>
+      <c r="AI70" s="306"/>
+      <c r="AJ70" s="306"/>
+      <c r="AK70" s="306"/>
+      <c r="AL70" s="306"/>
+      <c r="AM70" s="306"/>
+      <c r="AN70" s="306"/>
+      <c r="AO70" s="306"/>
+      <c r="AP70" s="306"/>
+      <c r="AQ70" s="306"/>
+      <c r="AR70" s="306"/>
+      <c r="AT70" s="306" t="s">
         <v>260</v>
       </c>
-      <c r="AU70" s="316"/>
-      <c r="AV70" s="316"/>
-      <c r="AW70" s="316"/>
-      <c r="AX70" s="316"/>
-      <c r="AY70" s="316"/>
-      <c r="AZ70" s="316"/>
-      <c r="BA70" s="316"/>
-      <c r="BB70" s="316"/>
-      <c r="BC70" s="316"/>
-      <c r="BD70" s="316"/>
-      <c r="BE70" s="316"/>
-      <c r="BF70" s="316"/>
-      <c r="BG70" s="316"/>
-      <c r="BI70" s="316" t="s">
+      <c r="AU70" s="306"/>
+      <c r="AV70" s="306"/>
+      <c r="AW70" s="306"/>
+      <c r="AX70" s="306"/>
+      <c r="AY70" s="306"/>
+      <c r="AZ70" s="306"/>
+      <c r="BA70" s="306"/>
+      <c r="BB70" s="306"/>
+      <c r="BC70" s="306"/>
+      <c r="BD70" s="306"/>
+      <c r="BE70" s="306"/>
+      <c r="BF70" s="306"/>
+      <c r="BG70" s="306"/>
+      <c r="BI70" s="306" t="s">
         <v>261</v>
       </c>
-      <c r="BJ70" s="316"/>
-      <c r="BK70" s="316"/>
-      <c r="BL70" s="316"/>
-      <c r="BM70" s="316"/>
-      <c r="BN70" s="316"/>
-      <c r="BO70" s="316"/>
-      <c r="BP70" s="316"/>
-      <c r="BQ70" s="316"/>
-      <c r="BR70" s="316"/>
-      <c r="BS70" s="316"/>
-      <c r="BT70" s="316"/>
-      <c r="BU70" s="316"/>
-      <c r="BV70" s="316"/>
-      <c r="BX70" s="316" t="s">
+      <c r="BJ70" s="306"/>
+      <c r="BK70" s="306"/>
+      <c r="BL70" s="306"/>
+      <c r="BM70" s="306"/>
+      <c r="BN70" s="306"/>
+      <c r="BO70" s="306"/>
+      <c r="BP70" s="306"/>
+      <c r="BQ70" s="306"/>
+      <c r="BR70" s="306"/>
+      <c r="BS70" s="306"/>
+      <c r="BT70" s="306"/>
+      <c r="BU70" s="306"/>
+      <c r="BV70" s="306"/>
+      <c r="BX70" s="306" t="s">
         <v>262</v>
       </c>
-      <c r="BY70" s="316"/>
-      <c r="BZ70" s="316"/>
-      <c r="CA70" s="316"/>
-      <c r="CB70" s="316"/>
-      <c r="CC70" s="316"/>
-      <c r="CD70" s="316"/>
-      <c r="CE70" s="316"/>
-      <c r="CF70" s="316"/>
-      <c r="CG70" s="316"/>
-      <c r="CH70" s="316"/>
-      <c r="CI70" s="316"/>
-      <c r="CJ70" s="316"/>
-      <c r="CK70" s="316"/>
+      <c r="BY70" s="306"/>
+      <c r="BZ70" s="306"/>
+      <c r="CA70" s="306"/>
+      <c r="CB70" s="306"/>
+      <c r="CC70" s="306"/>
+      <c r="CD70" s="306"/>
+      <c r="CE70" s="306"/>
+      <c r="CF70" s="306"/>
+      <c r="CG70" s="306"/>
+      <c r="CH70" s="306"/>
+      <c r="CI70" s="306"/>
+      <c r="CJ70" s="306"/>
+      <c r="CK70" s="306"/>
     </row>
     <row r="71" spans="1:89" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
@@ -14369,106 +14369,106 @@
       </c>
     </row>
     <row r="85" spans="1:108" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="322" t="s">
+      <c r="A85" s="307" t="s">
         <v>270</v>
       </c>
-      <c r="B85" s="322"/>
-      <c r="C85" s="322"/>
-      <c r="D85" s="322"/>
-      <c r="E85" s="322"/>
-      <c r="F85" s="322"/>
-      <c r="G85" s="322"/>
-      <c r="H85" s="322"/>
-      <c r="I85" s="322"/>
-      <c r="J85" s="322"/>
-      <c r="K85" s="322"/>
-      <c r="L85" s="322"/>
-      <c r="M85" s="322"/>
-      <c r="N85" s="322"/>
+      <c r="B85" s="307"/>
+      <c r="C85" s="307"/>
+      <c r="D85" s="307"/>
+      <c r="E85" s="307"/>
+      <c r="F85" s="307"/>
+      <c r="G85" s="307"/>
+      <c r="H85" s="307"/>
+      <c r="I85" s="307"/>
+      <c r="J85" s="307"/>
+      <c r="K85" s="307"/>
+      <c r="L85" s="307"/>
+      <c r="M85" s="307"/>
+      <c r="N85" s="307"/>
       <c r="O85" s="208"/>
-      <c r="P85" s="322" t="s">
+      <c r="P85" s="307" t="s">
         <v>271</v>
       </c>
-      <c r="Q85" s="322"/>
-      <c r="R85" s="322"/>
-      <c r="S85" s="322"/>
-      <c r="T85" s="322"/>
-      <c r="U85" s="322"/>
-      <c r="V85" s="322"/>
-      <c r="W85" s="322"/>
-      <c r="X85" s="322"/>
-      <c r="Y85" s="322"/>
-      <c r="Z85" s="322"/>
-      <c r="AA85" s="322"/>
-      <c r="AB85" s="322"/>
-      <c r="AC85" s="322"/>
+      <c r="Q85" s="307"/>
+      <c r="R85" s="307"/>
+      <c r="S85" s="307"/>
+      <c r="T85" s="307"/>
+      <c r="U85" s="307"/>
+      <c r="V85" s="307"/>
+      <c r="W85" s="307"/>
+      <c r="X85" s="307"/>
+      <c r="Y85" s="307"/>
+      <c r="Z85" s="307"/>
+      <c r="AA85" s="307"/>
+      <c r="AB85" s="307"/>
+      <c r="AC85" s="307"/>
       <c r="AD85" s="208"/>
-      <c r="AE85" s="322" t="s">
+      <c r="AE85" s="307" t="s">
         <v>272</v>
       </c>
-      <c r="AF85" s="322"/>
-      <c r="AG85" s="322"/>
-      <c r="AH85" s="322"/>
-      <c r="AI85" s="322"/>
-      <c r="AJ85" s="322"/>
-      <c r="AK85" s="322"/>
-      <c r="AL85" s="322"/>
-      <c r="AM85" s="322"/>
-      <c r="AN85" s="322"/>
-      <c r="AO85" s="322"/>
-      <c r="AP85" s="322"/>
-      <c r="AQ85" s="322"/>
-      <c r="AR85" s="322"/>
-      <c r="AT85" s="322" t="s">
+      <c r="AF85" s="307"/>
+      <c r="AG85" s="307"/>
+      <c r="AH85" s="307"/>
+      <c r="AI85" s="307"/>
+      <c r="AJ85" s="307"/>
+      <c r="AK85" s="307"/>
+      <c r="AL85" s="307"/>
+      <c r="AM85" s="307"/>
+      <c r="AN85" s="307"/>
+      <c r="AO85" s="307"/>
+      <c r="AP85" s="307"/>
+      <c r="AQ85" s="307"/>
+      <c r="AR85" s="307"/>
+      <c r="AT85" s="307" t="s">
         <v>273</v>
       </c>
-      <c r="AU85" s="322"/>
-      <c r="AV85" s="322"/>
-      <c r="AW85" s="322"/>
-      <c r="AX85" s="322"/>
-      <c r="AY85" s="322"/>
-      <c r="AZ85" s="322"/>
-      <c r="BA85" s="322"/>
-      <c r="BB85" s="322"/>
-      <c r="BC85" s="322"/>
-      <c r="BD85" s="322"/>
-      <c r="BE85" s="322"/>
-      <c r="BF85" s="322"/>
-      <c r="BG85" s="322"/>
+      <c r="AU85" s="307"/>
+      <c r="AV85" s="307"/>
+      <c r="AW85" s="307"/>
+      <c r="AX85" s="307"/>
+      <c r="AY85" s="307"/>
+      <c r="AZ85" s="307"/>
+      <c r="BA85" s="307"/>
+      <c r="BB85" s="307"/>
+      <c r="BC85" s="307"/>
+      <c r="BD85" s="307"/>
+      <c r="BE85" s="307"/>
+      <c r="BF85" s="307"/>
+      <c r="BG85" s="307"/>
       <c r="BH85" s="208"/>
-      <c r="BI85" s="322" t="s">
+      <c r="BI85" s="307" t="s">
         <v>274</v>
       </c>
-      <c r="BJ85" s="322"/>
-      <c r="BK85" s="322"/>
-      <c r="BL85" s="322"/>
-      <c r="BM85" s="322"/>
-      <c r="BN85" s="322"/>
-      <c r="BO85" s="322"/>
-      <c r="BP85" s="322"/>
-      <c r="BQ85" s="322"/>
-      <c r="BR85" s="322"/>
-      <c r="BS85" s="322"/>
-      <c r="BT85" s="322"/>
-      <c r="BU85" s="322"/>
-      <c r="BV85" s="322"/>
+      <c r="BJ85" s="307"/>
+      <c r="BK85" s="307"/>
+      <c r="BL85" s="307"/>
+      <c r="BM85" s="307"/>
+      <c r="BN85" s="307"/>
+      <c r="BO85" s="307"/>
+      <c r="BP85" s="307"/>
+      <c r="BQ85" s="307"/>
+      <c r="BR85" s="307"/>
+      <c r="BS85" s="307"/>
+      <c r="BT85" s="307"/>
+      <c r="BU85" s="307"/>
+      <c r="BV85" s="307"/>
       <c r="BW85" s="208"/>
-      <c r="BX85" s="322" t="s">
+      <c r="BX85" s="307" t="s">
         <v>275</v>
       </c>
-      <c r="BY85" s="322"/>
-      <c r="BZ85" s="322"/>
-      <c r="CA85" s="322"/>
-      <c r="CB85" s="322"/>
-      <c r="CC85" s="322"/>
-      <c r="CD85" s="322"/>
-      <c r="CE85" s="322"/>
-      <c r="CF85" s="322"/>
-      <c r="CG85" s="322"/>
-      <c r="CH85" s="322"/>
-      <c r="CI85" s="322"/>
-      <c r="CJ85" s="322"/>
-      <c r="CK85" s="322"/>
+      <c r="BY85" s="307"/>
+      <c r="BZ85" s="307"/>
+      <c r="CA85" s="307"/>
+      <c r="CB85" s="307"/>
+      <c r="CC85" s="307"/>
+      <c r="CD85" s="307"/>
+      <c r="CE85" s="307"/>
+      <c r="CF85" s="307"/>
+      <c r="CG85" s="307"/>
+      <c r="CH85" s="307"/>
+      <c r="CI85" s="307"/>
+      <c r="CJ85" s="307"/>
+      <c r="CK85" s="307"/>
       <c r="CL85" s="211"/>
       <c r="CM85" s="76"/>
       <c r="CN85" s="76"/>
@@ -18370,107 +18370,107 @@
       <c r="DD99" s="76"/>
     </row>
     <row r="100" spans="1:123" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="319" t="s">
+      <c r="A100" s="305" t="s">
         <v>251</v>
       </c>
-      <c r="B100" s="319"/>
-      <c r="C100" s="319"/>
-      <c r="D100" s="319"/>
-      <c r="E100" s="319"/>
-      <c r="F100" s="319"/>
-      <c r="G100" s="319"/>
-      <c r="H100" s="319"/>
-      <c r="I100" s="319"/>
-      <c r="J100" s="319"/>
-      <c r="K100" s="319"/>
-      <c r="L100" s="319"/>
-      <c r="M100" s="319"/>
-      <c r="N100" s="319"/>
+      <c r="B100" s="305"/>
+      <c r="C100" s="305"/>
+      <c r="D100" s="305"/>
+      <c r="E100" s="305"/>
+      <c r="F100" s="305"/>
+      <c r="G100" s="305"/>
+      <c r="H100" s="305"/>
+      <c r="I100" s="305"/>
+      <c r="J100" s="305"/>
+      <c r="K100" s="305"/>
+      <c r="L100" s="305"/>
+      <c r="M100" s="305"/>
+      <c r="N100" s="305"/>
       <c r="O100" s="206"/>
-      <c r="P100" s="319" t="s">
+      <c r="P100" s="305" t="s">
         <v>252</v>
       </c>
-      <c r="Q100" s="319"/>
-      <c r="R100" s="319"/>
-      <c r="S100" s="319"/>
-      <c r="T100" s="319"/>
-      <c r="U100" s="319"/>
-      <c r="V100" s="319"/>
-      <c r="W100" s="319"/>
-      <c r="X100" s="319"/>
-      <c r="Y100" s="319"/>
-      <c r="Z100" s="319"/>
-      <c r="AA100" s="319"/>
-      <c r="AB100" s="319"/>
-      <c r="AC100" s="319"/>
+      <c r="Q100" s="305"/>
+      <c r="R100" s="305"/>
+      <c r="S100" s="305"/>
+      <c r="T100" s="305"/>
+      <c r="U100" s="305"/>
+      <c r="V100" s="305"/>
+      <c r="W100" s="305"/>
+      <c r="X100" s="305"/>
+      <c r="Y100" s="305"/>
+      <c r="Z100" s="305"/>
+      <c r="AA100" s="305"/>
+      <c r="AB100" s="305"/>
+      <c r="AC100" s="305"/>
       <c r="AD100" s="206"/>
-      <c r="AE100" s="319" t="s">
+      <c r="AE100" s="305" t="s">
         <v>253</v>
       </c>
-      <c r="AF100" s="319"/>
-      <c r="AG100" s="319"/>
-      <c r="AH100" s="319"/>
-      <c r="AI100" s="319"/>
-      <c r="AJ100" s="319"/>
-      <c r="AK100" s="319"/>
-      <c r="AL100" s="319"/>
-      <c r="AM100" s="319"/>
-      <c r="AN100" s="319"/>
-      <c r="AO100" s="319"/>
-      <c r="AP100" s="319"/>
-      <c r="AQ100" s="319"/>
-      <c r="AR100" s="319"/>
+      <c r="AF100" s="305"/>
+      <c r="AG100" s="305"/>
+      <c r="AH100" s="305"/>
+      <c r="AI100" s="305"/>
+      <c r="AJ100" s="305"/>
+      <c r="AK100" s="305"/>
+      <c r="AL100" s="305"/>
+      <c r="AM100" s="305"/>
+      <c r="AN100" s="305"/>
+      <c r="AO100" s="305"/>
+      <c r="AP100" s="305"/>
+      <c r="AQ100" s="305"/>
+      <c r="AR100" s="305"/>
       <c r="AS100" s="206"/>
-      <c r="AT100" s="319" t="s">
+      <c r="AT100" s="305" t="s">
         <v>254</v>
       </c>
-      <c r="AU100" s="319"/>
-      <c r="AV100" s="319"/>
-      <c r="AW100" s="319"/>
-      <c r="AX100" s="319"/>
-      <c r="AY100" s="319"/>
-      <c r="AZ100" s="319"/>
-      <c r="BA100" s="319"/>
-      <c r="BB100" s="319"/>
-      <c r="BC100" s="319"/>
-      <c r="BD100" s="319"/>
-      <c r="BE100" s="319"/>
-      <c r="BF100" s="319"/>
-      <c r="BG100" s="319"/>
+      <c r="AU100" s="305"/>
+      <c r="AV100" s="305"/>
+      <c r="AW100" s="305"/>
+      <c r="AX100" s="305"/>
+      <c r="AY100" s="305"/>
+      <c r="AZ100" s="305"/>
+      <c r="BA100" s="305"/>
+      <c r="BB100" s="305"/>
+      <c r="BC100" s="305"/>
+      <c r="BD100" s="305"/>
+      <c r="BE100" s="305"/>
+      <c r="BF100" s="305"/>
+      <c r="BG100" s="305"/>
       <c r="BH100" s="206"/>
-      <c r="BI100" s="319" t="s">
+      <c r="BI100" s="305" t="s">
         <v>255</v>
       </c>
-      <c r="BJ100" s="319"/>
-      <c r="BK100" s="319"/>
-      <c r="BL100" s="319"/>
-      <c r="BM100" s="319"/>
-      <c r="BN100" s="319"/>
-      <c r="BO100" s="319"/>
-      <c r="BP100" s="319"/>
-      <c r="BQ100" s="319"/>
-      <c r="BR100" s="319"/>
-      <c r="BS100" s="319"/>
-      <c r="BT100" s="319"/>
-      <c r="BU100" s="319"/>
-      <c r="BV100" s="319"/>
+      <c r="BJ100" s="305"/>
+      <c r="BK100" s="305"/>
+      <c r="BL100" s="305"/>
+      <c r="BM100" s="305"/>
+      <c r="BN100" s="305"/>
+      <c r="BO100" s="305"/>
+      <c r="BP100" s="305"/>
+      <c r="BQ100" s="305"/>
+      <c r="BR100" s="305"/>
+      <c r="BS100" s="305"/>
+      <c r="BT100" s="305"/>
+      <c r="BU100" s="305"/>
+      <c r="BV100" s="305"/>
       <c r="BW100" s="206"/>
-      <c r="BX100" s="319" t="s">
+      <c r="BX100" s="305" t="s">
         <v>256</v>
       </c>
-      <c r="BY100" s="319"/>
-      <c r="BZ100" s="319"/>
-      <c r="CA100" s="319"/>
-      <c r="CB100" s="319"/>
-      <c r="CC100" s="319"/>
-      <c r="CD100" s="319"/>
-      <c r="CE100" s="319"/>
-      <c r="CF100" s="319"/>
-      <c r="CG100" s="319"/>
-      <c r="CH100" s="319"/>
-      <c r="CI100" s="319"/>
-      <c r="CJ100" s="319"/>
-      <c r="CK100" s="319"/>
+      <c r="BY100" s="305"/>
+      <c r="BZ100" s="305"/>
+      <c r="CA100" s="305"/>
+      <c r="CB100" s="305"/>
+      <c r="CC100" s="305"/>
+      <c r="CD100" s="305"/>
+      <c r="CE100" s="305"/>
+      <c r="CF100" s="305"/>
+      <c r="CG100" s="305"/>
+      <c r="CH100" s="305"/>
+      <c r="CI100" s="305"/>
+      <c r="CJ100" s="305"/>
+      <c r="CK100" s="305"/>
       <c r="CL100" s="211"/>
       <c r="CM100" s="76"/>
       <c r="CN100" s="76"/>
@@ -22597,107 +22597,107 @@
       <c r="DS114" s="206"/>
     </row>
     <row r="115" spans="1:123" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="319" t="s">
+      <c r="A115" s="305" t="s">
         <v>265</v>
       </c>
-      <c r="B115" s="319"/>
-      <c r="C115" s="319"/>
-      <c r="D115" s="319"/>
-      <c r="E115" s="319"/>
-      <c r="F115" s="319"/>
-      <c r="G115" s="319"/>
-      <c r="H115" s="319"/>
-      <c r="I115" s="319"/>
-      <c r="J115" s="319"/>
-      <c r="K115" s="319"/>
-      <c r="L115" s="319"/>
-      <c r="M115" s="319"/>
-      <c r="N115" s="319"/>
+      <c r="B115" s="305"/>
+      <c r="C115" s="305"/>
+      <c r="D115" s="305"/>
+      <c r="E115" s="305"/>
+      <c r="F115" s="305"/>
+      <c r="G115" s="305"/>
+      <c r="H115" s="305"/>
+      <c r="I115" s="305"/>
+      <c r="J115" s="305"/>
+      <c r="K115" s="305"/>
+      <c r="L115" s="305"/>
+      <c r="M115" s="305"/>
+      <c r="N115" s="305"/>
       <c r="O115" s="206"/>
-      <c r="P115" s="319" t="s">
+      <c r="P115" s="305" t="s">
         <v>266</v>
       </c>
-      <c r="Q115" s="319"/>
-      <c r="R115" s="319"/>
-      <c r="S115" s="319"/>
-      <c r="T115" s="319"/>
-      <c r="U115" s="319"/>
-      <c r="V115" s="319"/>
-      <c r="W115" s="319"/>
-      <c r="X115" s="319"/>
-      <c r="Y115" s="319"/>
-      <c r="Z115" s="319"/>
-      <c r="AA115" s="319"/>
-      <c r="AB115" s="319"/>
-      <c r="AC115" s="319"/>
+      <c r="Q115" s="305"/>
+      <c r="R115" s="305"/>
+      <c r="S115" s="305"/>
+      <c r="T115" s="305"/>
+      <c r="U115" s="305"/>
+      <c r="V115" s="305"/>
+      <c r="W115" s="305"/>
+      <c r="X115" s="305"/>
+      <c r="Y115" s="305"/>
+      <c r="Z115" s="305"/>
+      <c r="AA115" s="305"/>
+      <c r="AB115" s="305"/>
+      <c r="AC115" s="305"/>
       <c r="AD115" s="206"/>
-      <c r="AE115" s="319" t="s">
+      <c r="AE115" s="305" t="s">
         <v>267</v>
       </c>
-      <c r="AF115" s="319"/>
-      <c r="AG115" s="319"/>
-      <c r="AH115" s="319"/>
-      <c r="AI115" s="319"/>
-      <c r="AJ115" s="319"/>
-      <c r="AK115" s="319"/>
-      <c r="AL115" s="319"/>
-      <c r="AM115" s="319"/>
-      <c r="AN115" s="319"/>
-      <c r="AO115" s="319"/>
-      <c r="AP115" s="319"/>
-      <c r="AQ115" s="319"/>
-      <c r="AR115" s="319"/>
+      <c r="AF115" s="305"/>
+      <c r="AG115" s="305"/>
+      <c r="AH115" s="305"/>
+      <c r="AI115" s="305"/>
+      <c r="AJ115" s="305"/>
+      <c r="AK115" s="305"/>
+      <c r="AL115" s="305"/>
+      <c r="AM115" s="305"/>
+      <c r="AN115" s="305"/>
+      <c r="AO115" s="305"/>
+      <c r="AP115" s="305"/>
+      <c r="AQ115" s="305"/>
+      <c r="AR115" s="305"/>
       <c r="AS115" s="206"/>
-      <c r="AT115" s="319" t="s">
+      <c r="AT115" s="305" t="s">
         <v>268</v>
       </c>
-      <c r="AU115" s="319"/>
-      <c r="AV115" s="319"/>
-      <c r="AW115" s="319"/>
-      <c r="AX115" s="319"/>
-      <c r="AY115" s="319"/>
-      <c r="AZ115" s="319"/>
-      <c r="BA115" s="319"/>
-      <c r="BB115" s="319"/>
-      <c r="BC115" s="319"/>
-      <c r="BD115" s="319"/>
-      <c r="BE115" s="319"/>
-      <c r="BF115" s="319"/>
-      <c r="BG115" s="319"/>
+      <c r="AU115" s="305"/>
+      <c r="AV115" s="305"/>
+      <c r="AW115" s="305"/>
+      <c r="AX115" s="305"/>
+      <c r="AY115" s="305"/>
+      <c r="AZ115" s="305"/>
+      <c r="BA115" s="305"/>
+      <c r="BB115" s="305"/>
+      <c r="BC115" s="305"/>
+      <c r="BD115" s="305"/>
+      <c r="BE115" s="305"/>
+      <c r="BF115" s="305"/>
+      <c r="BG115" s="305"/>
       <c r="BH115" s="206"/>
-      <c r="BI115" s="319" t="s">
+      <c r="BI115" s="305" t="s">
         <v>269</v>
       </c>
-      <c r="BJ115" s="319"/>
-      <c r="BK115" s="319"/>
-      <c r="BL115" s="319"/>
-      <c r="BM115" s="319"/>
-      <c r="BN115" s="319"/>
-      <c r="BO115" s="319"/>
-      <c r="BP115" s="319"/>
-      <c r="BQ115" s="319"/>
-      <c r="BR115" s="319"/>
-      <c r="BS115" s="319"/>
-      <c r="BT115" s="319"/>
-      <c r="BU115" s="319"/>
-      <c r="BV115" s="319"/>
+      <c r="BJ115" s="305"/>
+      <c r="BK115" s="305"/>
+      <c r="BL115" s="305"/>
+      <c r="BM115" s="305"/>
+      <c r="BN115" s="305"/>
+      <c r="BO115" s="305"/>
+      <c r="BP115" s="305"/>
+      <c r="BQ115" s="305"/>
+      <c r="BR115" s="305"/>
+      <c r="BS115" s="305"/>
+      <c r="BT115" s="305"/>
+      <c r="BU115" s="305"/>
+      <c r="BV115" s="305"/>
       <c r="BW115" s="206"/>
-      <c r="BX115" s="319" t="s">
+      <c r="BX115" s="305" t="s">
         <v>264</v>
       </c>
-      <c r="BY115" s="319"/>
-      <c r="BZ115" s="319"/>
-      <c r="CA115" s="319"/>
-      <c r="CB115" s="319"/>
-      <c r="CC115" s="319"/>
-      <c r="CD115" s="319"/>
-      <c r="CE115" s="319"/>
-      <c r="CF115" s="319"/>
-      <c r="CG115" s="319"/>
-      <c r="CH115" s="319"/>
-      <c r="CI115" s="319"/>
-      <c r="CJ115" s="319"/>
-      <c r="CK115" s="319"/>
+      <c r="BY115" s="305"/>
+      <c r="BZ115" s="305"/>
+      <c r="CA115" s="305"/>
+      <c r="CB115" s="305"/>
+      <c r="CC115" s="305"/>
+      <c r="CD115" s="305"/>
+      <c r="CE115" s="305"/>
+      <c r="CF115" s="305"/>
+      <c r="CG115" s="305"/>
+      <c r="CH115" s="305"/>
+      <c r="CI115" s="305"/>
+      <c r="CJ115" s="305"/>
+      <c r="CK115" s="305"/>
       <c r="CL115" s="206"/>
       <c r="CM115" s="206"/>
       <c r="CN115" s="206"/>
@@ -26824,102 +26824,102 @@
       <c r="DS129" s="206"/>
     </row>
     <row r="130" spans="1:123" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="316" t="s">
+      <c r="A130" s="306" t="s">
         <v>276</v>
       </c>
-      <c r="B130" s="316"/>
-      <c r="C130" s="316"/>
-      <c r="D130" s="316"/>
-      <c r="E130" s="316"/>
-      <c r="F130" s="316"/>
-      <c r="G130" s="316"/>
-      <c r="H130" s="316"/>
-      <c r="I130" s="316"/>
-      <c r="J130" s="316"/>
-      <c r="K130" s="316"/>
-      <c r="L130" s="316"/>
-      <c r="M130" s="316"/>
-      <c r="N130" s="316"/>
-      <c r="P130" s="304" t="s">
+      <c r="B130" s="306"/>
+      <c r="C130" s="306"/>
+      <c r="D130" s="306"/>
+      <c r="E130" s="306"/>
+      <c r="F130" s="306"/>
+      <c r="G130" s="306"/>
+      <c r="H130" s="306"/>
+      <c r="I130" s="306"/>
+      <c r="J130" s="306"/>
+      <c r="K130" s="306"/>
+      <c r="L130" s="306"/>
+      <c r="M130" s="306"/>
+      <c r="N130" s="306"/>
+      <c r="P130" s="313" t="s">
         <v>277</v>
       </c>
-      <c r="Q130" s="304"/>
-      <c r="R130" s="304"/>
-      <c r="S130" s="304"/>
-      <c r="T130" s="304"/>
-      <c r="U130" s="304"/>
-      <c r="V130" s="304"/>
-      <c r="W130" s="304"/>
-      <c r="X130" s="304"/>
-      <c r="Y130" s="304"/>
-      <c r="Z130" s="304"/>
-      <c r="AA130" s="304"/>
-      <c r="AB130" s="304"/>
-      <c r="AC130" s="304"/>
-      <c r="AE130" s="316" t="s">
+      <c r="Q130" s="313"/>
+      <c r="R130" s="313"/>
+      <c r="S130" s="313"/>
+      <c r="T130" s="313"/>
+      <c r="U130" s="313"/>
+      <c r="V130" s="313"/>
+      <c r="W130" s="313"/>
+      <c r="X130" s="313"/>
+      <c r="Y130" s="313"/>
+      <c r="Z130" s="313"/>
+      <c r="AA130" s="313"/>
+      <c r="AB130" s="313"/>
+      <c r="AC130" s="313"/>
+      <c r="AE130" s="306" t="s">
         <v>278</v>
       </c>
-      <c r="AF130" s="316"/>
-      <c r="AG130" s="316"/>
-      <c r="AH130" s="316"/>
-      <c r="AI130" s="316"/>
-      <c r="AJ130" s="316"/>
-      <c r="AK130" s="316"/>
-      <c r="AL130" s="316"/>
-      <c r="AM130" s="316"/>
-      <c r="AN130" s="316"/>
-      <c r="AO130" s="316"/>
-      <c r="AP130" s="316"/>
-      <c r="AQ130" s="316"/>
-      <c r="AR130" s="316"/>
-      <c r="AT130" s="316" t="s">
+      <c r="AF130" s="306"/>
+      <c r="AG130" s="306"/>
+      <c r="AH130" s="306"/>
+      <c r="AI130" s="306"/>
+      <c r="AJ130" s="306"/>
+      <c r="AK130" s="306"/>
+      <c r="AL130" s="306"/>
+      <c r="AM130" s="306"/>
+      <c r="AN130" s="306"/>
+      <c r="AO130" s="306"/>
+      <c r="AP130" s="306"/>
+      <c r="AQ130" s="306"/>
+      <c r="AR130" s="306"/>
+      <c r="AT130" s="306" t="s">
         <v>279</v>
       </c>
-      <c r="AU130" s="316"/>
-      <c r="AV130" s="316"/>
-      <c r="AW130" s="316"/>
-      <c r="AX130" s="316"/>
-      <c r="AY130" s="316"/>
-      <c r="AZ130" s="316"/>
-      <c r="BA130" s="316"/>
-      <c r="BB130" s="316"/>
-      <c r="BC130" s="316"/>
-      <c r="BD130" s="316"/>
-      <c r="BE130" s="316"/>
-      <c r="BF130" s="316"/>
-      <c r="BG130" s="316"/>
-      <c r="BI130" s="316" t="s">
+      <c r="AU130" s="306"/>
+      <c r="AV130" s="306"/>
+      <c r="AW130" s="306"/>
+      <c r="AX130" s="306"/>
+      <c r="AY130" s="306"/>
+      <c r="AZ130" s="306"/>
+      <c r="BA130" s="306"/>
+      <c r="BB130" s="306"/>
+      <c r="BC130" s="306"/>
+      <c r="BD130" s="306"/>
+      <c r="BE130" s="306"/>
+      <c r="BF130" s="306"/>
+      <c r="BG130" s="306"/>
+      <c r="BI130" s="306" t="s">
         <v>280</v>
       </c>
-      <c r="BJ130" s="316"/>
-      <c r="BK130" s="316"/>
-      <c r="BL130" s="316"/>
-      <c r="BM130" s="316"/>
-      <c r="BN130" s="316"/>
-      <c r="BO130" s="316"/>
-      <c r="BP130" s="316"/>
-      <c r="BQ130" s="316"/>
-      <c r="BR130" s="316"/>
-      <c r="BS130" s="316"/>
-      <c r="BT130" s="316"/>
-      <c r="BU130" s="316"/>
-      <c r="BV130" s="316"/>
-      <c r="BX130" s="316" t="s">
+      <c r="BJ130" s="306"/>
+      <c r="BK130" s="306"/>
+      <c r="BL130" s="306"/>
+      <c r="BM130" s="306"/>
+      <c r="BN130" s="306"/>
+      <c r="BO130" s="306"/>
+      <c r="BP130" s="306"/>
+      <c r="BQ130" s="306"/>
+      <c r="BR130" s="306"/>
+      <c r="BS130" s="306"/>
+      <c r="BT130" s="306"/>
+      <c r="BU130" s="306"/>
+      <c r="BV130" s="306"/>
+      <c r="BX130" s="306" t="s">
         <v>281</v>
       </c>
-      <c r="BY130" s="316"/>
-      <c r="BZ130" s="316"/>
-      <c r="CA130" s="316"/>
-      <c r="CB130" s="316"/>
-      <c r="CC130" s="316"/>
-      <c r="CD130" s="316"/>
-      <c r="CE130" s="316"/>
-      <c r="CF130" s="316"/>
-      <c r="CG130" s="316"/>
-      <c r="CH130" s="316"/>
-      <c r="CI130" s="316"/>
-      <c r="CJ130" s="316"/>
-      <c r="CK130" s="316"/>
+      <c r="BY130" s="306"/>
+      <c r="BZ130" s="306"/>
+      <c r="CA130" s="306"/>
+      <c r="CB130" s="306"/>
+      <c r="CC130" s="306"/>
+      <c r="CD130" s="306"/>
+      <c r="CE130" s="306"/>
+      <c r="CF130" s="306"/>
+      <c r="CG130" s="306"/>
+      <c r="CH130" s="306"/>
+      <c r="CI130" s="306"/>
+      <c r="CJ130" s="306"/>
+      <c r="CK130" s="306"/>
       <c r="CL130" s="206"/>
       <c r="CM130" s="206"/>
       <c r="CN130" s="206"/>
@@ -30976,71 +30976,71 @@
       <c r="DS144" s="206"/>
     </row>
     <row r="145" spans="1:60" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="304" t="s">
+      <c r="A145" s="313" t="s">
         <v>198</v>
       </c>
-      <c r="B145" s="304"/>
-      <c r="C145" s="304"/>
-      <c r="D145" s="304"/>
-      <c r="E145" s="304"/>
-      <c r="F145" s="304"/>
-      <c r="G145" s="304"/>
-      <c r="H145" s="304"/>
-      <c r="I145" s="304"/>
-      <c r="J145" s="304"/>
-      <c r="K145" s="304"/>
-      <c r="L145" s="304"/>
-      <c r="M145" s="304"/>
-      <c r="N145" s="304"/>
-      <c r="P145" s="325" t="s">
+      <c r="B145" s="313"/>
+      <c r="C145" s="313"/>
+      <c r="D145" s="313"/>
+      <c r="E145" s="313"/>
+      <c r="F145" s="313"/>
+      <c r="G145" s="313"/>
+      <c r="H145" s="313"/>
+      <c r="I145" s="313"/>
+      <c r="J145" s="313"/>
+      <c r="K145" s="313"/>
+      <c r="L145" s="313"/>
+      <c r="M145" s="313"/>
+      <c r="N145" s="313"/>
+      <c r="P145" s="308" t="s">
         <v>236</v>
       </c>
-      <c r="Q145" s="325"/>
-      <c r="R145" s="325"/>
-      <c r="S145" s="325"/>
-      <c r="T145" s="325"/>
-      <c r="U145" s="325"/>
-      <c r="V145" s="325"/>
-      <c r="W145" s="325"/>
-      <c r="X145" s="325"/>
-      <c r="Y145" s="325"/>
-      <c r="Z145" s="325"/>
-      <c r="AA145" s="325"/>
-      <c r="AB145" s="325"/>
-      <c r="AC145" s="325"/>
+      <c r="Q145" s="308"/>
+      <c r="R145" s="308"/>
+      <c r="S145" s="308"/>
+      <c r="T145" s="308"/>
+      <c r="U145" s="308"/>
+      <c r="V145" s="308"/>
+      <c r="W145" s="308"/>
+      <c r="X145" s="308"/>
+      <c r="Y145" s="308"/>
+      <c r="Z145" s="308"/>
+      <c r="AA145" s="308"/>
+      <c r="AB145" s="308"/>
+      <c r="AC145" s="308"/>
       <c r="AD145"/>
-      <c r="AE145" s="325" t="s">
+      <c r="AE145" s="308" t="s">
         <v>237</v>
       </c>
-      <c r="AF145" s="325"/>
-      <c r="AG145" s="325"/>
-      <c r="AH145" s="325"/>
-      <c r="AI145" s="325"/>
-      <c r="AJ145" s="325"/>
-      <c r="AK145" s="325"/>
-      <c r="AL145" s="325"/>
-      <c r="AM145" s="325"/>
-      <c r="AN145" s="325"/>
-      <c r="AO145" s="325"/>
-      <c r="AP145" s="325"/>
-      <c r="AQ145" s="325"/>
-      <c r="AR145" s="325"/>
-      <c r="AT145" s="325" t="s">
+      <c r="AF145" s="308"/>
+      <c r="AG145" s="308"/>
+      <c r="AH145" s="308"/>
+      <c r="AI145" s="308"/>
+      <c r="AJ145" s="308"/>
+      <c r="AK145" s="308"/>
+      <c r="AL145" s="308"/>
+      <c r="AM145" s="308"/>
+      <c r="AN145" s="308"/>
+      <c r="AO145" s="308"/>
+      <c r="AP145" s="308"/>
+      <c r="AQ145" s="308"/>
+      <c r="AR145" s="308"/>
+      <c r="AT145" s="308" t="s">
         <v>238</v>
       </c>
-      <c r="AU145" s="325"/>
-      <c r="AV145" s="325"/>
-      <c r="AW145" s="325"/>
-      <c r="AX145" s="325"/>
-      <c r="AY145" s="325"/>
-      <c r="AZ145" s="325"/>
-      <c r="BA145" s="325"/>
-      <c r="BB145" s="325"/>
-      <c r="BC145" s="325"/>
-      <c r="BD145" s="325"/>
-      <c r="BE145" s="325"/>
-      <c r="BF145" s="325"/>
-      <c r="BG145" s="325"/>
+      <c r="AU145" s="308"/>
+      <c r="AV145" s="308"/>
+      <c r="AW145" s="308"/>
+      <c r="AX145" s="308"/>
+      <c r="AY145" s="308"/>
+      <c r="AZ145" s="308"/>
+      <c r="BA145" s="308"/>
+      <c r="BB145" s="308"/>
+      <c r="BC145" s="308"/>
+      <c r="BD145" s="308"/>
+      <c r="BE145" s="308"/>
+      <c r="BF145" s="308"/>
+      <c r="BG145" s="308"/>
     </row>
     <row r="146" spans="1:60" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1"/>
@@ -33434,191 +33434,191 @@
       </c>
     </row>
     <row r="160" spans="1:60" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="311" t="s">
+      <c r="A160" s="300" t="s">
         <v>199</v>
       </c>
-      <c r="B160" s="311"/>
-      <c r="C160" s="311"/>
-      <c r="D160" s="312" t="s">
+      <c r="B160" s="300"/>
+      <c r="C160" s="300"/>
+      <c r="D160" s="301" t="s">
         <v>193</v>
       </c>
-      <c r="E160" s="312"/>
-      <c r="F160" s="312"/>
-      <c r="G160" s="313" t="s">
+      <c r="E160" s="301"/>
+      <c r="F160" s="301"/>
+      <c r="G160" s="302" t="s">
         <v>194</v>
       </c>
-      <c r="H160" s="313"/>
-      <c r="I160" s="313"/>
-      <c r="J160" s="314" t="s">
+      <c r="H160" s="302"/>
+      <c r="I160" s="302"/>
+      <c r="J160" s="303" t="s">
         <v>195</v>
       </c>
-      <c r="K160" s="314"/>
-      <c r="L160" s="314"/>
-      <c r="M160" s="315" t="s">
+      <c r="K160" s="303"/>
+      <c r="L160" s="303"/>
+      <c r="M160" s="304" t="s">
         <v>196</v>
       </c>
-      <c r="N160" s="315"/>
-      <c r="O160" s="315"/>
-      <c r="P160" s="309" t="s">
+      <c r="N160" s="304"/>
+      <c r="O160" s="304"/>
+      <c r="P160" s="321" t="s">
         <v>187</v>
       </c>
-      <c r="Q160" s="309"/>
-      <c r="R160" s="309"/>
-      <c r="S160" s="310" t="s">
+      <c r="Q160" s="321"/>
+      <c r="R160" s="321"/>
+      <c r="S160" s="311" t="s">
         <v>188</v>
       </c>
-      <c r="T160" s="310"/>
-      <c r="U160" s="310"/>
-      <c r="V160" s="308" t="s">
+      <c r="T160" s="311"/>
+      <c r="U160" s="311"/>
+      <c r="V160" s="312" t="s">
         <v>189</v>
       </c>
-      <c r="W160" s="308"/>
-      <c r="X160" s="308"/>
-      <c r="Y160" s="306" t="s">
+      <c r="W160" s="312"/>
+      <c r="X160" s="312"/>
+      <c r="Y160" s="319" t="s">
         <v>190</v>
       </c>
-      <c r="Z160" s="306"/>
-      <c r="AA160" s="306"/>
-      <c r="AB160" s="307" t="s">
+      <c r="Z160" s="319"/>
+      <c r="AA160" s="319"/>
+      <c r="AB160" s="320" t="s">
         <v>191</v>
       </c>
-      <c r="AC160" s="307"/>
-      <c r="AD160" s="307"/>
-      <c r="AE160" s="309" t="s">
+      <c r="AC160" s="320"/>
+      <c r="AD160" s="320"/>
+      <c r="AE160" s="321" t="s">
         <v>187</v>
       </c>
-      <c r="AF160" s="309"/>
-      <c r="AG160" s="309"/>
-      <c r="AH160" s="310" t="s">
+      <c r="AF160" s="321"/>
+      <c r="AG160" s="321"/>
+      <c r="AH160" s="311" t="s">
         <v>188</v>
       </c>
-      <c r="AI160" s="310"/>
-      <c r="AJ160" s="310"/>
-      <c r="AK160" s="308" t="s">
+      <c r="AI160" s="311"/>
+      <c r="AJ160" s="311"/>
+      <c r="AK160" s="312" t="s">
         <v>189</v>
       </c>
-      <c r="AL160" s="308"/>
-      <c r="AM160" s="308"/>
-      <c r="AN160" s="306" t="s">
+      <c r="AL160" s="312"/>
+      <c r="AM160" s="312"/>
+      <c r="AN160" s="319" t="s">
         <v>190</v>
       </c>
-      <c r="AO160" s="306"/>
-      <c r="AP160" s="306"/>
-      <c r="AQ160" s="307" t="s">
+      <c r="AO160" s="319"/>
+      <c r="AP160" s="319"/>
+      <c r="AQ160" s="320" t="s">
         <v>191</v>
       </c>
-      <c r="AR160" s="307"/>
-      <c r="AS160" s="307"/>
-      <c r="AT160" s="309" t="s">
+      <c r="AR160" s="320"/>
+      <c r="AS160" s="320"/>
+      <c r="AT160" s="321" t="s">
         <v>187</v>
       </c>
-      <c r="AU160" s="309"/>
-      <c r="AV160" s="309"/>
-      <c r="AW160" s="310" t="s">
+      <c r="AU160" s="321"/>
+      <c r="AV160" s="321"/>
+      <c r="AW160" s="311" t="s">
         <v>188</v>
       </c>
-      <c r="AX160" s="310"/>
-      <c r="AY160" s="310"/>
-      <c r="AZ160" s="308" t="s">
+      <c r="AX160" s="311"/>
+      <c r="AY160" s="311"/>
+      <c r="AZ160" s="312" t="s">
         <v>189</v>
       </c>
-      <c r="BA160" s="308"/>
-      <c r="BB160" s="308"/>
-      <c r="BC160" s="306" t="s">
+      <c r="BA160" s="312"/>
+      <c r="BB160" s="312"/>
+      <c r="BC160" s="319" t="s">
         <v>190</v>
       </c>
-      <c r="BD160" s="306"/>
-      <c r="BE160" s="306"/>
-      <c r="BF160" s="307" t="s">
+      <c r="BD160" s="319"/>
+      <c r="BE160" s="319"/>
+      <c r="BF160" s="320" t="s">
         <v>191</v>
       </c>
-      <c r="BG160" s="307"/>
-      <c r="BH160" s="307"/>
+      <c r="BG160" s="320"/>
+      <c r="BH160" s="320"/>
     </row>
     <row r="161" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="324" t="s">
+      <c r="A161" s="310" t="s">
         <v>285</v>
       </c>
-      <c r="B161" s="324"/>
-      <c r="C161" s="324"/>
-      <c r="D161" s="324"/>
-      <c r="E161" s="324"/>
-      <c r="F161" s="324"/>
-      <c r="G161" s="324"/>
-      <c r="H161" s="324"/>
-      <c r="I161" s="324"/>
-      <c r="J161" s="324"/>
-      <c r="K161" s="324"/>
-      <c r="L161" s="324"/>
-      <c r="M161" s="324"/>
-      <c r="N161" s="324"/>
+      <c r="B161" s="310"/>
+      <c r="C161" s="310"/>
+      <c r="D161" s="310"/>
+      <c r="E161" s="310"/>
+      <c r="F161" s="310"/>
+      <c r="G161" s="310"/>
+      <c r="H161" s="310"/>
+      <c r="I161" s="310"/>
+      <c r="J161" s="310"/>
+      <c r="K161" s="310"/>
+      <c r="L161" s="310"/>
+      <c r="M161" s="310"/>
+      <c r="N161" s="310"/>
       <c r="O161"/>
-      <c r="P161" s="300" t="s">
+      <c r="P161" s="322" t="s">
         <v>284</v>
       </c>
-      <c r="Q161" s="300"/>
-      <c r="R161" s="300"/>
-      <c r="S161" s="300"/>
-      <c r="T161" s="300"/>
-      <c r="U161" s="300"/>
-      <c r="V161" s="300"/>
-      <c r="W161" s="300"/>
-      <c r="X161" s="300"/>
-      <c r="Y161" s="300"/>
-      <c r="Z161" s="300"/>
-      <c r="AA161" s="300"/>
-      <c r="AB161" s="300"/>
-      <c r="AC161" s="300"/>
-      <c r="AE161" s="300" t="s">
+      <c r="Q161" s="322"/>
+      <c r="R161" s="322"/>
+      <c r="S161" s="322"/>
+      <c r="T161" s="322"/>
+      <c r="U161" s="322"/>
+      <c r="V161" s="322"/>
+      <c r="W161" s="322"/>
+      <c r="X161" s="322"/>
+      <c r="Y161" s="322"/>
+      <c r="Z161" s="322"/>
+      <c r="AA161" s="322"/>
+      <c r="AB161" s="322"/>
+      <c r="AC161" s="322"/>
+      <c r="AE161" s="322" t="s">
         <v>286</v>
       </c>
-      <c r="AF161" s="300"/>
-      <c r="AG161" s="300"/>
-      <c r="AH161" s="300"/>
-      <c r="AI161" s="300"/>
-      <c r="AJ161" s="300"/>
-      <c r="AK161" s="300"/>
-      <c r="AL161" s="300"/>
-      <c r="AM161" s="300"/>
-      <c r="AN161" s="300"/>
-      <c r="AO161" s="300"/>
-      <c r="AP161" s="300"/>
-      <c r="AQ161" s="300"/>
-      <c r="AR161" s="300"/>
+      <c r="AF161" s="322"/>
+      <c r="AG161" s="322"/>
+      <c r="AH161" s="322"/>
+      <c r="AI161" s="322"/>
+      <c r="AJ161" s="322"/>
+      <c r="AK161" s="322"/>
+      <c r="AL161" s="322"/>
+      <c r="AM161" s="322"/>
+      <c r="AN161" s="322"/>
+      <c r="AO161" s="322"/>
+      <c r="AP161" s="322"/>
+      <c r="AQ161" s="322"/>
+      <c r="AR161" s="322"/>
       <c r="AS161"/>
-      <c r="AT161" s="300" t="s">
+      <c r="AT161" s="322" t="s">
         <v>263</v>
       </c>
-      <c r="AU161" s="300"/>
-      <c r="AV161" s="300"/>
-      <c r="AW161" s="300"/>
-      <c r="AX161" s="300"/>
-      <c r="AY161" s="300"/>
-      <c r="AZ161" s="300"/>
-      <c r="BA161" s="300"/>
-      <c r="BB161" s="300"/>
-      <c r="BC161" s="300"/>
-      <c r="BD161" s="300"/>
-      <c r="BE161" s="300"/>
-      <c r="BF161" s="300"/>
-      <c r="BG161" s="300"/>
+      <c r="AU161" s="322"/>
+      <c r="AV161" s="322"/>
+      <c r="AW161" s="322"/>
+      <c r="AX161" s="322"/>
+      <c r="AY161" s="322"/>
+      <c r="AZ161" s="322"/>
+      <c r="BA161" s="322"/>
+      <c r="BB161" s="322"/>
+      <c r="BC161" s="322"/>
+      <c r="BD161" s="322"/>
+      <c r="BE161" s="322"/>
+      <c r="BF161" s="322"/>
+      <c r="BG161" s="322"/>
       <c r="BH161"/>
-      <c r="BI161" s="300" t="s">
+      <c r="BI161" s="322" t="s">
         <v>287</v>
       </c>
-      <c r="BJ161" s="300"/>
-      <c r="BK161" s="300"/>
-      <c r="BL161" s="300"/>
-      <c r="BM161" s="300"/>
-      <c r="BN161" s="300"/>
-      <c r="BO161" s="300"/>
-      <c r="BP161" s="300"/>
-      <c r="BQ161" s="300"/>
-      <c r="BR161" s="300"/>
-      <c r="BS161" s="300"/>
-      <c r="BT161" s="300"/>
-      <c r="BU161" s="300"/>
-      <c r="BV161" s="300"/>
+      <c r="BJ161" s="322"/>
+      <c r="BK161" s="322"/>
+      <c r="BL161" s="322"/>
+      <c r="BM161" s="322"/>
+      <c r="BN161" s="322"/>
+      <c r="BO161" s="322"/>
+      <c r="BP161" s="322"/>
+      <c r="BQ161" s="322"/>
+      <c r="BR161" s="322"/>
+      <c r="BS161" s="322"/>
+      <c r="BT161" s="322"/>
+      <c r="BU161" s="322"/>
+      <c r="BV161" s="322"/>
     </row>
     <row r="162" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1"/>
@@ -36696,22 +36696,22 @@
       <c r="BV176" s="219"/>
     </row>
     <row r="177" spans="1:75" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="326" t="s">
+      <c r="A177" s="299" t="s">
         <v>282</v>
       </c>
-      <c r="B177" s="326"/>
-      <c r="C177" s="326"/>
-      <c r="D177" s="326"/>
-      <c r="E177" s="326"/>
-      <c r="F177" s="326"/>
-      <c r="G177" s="326"/>
-      <c r="H177" s="326"/>
-      <c r="I177" s="326"/>
-      <c r="J177" s="326"/>
-      <c r="K177" s="326"/>
-      <c r="L177" s="326"/>
-      <c r="M177" s="326"/>
-      <c r="N177" s="326"/>
+      <c r="B177" s="299"/>
+      <c r="C177" s="299"/>
+      <c r="D177" s="299"/>
+      <c r="E177" s="299"/>
+      <c r="F177" s="299"/>
+      <c r="G177" s="299"/>
+      <c r="H177" s="299"/>
+      <c r="I177" s="299"/>
+      <c r="J177" s="299"/>
+      <c r="K177" s="299"/>
+      <c r="L177" s="299"/>
+      <c r="M177" s="299"/>
+      <c r="N177" s="299"/>
       <c r="O177" s="206"/>
       <c r="P177" s="206"/>
       <c r="Q177" s="206"/>
@@ -38229,31 +38229,31 @@
       <c r="BW191" s="206"/>
     </row>
     <row r="192" spans="1:75" ht="14.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="311" t="s">
+      <c r="A192" s="300" t="s">
         <v>199</v>
       </c>
-      <c r="B192" s="311"/>
-      <c r="C192" s="311"/>
-      <c r="D192" s="312" t="s">
+      <c r="B192" s="300"/>
+      <c r="C192" s="300"/>
+      <c r="D192" s="301" t="s">
         <v>193</v>
       </c>
-      <c r="E192" s="312"/>
-      <c r="F192" s="312"/>
-      <c r="G192" s="313" t="s">
+      <c r="E192" s="301"/>
+      <c r="F192" s="301"/>
+      <c r="G192" s="302" t="s">
         <v>194</v>
       </c>
-      <c r="H192" s="313"/>
-      <c r="I192" s="313"/>
-      <c r="J192" s="314" t="s">
+      <c r="H192" s="302"/>
+      <c r="I192" s="302"/>
+      <c r="J192" s="303" t="s">
         <v>195</v>
       </c>
-      <c r="K192" s="314"/>
-      <c r="L192" s="314"/>
-      <c r="M192" s="315" t="s">
+      <c r="K192" s="303"/>
+      <c r="L192" s="303"/>
+      <c r="M192" s="304" t="s">
         <v>196</v>
       </c>
-      <c r="N192" s="315"/>
-      <c r="O192" s="315"/>
+      <c r="N192" s="304"/>
+      <c r="O192" s="304"/>
       <c r="P192" s="206"/>
       <c r="Q192" s="206"/>
       <c r="R192" s="206"/>
@@ -38316,38 +38316,38 @@
       <c r="BW192" s="206"/>
     </row>
     <row r="193" spans="1:44" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="316" t="s">
+      <c r="A193" s="306" t="s">
         <v>165</v>
       </c>
-      <c r="B193" s="316"/>
-      <c r="C193" s="316"/>
-      <c r="D193" s="316"/>
-      <c r="E193" s="316"/>
-      <c r="F193" s="316"/>
-      <c r="G193" s="316"/>
-      <c r="H193" s="316"/>
-      <c r="I193" s="316"/>
-      <c r="J193" s="316"/>
-      <c r="K193" s="316"/>
-      <c r="L193" s="316"/>
-      <c r="M193" s="316"/>
-      <c r="N193" s="316"/>
-      <c r="P193" s="316" t="s">
+      <c r="B193" s="306"/>
+      <c r="C193" s="306"/>
+      <c r="D193" s="306"/>
+      <c r="E193" s="306"/>
+      <c r="F193" s="306"/>
+      <c r="G193" s="306"/>
+      <c r="H193" s="306"/>
+      <c r="I193" s="306"/>
+      <c r="J193" s="306"/>
+      <c r="K193" s="306"/>
+      <c r="L193" s="306"/>
+      <c r="M193" s="306"/>
+      <c r="N193" s="306"/>
+      <c r="P193" s="306" t="s">
         <v>197</v>
       </c>
-      <c r="Q193" s="316"/>
-      <c r="R193" s="316"/>
-      <c r="S193" s="316"/>
-      <c r="T193" s="316"/>
-      <c r="U193" s="316"/>
-      <c r="V193" s="316"/>
-      <c r="W193" s="316"/>
-      <c r="X193" s="316"/>
-      <c r="Y193" s="316"/>
-      <c r="Z193" s="316"/>
-      <c r="AA193" s="316"/>
-      <c r="AB193" s="316"/>
-      <c r="AC193" s="316"/>
+      <c r="Q193" s="306"/>
+      <c r="R193" s="306"/>
+      <c r="S193" s="306"/>
+      <c r="T193" s="306"/>
+      <c r="U193" s="306"/>
+      <c r="V193" s="306"/>
+      <c r="W193" s="306"/>
+      <c r="X193" s="306"/>
+      <c r="Y193" s="306"/>
+      <c r="Z193" s="306"/>
+      <c r="AA193" s="306"/>
+      <c r="AB193" s="306"/>
+      <c r="AC193" s="306"/>
     </row>
     <row r="194" spans="1:44" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="1"/>
@@ -39548,133 +39548,133 @@
       <c r="AC207" s="146">
         <v>22</v>
       </c>
-      <c r="AD207" s="311" t="s">
+      <c r="AD207" s="300" t="s">
         <v>192</v>
       </c>
-      <c r="AE207" s="311"/>
-      <c r="AF207" s="311"/>
-      <c r="AG207" s="312" t="s">
+      <c r="AE207" s="300"/>
+      <c r="AF207" s="300"/>
+      <c r="AG207" s="301" t="s">
         <v>193</v>
       </c>
-      <c r="AH207" s="312"/>
-      <c r="AI207" s="312"/>
-      <c r="AJ207" s="313" t="s">
+      <c r="AH207" s="301"/>
+      <c r="AI207" s="301"/>
+      <c r="AJ207" s="302" t="s">
         <v>194</v>
       </c>
-      <c r="AK207" s="313"/>
-      <c r="AL207" s="313"/>
-      <c r="AM207" s="314" t="s">
+      <c r="AK207" s="302"/>
+      <c r="AL207" s="302"/>
+      <c r="AM207" s="303" t="s">
         <v>195</v>
       </c>
-      <c r="AN207" s="314"/>
-      <c r="AO207" s="314"/>
-      <c r="AP207" s="315" t="s">
+      <c r="AN207" s="303"/>
+      <c r="AO207" s="303"/>
+      <c r="AP207" s="304" t="s">
         <v>196</v>
       </c>
-      <c r="AQ207" s="315"/>
-      <c r="AR207" s="315"/>
+      <c r="AQ207" s="304"/>
+      <c r="AR207" s="304"/>
     </row>
     <row r="208" spans="1:44" ht="20.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A208" s="303" t="s">
+      <c r="A208" s="298" t="s">
         <v>166</v>
       </c>
-      <c r="B208" s="303"/>
-      <c r="C208" s="303"/>
-      <c r="D208" s="303"/>
-      <c r="E208" s="303"/>
-      <c r="F208" s="303"/>
-      <c r="G208" s="303"/>
-      <c r="H208" s="303"/>
-      <c r="I208" s="303"/>
-      <c r="J208" s="303"/>
-      <c r="K208" s="303"/>
-      <c r="L208" s="303"/>
-      <c r="M208" s="303"/>
-      <c r="N208" s="303"/>
-      <c r="O208" s="303"/>
-      <c r="P208" s="303"/>
-      <c r="Q208" s="303"/>
-      <c r="R208" s="303"/>
-      <c r="S208" s="303"/>
-      <c r="T208" s="303"/>
-      <c r="U208" s="303"/>
-      <c r="V208" s="303"/>
-      <c r="W208" s="303"/>
-      <c r="X208" s="303"/>
-      <c r="Y208" s="303"/>
-      <c r="Z208" s="303"/>
-      <c r="AA208" s="303"/>
-      <c r="AB208" s="303"/>
-      <c r="AC208" s="303"/>
-      <c r="AD208" s="303"/>
+      <c r="B208" s="298"/>
+      <c r="C208" s="298"/>
+      <c r="D208" s="298"/>
+      <c r="E208" s="298"/>
+      <c r="F208" s="298"/>
+      <c r="G208" s="298"/>
+      <c r="H208" s="298"/>
+      <c r="I208" s="298"/>
+      <c r="J208" s="298"/>
+      <c r="K208" s="298"/>
+      <c r="L208" s="298"/>
+      <c r="M208" s="298"/>
+      <c r="N208" s="298"/>
+      <c r="O208" s="298"/>
+      <c r="P208" s="298"/>
+      <c r="Q208" s="298"/>
+      <c r="R208" s="298"/>
+      <c r="S208" s="298"/>
+      <c r="T208" s="298"/>
+      <c r="U208" s="298"/>
+      <c r="V208" s="298"/>
+      <c r="W208" s="298"/>
+      <c r="X208" s="298"/>
+      <c r="Y208" s="298"/>
+      <c r="Z208" s="298"/>
+      <c r="AA208" s="298"/>
+      <c r="AB208" s="298"/>
+      <c r="AC208" s="298"/>
+      <c r="AD208" s="298"/>
     </row>
     <row r="209" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="300" t="s">
+      <c r="A209" s="322" t="s">
         <v>167</v>
       </c>
-      <c r="B209" s="300"/>
-      <c r="C209" s="300"/>
-      <c r="D209" s="300"/>
-      <c r="E209" s="300"/>
-      <c r="F209" s="300"/>
-      <c r="G209" s="300"/>
-      <c r="H209" s="300"/>
-      <c r="I209" s="300"/>
-      <c r="J209" s="300"/>
-      <c r="K209" s="300"/>
-      <c r="L209" s="300"/>
-      <c r="M209" s="300"/>
-      <c r="N209" s="300"/>
+      <c r="B209" s="322"/>
+      <c r="C209" s="322"/>
+      <c r="D209" s="322"/>
+      <c r="E209" s="322"/>
+      <c r="F209" s="322"/>
+      <c r="G209" s="322"/>
+      <c r="H209" s="322"/>
+      <c r="I209" s="322"/>
+      <c r="J209" s="322"/>
+      <c r="K209" s="322"/>
+      <c r="L209" s="322"/>
+      <c r="M209" s="322"/>
+      <c r="N209" s="322"/>
       <c r="O209"/>
-      <c r="P209" s="300" t="s">
+      <c r="P209" s="322" t="s">
         <v>168</v>
       </c>
-      <c r="Q209" s="300"/>
-      <c r="R209" s="300"/>
-      <c r="S209" s="300"/>
-      <c r="T209" s="300"/>
-      <c r="U209" s="300"/>
-      <c r="V209" s="300"/>
-      <c r="W209" s="300"/>
-      <c r="X209" s="300"/>
-      <c r="Y209" s="300"/>
-      <c r="Z209" s="300"/>
-      <c r="AA209" s="300"/>
-      <c r="AB209" s="300"/>
-      <c r="AC209" s="300"/>
-      <c r="AE209" s="305" t="s">
+      <c r="Q209" s="322"/>
+      <c r="R209" s="322"/>
+      <c r="S209" s="322"/>
+      <c r="T209" s="322"/>
+      <c r="U209" s="322"/>
+      <c r="V209" s="322"/>
+      <c r="W209" s="322"/>
+      <c r="X209" s="322"/>
+      <c r="Y209" s="322"/>
+      <c r="Z209" s="322"/>
+      <c r="AA209" s="322"/>
+      <c r="AB209" s="322"/>
+      <c r="AC209" s="322"/>
+      <c r="AE209" s="317" t="s">
         <v>169</v>
       </c>
-      <c r="AF209" s="305"/>
-      <c r="AG209" s="305"/>
-      <c r="AH209" s="305"/>
-      <c r="AI209" s="305"/>
-      <c r="AJ209" s="305"/>
-      <c r="AK209" s="305"/>
-      <c r="AL209" s="305"/>
-      <c r="AM209" s="305"/>
-      <c r="AN209" s="305"/>
-      <c r="AO209" s="305"/>
-      <c r="AP209" s="305"/>
-      <c r="AQ209" s="305"/>
-      <c r="AR209" s="305"/>
+      <c r="AF209" s="317"/>
+      <c r="AG209" s="317"/>
+      <c r="AH209" s="317"/>
+      <c r="AI209" s="317"/>
+      <c r="AJ209" s="317"/>
+      <c r="AK209" s="317"/>
+      <c r="AL209" s="317"/>
+      <c r="AM209" s="317"/>
+      <c r="AN209" s="317"/>
+      <c r="AO209" s="317"/>
+      <c r="AP209" s="317"/>
+      <c r="AQ209" s="317"/>
+      <c r="AR209" s="317"/>
       <c r="AS209"/>
-      <c r="AT209" s="302" t="s">
+      <c r="AT209" s="323" t="s">
         <v>170</v>
       </c>
-      <c r="AU209" s="302"/>
-      <c r="AV209" s="302"/>
-      <c r="AW209" s="302"/>
-      <c r="AX209" s="302"/>
-      <c r="AY209" s="302"/>
-      <c r="AZ209" s="302"/>
-      <c r="BA209" s="302"/>
-      <c r="BB209" s="302"/>
-      <c r="BC209" s="302"/>
-      <c r="BD209" s="302"/>
-      <c r="BE209" s="302"/>
-      <c r="BF209" s="302"/>
-      <c r="BG209" s="302"/>
+      <c r="AU209" s="323"/>
+      <c r="AV209" s="323"/>
+      <c r="AW209" s="323"/>
+      <c r="AX209" s="323"/>
+      <c r="AY209" s="323"/>
+      <c r="AZ209" s="323"/>
+      <c r="BA209" s="323"/>
+      <c r="BB209" s="323"/>
+      <c r="BC209" s="323"/>
+      <c r="BD209" s="323"/>
+      <c r="BE209" s="323"/>
+      <c r="BF209" s="323"/>
+      <c r="BG209" s="323"/>
     </row>
     <row r="210" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="1"/>
@@ -42081,90 +42081,90 @@
       </c>
     </row>
     <row r="224" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A224" s="298" t="s">
+      <c r="A224" s="316" t="s">
         <v>171</v>
       </c>
-      <c r="B224" s="298"/>
-      <c r="C224" s="298"/>
-      <c r="D224" s="298"/>
-      <c r="E224" s="298"/>
-      <c r="F224" s="298"/>
-      <c r="G224" s="298"/>
-      <c r="H224" s="298"/>
-      <c r="I224" s="298"/>
-      <c r="J224" s="298"/>
-      <c r="K224" s="298"/>
-      <c r="L224" s="298"/>
-      <c r="M224" s="298"/>
-      <c r="N224" s="298"/>
+      <c r="B224" s="316"/>
+      <c r="C224" s="316"/>
+      <c r="D224" s="316"/>
+      <c r="E224" s="316"/>
+      <c r="F224" s="316"/>
+      <c r="G224" s="316"/>
+      <c r="H224" s="316"/>
+      <c r="I224" s="316"/>
+      <c r="J224" s="316"/>
+      <c r="K224" s="316"/>
+      <c r="L224" s="316"/>
+      <c r="M224" s="316"/>
+      <c r="N224" s="316"/>
       <c r="O224" s="120"/>
-      <c r="P224" s="302" t="s">
+      <c r="P224" s="323" t="s">
         <v>172</v>
       </c>
-      <c r="Q224" s="302"/>
-      <c r="R224" s="302"/>
-      <c r="S224" s="302"/>
-      <c r="T224" s="302"/>
-      <c r="U224" s="302"/>
-      <c r="V224" s="302"/>
-      <c r="W224" s="302"/>
-      <c r="X224" s="302"/>
-      <c r="Y224" s="302"/>
-      <c r="Z224" s="302"/>
-      <c r="AA224" s="302"/>
-      <c r="AB224" s="302"/>
-      <c r="AC224" s="302"/>
+      <c r="Q224" s="323"/>
+      <c r="R224" s="323"/>
+      <c r="S224" s="323"/>
+      <c r="T224" s="323"/>
+      <c r="U224" s="323"/>
+      <c r="V224" s="323"/>
+      <c r="W224" s="323"/>
+      <c r="X224" s="323"/>
+      <c r="Y224" s="323"/>
+      <c r="Z224" s="323"/>
+      <c r="AA224" s="323"/>
+      <c r="AB224" s="323"/>
+      <c r="AC224" s="323"/>
       <c r="AD224" s="121"/>
-      <c r="AE224" s="302" t="s">
+      <c r="AE224" s="323" t="s">
         <v>173</v>
       </c>
-      <c r="AF224" s="302"/>
-      <c r="AG224" s="302"/>
-      <c r="AH224" s="302"/>
-      <c r="AI224" s="302"/>
-      <c r="AJ224" s="302"/>
-      <c r="AK224" s="302"/>
-      <c r="AL224" s="302"/>
-      <c r="AM224" s="302"/>
-      <c r="AN224" s="302"/>
-      <c r="AO224" s="302"/>
-      <c r="AP224" s="302"/>
-      <c r="AQ224" s="302"/>
-      <c r="AR224" s="302"/>
+      <c r="AF224" s="323"/>
+      <c r="AG224" s="323"/>
+      <c r="AH224" s="323"/>
+      <c r="AI224" s="323"/>
+      <c r="AJ224" s="323"/>
+      <c r="AK224" s="323"/>
+      <c r="AL224" s="323"/>
+      <c r="AM224" s="323"/>
+      <c r="AN224" s="323"/>
+      <c r="AO224" s="323"/>
+      <c r="AP224" s="323"/>
+      <c r="AQ224" s="323"/>
+      <c r="AR224" s="323"/>
       <c r="AS224" s="120"/>
-      <c r="AT224" s="320" t="s">
+      <c r="AT224" s="324" t="s">
         <v>174</v>
       </c>
-      <c r="AU224" s="320"/>
-      <c r="AV224" s="320"/>
-      <c r="AW224" s="320"/>
-      <c r="AX224" s="320"/>
-      <c r="AY224" s="320"/>
-      <c r="AZ224" s="320"/>
-      <c r="BA224" s="320"/>
-      <c r="BB224" s="320"/>
-      <c r="BC224" s="320"/>
-      <c r="BD224" s="320"/>
-      <c r="BE224" s="320"/>
-      <c r="BF224" s="320"/>
-      <c r="BG224" s="320"/>
+      <c r="AU224" s="324"/>
+      <c r="AV224" s="324"/>
+      <c r="AW224" s="324"/>
+      <c r="AX224" s="324"/>
+      <c r="AY224" s="324"/>
+      <c r="AZ224" s="324"/>
+      <c r="BA224" s="324"/>
+      <c r="BB224" s="324"/>
+      <c r="BC224" s="324"/>
+      <c r="BD224" s="324"/>
+      <c r="BE224" s="324"/>
+      <c r="BF224" s="324"/>
+      <c r="BG224" s="324"/>
       <c r="BH224" s="120"/>
-      <c r="BI224" s="321" t="s">
+      <c r="BI224" s="325" t="s">
         <v>175</v>
       </c>
-      <c r="BJ224" s="321"/>
-      <c r="BK224" s="321"/>
-      <c r="BL224" s="321"/>
-      <c r="BM224" s="321"/>
-      <c r="BN224" s="321"/>
-      <c r="BO224" s="321"/>
-      <c r="BP224" s="321"/>
-      <c r="BQ224" s="321"/>
-      <c r="BR224" s="321"/>
-      <c r="BS224" s="321"/>
-      <c r="BT224" s="321"/>
-      <c r="BU224" s="321"/>
-      <c r="BV224" s="321"/>
+      <c r="BJ224" s="325"/>
+      <c r="BK224" s="325"/>
+      <c r="BL224" s="325"/>
+      <c r="BM224" s="325"/>
+      <c r="BN224" s="325"/>
+      <c r="BO224" s="325"/>
+      <c r="BP224" s="325"/>
+      <c r="BQ224" s="325"/>
+      <c r="BR224" s="325"/>
+      <c r="BS224" s="325"/>
+      <c r="BT224" s="325"/>
+      <c r="BU224" s="325"/>
+      <c r="BV224" s="325"/>
     </row>
     <row r="225" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="1"/>
@@ -45181,90 +45181,90 @@
       </c>
     </row>
     <row r="239" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="298" t="s">
+      <c r="A239" s="316" t="s">
         <v>176</v>
       </c>
-      <c r="B239" s="298"/>
-      <c r="C239" s="298"/>
-      <c r="D239" s="298"/>
-      <c r="E239" s="298"/>
-      <c r="F239" s="298"/>
-      <c r="G239" s="298"/>
-      <c r="H239" s="298"/>
-      <c r="I239" s="298"/>
-      <c r="J239" s="298"/>
-      <c r="K239" s="298"/>
-      <c r="L239" s="298"/>
-      <c r="M239" s="298"/>
-      <c r="N239" s="298"/>
+      <c r="B239" s="316"/>
+      <c r="C239" s="316"/>
+      <c r="D239" s="316"/>
+      <c r="E239" s="316"/>
+      <c r="F239" s="316"/>
+      <c r="G239" s="316"/>
+      <c r="H239" s="316"/>
+      <c r="I239" s="316"/>
+      <c r="J239" s="316"/>
+      <c r="K239" s="316"/>
+      <c r="L239" s="316"/>
+      <c r="M239" s="316"/>
+      <c r="N239" s="316"/>
       <c r="O239" s="120"/>
-      <c r="P239" s="298" t="s">
+      <c r="P239" s="316" t="s">
         <v>177</v>
       </c>
-      <c r="Q239" s="298"/>
-      <c r="R239" s="298"/>
-      <c r="S239" s="298"/>
-      <c r="T239" s="298"/>
-      <c r="U239" s="298"/>
-      <c r="V239" s="298"/>
-      <c r="W239" s="298"/>
-      <c r="X239" s="298"/>
-      <c r="Y239" s="298"/>
-      <c r="Z239" s="298"/>
-      <c r="AA239" s="298"/>
-      <c r="AB239" s="298"/>
-      <c r="AC239" s="298"/>
+      <c r="Q239" s="316"/>
+      <c r="R239" s="316"/>
+      <c r="S239" s="316"/>
+      <c r="T239" s="316"/>
+      <c r="U239" s="316"/>
+      <c r="V239" s="316"/>
+      <c r="W239" s="316"/>
+      <c r="X239" s="316"/>
+      <c r="Y239" s="316"/>
+      <c r="Z239" s="316"/>
+      <c r="AA239" s="316"/>
+      <c r="AB239" s="316"/>
+      <c r="AC239" s="316"/>
       <c r="AD239" s="121"/>
-      <c r="AE239" s="298" t="s">
+      <c r="AE239" s="316" t="s">
         <v>178</v>
       </c>
-      <c r="AF239" s="298"/>
-      <c r="AG239" s="298"/>
-      <c r="AH239" s="298"/>
-      <c r="AI239" s="298"/>
-      <c r="AJ239" s="298"/>
-      <c r="AK239" s="298"/>
-      <c r="AL239" s="298"/>
-      <c r="AM239" s="298"/>
-      <c r="AN239" s="298"/>
-      <c r="AO239" s="298"/>
-      <c r="AP239" s="298"/>
-      <c r="AQ239" s="298"/>
-      <c r="AR239" s="298"/>
+      <c r="AF239" s="316"/>
+      <c r="AG239" s="316"/>
+      <c r="AH239" s="316"/>
+      <c r="AI239" s="316"/>
+      <c r="AJ239" s="316"/>
+      <c r="AK239" s="316"/>
+      <c r="AL239" s="316"/>
+      <c r="AM239" s="316"/>
+      <c r="AN239" s="316"/>
+      <c r="AO239" s="316"/>
+      <c r="AP239" s="316"/>
+      <c r="AQ239" s="316"/>
+      <c r="AR239" s="316"/>
       <c r="AS239" s="120"/>
-      <c r="AT239" s="298" t="s">
+      <c r="AT239" s="316" t="s">
         <v>179</v>
       </c>
-      <c r="AU239" s="298"/>
-      <c r="AV239" s="298"/>
-      <c r="AW239" s="298"/>
-      <c r="AX239" s="298"/>
-      <c r="AY239" s="298"/>
-      <c r="AZ239" s="298"/>
-      <c r="BA239" s="298"/>
-      <c r="BB239" s="298"/>
-      <c r="BC239" s="298"/>
-      <c r="BD239" s="298"/>
-      <c r="BE239" s="298"/>
-      <c r="BF239" s="298"/>
-      <c r="BG239" s="298"/>
+      <c r="AU239" s="316"/>
+      <c r="AV239" s="316"/>
+      <c r="AW239" s="316"/>
+      <c r="AX239" s="316"/>
+      <c r="AY239" s="316"/>
+      <c r="AZ239" s="316"/>
+      <c r="BA239" s="316"/>
+      <c r="BB239" s="316"/>
+      <c r="BC239" s="316"/>
+      <c r="BD239" s="316"/>
+      <c r="BE239" s="316"/>
+      <c r="BF239" s="316"/>
+      <c r="BG239" s="316"/>
       <c r="BH239"/>
-      <c r="BI239" s="298" t="s">
+      <c r="BI239" s="316" t="s">
         <v>180</v>
       </c>
-      <c r="BJ239" s="298"/>
-      <c r="BK239" s="298"/>
-      <c r="BL239" s="298"/>
-      <c r="BM239" s="298"/>
-      <c r="BN239" s="298"/>
-      <c r="BO239" s="298"/>
-      <c r="BP239" s="298"/>
-      <c r="BQ239" s="298"/>
-      <c r="BR239" s="298"/>
-      <c r="BS239" s="298"/>
-      <c r="BT239" s="298"/>
-      <c r="BU239" s="298"/>
-      <c r="BV239" s="298"/>
+      <c r="BJ239" s="316"/>
+      <c r="BK239" s="316"/>
+      <c r="BL239" s="316"/>
+      <c r="BM239" s="316"/>
+      <c r="BN239" s="316"/>
+      <c r="BO239" s="316"/>
+      <c r="BP239" s="316"/>
+      <c r="BQ239" s="316"/>
+      <c r="BR239" s="316"/>
+      <c r="BS239" s="316"/>
+      <c r="BT239" s="316"/>
+      <c r="BU239" s="316"/>
+      <c r="BV239" s="316"/>
     </row>
     <row r="240" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="1"/>
@@ -48310,124 +48310,124 @@
       <c r="CZ253" s="297"/>
     </row>
     <row r="254" spans="1:104" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A254" s="298" t="s">
+      <c r="A254" s="316" t="s">
         <v>181</v>
       </c>
-      <c r="B254" s="298"/>
-      <c r="C254" s="298"/>
-      <c r="D254" s="298"/>
-      <c r="E254" s="298"/>
-      <c r="F254" s="298"/>
-      <c r="G254" s="298"/>
-      <c r="H254" s="298"/>
-      <c r="I254" s="298"/>
-      <c r="J254" s="298"/>
-      <c r="K254" s="298"/>
-      <c r="L254" s="298"/>
-      <c r="M254" s="298"/>
-      <c r="N254" s="298"/>
+      <c r="B254" s="316"/>
+      <c r="C254" s="316"/>
+      <c r="D254" s="316"/>
+      <c r="E254" s="316"/>
+      <c r="F254" s="316"/>
+      <c r="G254" s="316"/>
+      <c r="H254" s="316"/>
+      <c r="I254" s="316"/>
+      <c r="J254" s="316"/>
+      <c r="K254" s="316"/>
+      <c r="L254" s="316"/>
+      <c r="M254" s="316"/>
+      <c r="N254" s="316"/>
       <c r="O254" s="120"/>
-      <c r="P254" s="298" t="s">
+      <c r="P254" s="316" t="s">
         <v>182</v>
       </c>
-      <c r="Q254" s="298"/>
-      <c r="R254" s="298"/>
-      <c r="S254" s="298"/>
-      <c r="T254" s="298"/>
-      <c r="U254" s="298"/>
-      <c r="V254" s="298"/>
-      <c r="W254" s="298"/>
-      <c r="X254" s="298"/>
-      <c r="Y254" s="298"/>
-      <c r="Z254" s="298"/>
-      <c r="AA254" s="298"/>
-      <c r="AB254" s="298"/>
-      <c r="AC254" s="298"/>
+      <c r="Q254" s="316"/>
+      <c r="R254" s="316"/>
+      <c r="S254" s="316"/>
+      <c r="T254" s="316"/>
+      <c r="U254" s="316"/>
+      <c r="V254" s="316"/>
+      <c r="W254" s="316"/>
+      <c r="X254" s="316"/>
+      <c r="Y254" s="316"/>
+      <c r="Z254" s="316"/>
+      <c r="AA254" s="316"/>
+      <c r="AB254" s="316"/>
+      <c r="AC254" s="316"/>
       <c r="AD254" s="121"/>
-      <c r="AE254" s="298" t="s">
+      <c r="AE254" s="316" t="s">
         <v>183</v>
       </c>
-      <c r="AF254" s="298"/>
-      <c r="AG254" s="298"/>
-      <c r="AH254" s="298"/>
-      <c r="AI254" s="298"/>
-      <c r="AJ254" s="298"/>
-      <c r="AK254" s="298"/>
-      <c r="AL254" s="298"/>
-      <c r="AM254" s="298"/>
-      <c r="AN254" s="298"/>
-      <c r="AO254" s="298"/>
-      <c r="AP254" s="298"/>
-      <c r="AQ254" s="298"/>
-      <c r="AR254" s="298"/>
+      <c r="AF254" s="316"/>
+      <c r="AG254" s="316"/>
+      <c r="AH254" s="316"/>
+      <c r="AI254" s="316"/>
+      <c r="AJ254" s="316"/>
+      <c r="AK254" s="316"/>
+      <c r="AL254" s="316"/>
+      <c r="AM254" s="316"/>
+      <c r="AN254" s="316"/>
+      <c r="AO254" s="316"/>
+      <c r="AP254" s="316"/>
+      <c r="AQ254" s="316"/>
+      <c r="AR254" s="316"/>
       <c r="AS254"/>
-      <c r="AT254" s="301" t="s">
+      <c r="AT254" s="326" t="s">
         <v>184</v>
       </c>
-      <c r="AU254" s="301"/>
-      <c r="AV254" s="301"/>
-      <c r="AW254" s="301"/>
-      <c r="AX254" s="301"/>
-      <c r="AY254" s="301"/>
-      <c r="AZ254" s="301"/>
-      <c r="BA254" s="301"/>
-      <c r="BB254" s="301"/>
-      <c r="BC254" s="301"/>
-      <c r="BD254" s="301"/>
-      <c r="BE254" s="301"/>
-      <c r="BF254" s="301"/>
-      <c r="BG254" s="301"/>
+      <c r="AU254" s="326"/>
+      <c r="AV254" s="326"/>
+      <c r="AW254" s="326"/>
+      <c r="AX254" s="326"/>
+      <c r="AY254" s="326"/>
+      <c r="AZ254" s="326"/>
+      <c r="BA254" s="326"/>
+      <c r="BB254" s="326"/>
+      <c r="BC254" s="326"/>
+      <c r="BD254" s="326"/>
+      <c r="BE254" s="326"/>
+      <c r="BF254" s="326"/>
+      <c r="BG254" s="326"/>
       <c r="BH254" s="120"/>
-      <c r="BI254" s="298" t="s">
+      <c r="BI254" s="316" t="s">
         <v>185</v>
       </c>
-      <c r="BJ254" s="298"/>
-      <c r="BK254" s="298"/>
-      <c r="BL254" s="298"/>
-      <c r="BM254" s="298"/>
-      <c r="BN254" s="298"/>
-      <c r="BO254" s="298"/>
-      <c r="BP254" s="298"/>
-      <c r="BQ254" s="298"/>
-      <c r="BR254" s="298"/>
-      <c r="BS254" s="298"/>
-      <c r="BT254" s="298"/>
-      <c r="BU254" s="298"/>
-      <c r="BV254" s="298"/>
+      <c r="BJ254" s="316"/>
+      <c r="BK254" s="316"/>
+      <c r="BL254" s="316"/>
+      <c r="BM254" s="316"/>
+      <c r="BN254" s="316"/>
+      <c r="BO254" s="316"/>
+      <c r="BP254" s="316"/>
+      <c r="BQ254" s="316"/>
+      <c r="BR254" s="316"/>
+      <c r="BS254" s="316"/>
+      <c r="BT254" s="316"/>
+      <c r="BU254" s="316"/>
+      <c r="BV254" s="316"/>
       <c r="BW254"/>
-      <c r="BX254" s="298" t="s">
+      <c r="BX254" s="316" t="s">
         <v>359</v>
       </c>
-      <c r="BY254" s="298"/>
-      <c r="BZ254" s="298"/>
-      <c r="CA254" s="298"/>
-      <c r="CB254" s="298"/>
-      <c r="CC254" s="298"/>
-      <c r="CD254" s="298"/>
-      <c r="CE254" s="298"/>
-      <c r="CF254" s="298"/>
-      <c r="CG254" s="298"/>
-      <c r="CH254" s="298"/>
-      <c r="CI254" s="298"/>
-      <c r="CJ254" s="298"/>
-      <c r="CK254" s="298"/>
+      <c r="BY254" s="316"/>
+      <c r="BZ254" s="316"/>
+      <c r="CA254" s="316"/>
+      <c r="CB254" s="316"/>
+      <c r="CC254" s="316"/>
+      <c r="CD254" s="316"/>
+      <c r="CE254" s="316"/>
+      <c r="CF254" s="316"/>
+      <c r="CG254" s="316"/>
+      <c r="CH254" s="316"/>
+      <c r="CI254" s="316"/>
+      <c r="CJ254" s="316"/>
+      <c r="CK254" s="316"/>
       <c r="CL254"/>
-      <c r="CM254" s="305" t="s">
+      <c r="CM254" s="317" t="s">
         <v>186</v>
       </c>
-      <c r="CN254" s="305"/>
-      <c r="CO254" s="305"/>
-      <c r="CP254" s="305"/>
-      <c r="CQ254" s="305"/>
-      <c r="CR254" s="305"/>
-      <c r="CS254" s="305"/>
-      <c r="CT254" s="305"/>
-      <c r="CU254" s="305"/>
-      <c r="CV254" s="305"/>
-      <c r="CW254" s="305"/>
-      <c r="CX254" s="305"/>
-      <c r="CY254" s="305"/>
-      <c r="CZ254" s="305"/>
+      <c r="CN254" s="317"/>
+      <c r="CO254" s="317"/>
+      <c r="CP254" s="317"/>
+      <c r="CQ254" s="317"/>
+      <c r="CR254" s="317"/>
+      <c r="CS254" s="317"/>
+      <c r="CT254" s="317"/>
+      <c r="CU254" s="317"/>
+      <c r="CV254" s="317"/>
+      <c r="CW254" s="317"/>
+      <c r="CX254" s="317"/>
+      <c r="CY254" s="317"/>
+      <c r="CZ254" s="317"/>
     </row>
     <row r="255" spans="1:104" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="1"/>
@@ -52691,37 +52691,37 @@
       <c r="BF270" s="289"/>
       <c r="BG270" s="289"/>
       <c r="BH270" s="66"/>
-      <c r="BI270" s="299" t="s">
+      <c r="BI270" s="327" t="s">
         <v>361</v>
       </c>
-      <c r="BJ270" s="299"/>
-      <c r="BK270" s="299"/>
-      <c r="BL270" s="299"/>
-      <c r="BM270" s="299"/>
-      <c r="BN270" s="299"/>
-      <c r="BO270" s="299"/>
-      <c r="BP270" s="299"/>
-      <c r="BQ270" s="299"/>
-      <c r="BR270" s="299"/>
-      <c r="BS270" s="299"/>
-      <c r="BT270" s="299"/>
-      <c r="BU270" s="299"/>
-      <c r="BV270" s="299"/>
-      <c r="BW270" s="299"/>
-      <c r="BX270" s="299"/>
-      <c r="BY270" s="299"/>
-      <c r="BZ270" s="299"/>
-      <c r="CA270" s="299"/>
-      <c r="CB270" s="299"/>
-      <c r="CC270" s="299"/>
-      <c r="CD270" s="299"/>
-      <c r="CE270" s="299"/>
-      <c r="CF270" s="299"/>
-      <c r="CG270" s="299"/>
-      <c r="CH270" s="299"/>
-      <c r="CI270" s="299"/>
-      <c r="CJ270" s="299"/>
-      <c r="CK270" s="299"/>
+      <c r="BJ270" s="327"/>
+      <c r="BK270" s="327"/>
+      <c r="BL270" s="327"/>
+      <c r="BM270" s="327"/>
+      <c r="BN270" s="327"/>
+      <c r="BO270" s="327"/>
+      <c r="BP270" s="327"/>
+      <c r="BQ270" s="327"/>
+      <c r="BR270" s="327"/>
+      <c r="BS270" s="327"/>
+      <c r="BT270" s="327"/>
+      <c r="BU270" s="327"/>
+      <c r="BV270" s="327"/>
+      <c r="BW270" s="327"/>
+      <c r="BX270" s="327"/>
+      <c r="BY270" s="327"/>
+      <c r="BZ270" s="327"/>
+      <c r="CA270" s="327"/>
+      <c r="CB270" s="327"/>
+      <c r="CC270" s="327"/>
+      <c r="CD270" s="327"/>
+      <c r="CE270" s="327"/>
+      <c r="CF270" s="327"/>
+      <c r="CG270" s="327"/>
+      <c r="CH270" s="327"/>
+      <c r="CI270" s="327"/>
+      <c r="CJ270" s="327"/>
+      <c r="CK270" s="327"/>
       <c r="CL270" s="66"/>
     </row>
     <row r="271" spans="1:104" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -52768,55 +52768,55 @@
       <c r="BF271" s="275"/>
       <c r="BG271" s="275"/>
       <c r="BH271" s="108"/>
-      <c r="BI271" s="298" t="s">
+      <c r="BI271" s="316" t="s">
         <v>360</v>
       </c>
-      <c r="BJ271" s="298"/>
-      <c r="BK271" s="298"/>
-      <c r="BL271" s="298"/>
-      <c r="BM271" s="298"/>
-      <c r="BN271" s="298"/>
-      <c r="BO271" s="298"/>
-      <c r="BP271" s="298"/>
-      <c r="BQ271" s="298"/>
-      <c r="BR271" s="298"/>
-      <c r="BS271" s="298"/>
-      <c r="BT271" s="298"/>
-      <c r="BU271" s="298"/>
-      <c r="BV271" s="298"/>
-      <c r="BX271" s="298" t="s">
+      <c r="BJ271" s="316"/>
+      <c r="BK271" s="316"/>
+      <c r="BL271" s="316"/>
+      <c r="BM271" s="316"/>
+      <c r="BN271" s="316"/>
+      <c r="BO271" s="316"/>
+      <c r="BP271" s="316"/>
+      <c r="BQ271" s="316"/>
+      <c r="BR271" s="316"/>
+      <c r="BS271" s="316"/>
+      <c r="BT271" s="316"/>
+      <c r="BU271" s="316"/>
+      <c r="BV271" s="316"/>
+      <c r="BX271" s="316" t="s">
         <v>288</v>
       </c>
-      <c r="BY271" s="298"/>
-      <c r="BZ271" s="298"/>
-      <c r="CA271" s="298"/>
-      <c r="CB271" s="298"/>
-      <c r="CC271" s="298"/>
-      <c r="CD271" s="298"/>
-      <c r="CE271" s="298"/>
-      <c r="CF271" s="298"/>
-      <c r="CG271" s="298"/>
-      <c r="CH271" s="298"/>
-      <c r="CI271" s="298"/>
-      <c r="CJ271" s="298"/>
-      <c r="CK271" s="298"/>
+      <c r="BY271" s="316"/>
+      <c r="BZ271" s="316"/>
+      <c r="CA271" s="316"/>
+      <c r="CB271" s="316"/>
+      <c r="CC271" s="316"/>
+      <c r="CD271" s="316"/>
+      <c r="CE271" s="316"/>
+      <c r="CF271" s="316"/>
+      <c r="CG271" s="316"/>
+      <c r="CH271" s="316"/>
+      <c r="CI271" s="316"/>
+      <c r="CJ271" s="316"/>
+      <c r="CK271" s="316"/>
       <c r="CL271" s="295"/>
-      <c r="CM271" s="298" t="s">
+      <c r="CM271" s="316" t="s">
         <v>294</v>
       </c>
-      <c r="CN271" s="298"/>
-      <c r="CO271" s="298"/>
-      <c r="CP271" s="298"/>
-      <c r="CQ271" s="298"/>
-      <c r="CR271" s="298"/>
-      <c r="CS271" s="298"/>
-      <c r="CT271" s="298"/>
-      <c r="CU271" s="298"/>
-      <c r="CV271" s="298"/>
-      <c r="CW271" s="298"/>
-      <c r="CX271" s="298"/>
-      <c r="CY271" s="298"/>
-      <c r="CZ271" s="298"/>
+      <c r="CN271" s="316"/>
+      <c r="CO271" s="316"/>
+      <c r="CP271" s="316"/>
+      <c r="CQ271" s="316"/>
+      <c r="CR271" s="316"/>
+      <c r="CS271" s="316"/>
+      <c r="CT271" s="316"/>
+      <c r="CU271" s="316"/>
+      <c r="CV271" s="316"/>
+      <c r="CW271" s="316"/>
+      <c r="CX271" s="316"/>
+      <c r="CY271" s="316"/>
+      <c r="CZ271" s="316"/>
     </row>
     <row r="272" spans="1:104" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="77"/>
@@ -55120,37 +55120,37 @@
       <c r="BF286" s="289"/>
       <c r="BG286" s="289"/>
       <c r="BH286" s="66"/>
-      <c r="BI286" s="299" t="s">
+      <c r="BI286" s="327" t="s">
         <v>362</v>
       </c>
-      <c r="BJ286" s="299"/>
-      <c r="BK286" s="299"/>
-      <c r="BL286" s="299"/>
-      <c r="BM286" s="299"/>
-      <c r="BN286" s="299"/>
-      <c r="BO286" s="299"/>
-      <c r="BP286" s="299"/>
-      <c r="BQ286" s="299"/>
-      <c r="BR286" s="299"/>
-      <c r="BS286" s="299"/>
-      <c r="BT286" s="299"/>
-      <c r="BU286" s="299"/>
-      <c r="BV286" s="299"/>
-      <c r="BW286" s="299"/>
-      <c r="BX286" s="299"/>
-      <c r="BY286" s="299"/>
-      <c r="BZ286" s="299"/>
-      <c r="CA286" s="299"/>
-      <c r="CB286" s="299"/>
-      <c r="CC286" s="299"/>
-      <c r="CD286" s="299"/>
-      <c r="CE286" s="299"/>
-      <c r="CF286" s="299"/>
-      <c r="CG286" s="299"/>
-      <c r="CH286" s="299"/>
-      <c r="CI286" s="299"/>
-      <c r="CJ286" s="299"/>
-      <c r="CK286" s="299"/>
+      <c r="BJ286" s="327"/>
+      <c r="BK286" s="327"/>
+      <c r="BL286" s="327"/>
+      <c r="BM286" s="327"/>
+      <c r="BN286" s="327"/>
+      <c r="BO286" s="327"/>
+      <c r="BP286" s="327"/>
+      <c r="BQ286" s="327"/>
+      <c r="BR286" s="327"/>
+      <c r="BS286" s="327"/>
+      <c r="BT286" s="327"/>
+      <c r="BU286" s="327"/>
+      <c r="BV286" s="327"/>
+      <c r="BW286" s="327"/>
+      <c r="BX286" s="327"/>
+      <c r="BY286" s="327"/>
+      <c r="BZ286" s="327"/>
+      <c r="CA286" s="327"/>
+      <c r="CB286" s="327"/>
+      <c r="CC286" s="327"/>
+      <c r="CD286" s="327"/>
+      <c r="CE286" s="327"/>
+      <c r="CF286" s="327"/>
+      <c r="CG286" s="327"/>
+      <c r="CH286" s="327"/>
+      <c r="CI286" s="327"/>
+      <c r="CJ286" s="327"/>
+      <c r="CK286" s="327"/>
       <c r="CL286" s="296"/>
       <c r="CM286" s="294"/>
       <c r="CN286" s="294"/>
@@ -55196,55 +55196,55 @@
       <c r="BE287" s="275"/>
       <c r="BF287" s="275"/>
       <c r="BG287" s="275"/>
-      <c r="BI287" s="298" t="s">
+      <c r="BI287" s="316" t="s">
         <v>360</v>
       </c>
-      <c r="BJ287" s="298"/>
-      <c r="BK287" s="298"/>
-      <c r="BL287" s="298"/>
-      <c r="BM287" s="298"/>
-      <c r="BN287" s="298"/>
-      <c r="BO287" s="298"/>
-      <c r="BP287" s="298"/>
-      <c r="BQ287" s="298"/>
-      <c r="BR287" s="298"/>
-      <c r="BS287" s="298"/>
-      <c r="BT287" s="298"/>
-      <c r="BU287" s="298"/>
-      <c r="BV287" s="298"/>
-      <c r="BX287" s="298" t="s">
+      <c r="BJ287" s="316"/>
+      <c r="BK287" s="316"/>
+      <c r="BL287" s="316"/>
+      <c r="BM287" s="316"/>
+      <c r="BN287" s="316"/>
+      <c r="BO287" s="316"/>
+      <c r="BP287" s="316"/>
+      <c r="BQ287" s="316"/>
+      <c r="BR287" s="316"/>
+      <c r="BS287" s="316"/>
+      <c r="BT287" s="316"/>
+      <c r="BU287" s="316"/>
+      <c r="BV287" s="316"/>
+      <c r="BX287" s="316" t="s">
         <v>288</v>
       </c>
-      <c r="BY287" s="298"/>
-      <c r="BZ287" s="298"/>
-      <c r="CA287" s="298"/>
-      <c r="CB287" s="298"/>
-      <c r="CC287" s="298"/>
-      <c r="CD287" s="298"/>
-      <c r="CE287" s="298"/>
-      <c r="CF287" s="298"/>
-      <c r="CG287" s="298"/>
-      <c r="CH287" s="298"/>
-      <c r="CI287" s="298"/>
-      <c r="CJ287" s="298"/>
-      <c r="CK287" s="298"/>
+      <c r="BY287" s="316"/>
+      <c r="BZ287" s="316"/>
+      <c r="CA287" s="316"/>
+      <c r="CB287" s="316"/>
+      <c r="CC287" s="316"/>
+      <c r="CD287" s="316"/>
+      <c r="CE287" s="316"/>
+      <c r="CF287" s="316"/>
+      <c r="CG287" s="316"/>
+      <c r="CH287" s="316"/>
+      <c r="CI287" s="316"/>
+      <c r="CJ287" s="316"/>
+      <c r="CK287" s="316"/>
       <c r="CL287" s="295"/>
-      <c r="CM287" s="300" t="s">
+      <c r="CM287" s="322" t="s">
         <v>292</v>
       </c>
-      <c r="CN287" s="300"/>
-      <c r="CO287" s="300"/>
-      <c r="CP287" s="300"/>
-      <c r="CQ287" s="300"/>
-      <c r="CR287" s="300"/>
-      <c r="CS287" s="300"/>
-      <c r="CT287" s="300"/>
-      <c r="CU287" s="300"/>
-      <c r="CV287" s="300"/>
-      <c r="CW287" s="300"/>
-      <c r="CX287" s="300"/>
-      <c r="CY287" s="300"/>
-      <c r="CZ287" s="300"/>
+      <c r="CN287" s="322"/>
+      <c r="CO287" s="322"/>
+      <c r="CP287" s="322"/>
+      <c r="CQ287" s="322"/>
+      <c r="CR287" s="322"/>
+      <c r="CS287" s="322"/>
+      <c r="CT287" s="322"/>
+      <c r="CU287" s="322"/>
+      <c r="CV287" s="322"/>
+      <c r="CW287" s="322"/>
+      <c r="CX287" s="322"/>
+      <c r="CY287" s="322"/>
+      <c r="CZ287" s="322"/>
     </row>
     <row r="288" spans="1:104" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" s="77"/>
@@ -57427,37 +57427,37 @@
       <c r="BF302" s="66"/>
       <c r="BG302" s="66"/>
       <c r="BH302" s="66"/>
-      <c r="BI302" s="299" t="s">
+      <c r="BI302" s="327" t="s">
         <v>363</v>
       </c>
-      <c r="BJ302" s="299"/>
-      <c r="BK302" s="299"/>
-      <c r="BL302" s="299"/>
-      <c r="BM302" s="299"/>
-      <c r="BN302" s="299"/>
-      <c r="BO302" s="299"/>
-      <c r="BP302" s="299"/>
-      <c r="BQ302" s="299"/>
-      <c r="BR302" s="299"/>
-      <c r="BS302" s="299"/>
-      <c r="BT302" s="299"/>
-      <c r="BU302" s="299"/>
-      <c r="BV302" s="299"/>
-      <c r="BW302" s="299"/>
-      <c r="BX302" s="299"/>
-      <c r="BY302" s="299"/>
-      <c r="BZ302" s="299"/>
-      <c r="CA302" s="299"/>
-      <c r="CB302" s="299"/>
-      <c r="CC302" s="299"/>
-      <c r="CD302" s="299"/>
-      <c r="CE302" s="299"/>
-      <c r="CF302" s="299"/>
-      <c r="CG302" s="299"/>
-      <c r="CH302" s="299"/>
-      <c r="CI302" s="299"/>
-      <c r="CJ302" s="299"/>
-      <c r="CK302" s="299"/>
+      <c r="BJ302" s="327"/>
+      <c r="BK302" s="327"/>
+      <c r="BL302" s="327"/>
+      <c r="BM302" s="327"/>
+      <c r="BN302" s="327"/>
+      <c r="BO302" s="327"/>
+      <c r="BP302" s="327"/>
+      <c r="BQ302" s="327"/>
+      <c r="BR302" s="327"/>
+      <c r="BS302" s="327"/>
+      <c r="BT302" s="327"/>
+      <c r="BU302" s="327"/>
+      <c r="BV302" s="327"/>
+      <c r="BW302" s="327"/>
+      <c r="BX302" s="327"/>
+      <c r="BY302" s="327"/>
+      <c r="BZ302" s="327"/>
+      <c r="CA302" s="327"/>
+      <c r="CB302" s="327"/>
+      <c r="CC302" s="327"/>
+      <c r="CD302" s="327"/>
+      <c r="CE302" s="327"/>
+      <c r="CF302" s="327"/>
+      <c r="CG302" s="327"/>
+      <c r="CH302" s="327"/>
+      <c r="CI302" s="327"/>
+      <c r="CJ302" s="327"/>
+      <c r="CK302" s="327"/>
       <c r="CL302" s="295"/>
     </row>
     <row r="303" spans="1:104" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -57491,38 +57491,38 @@
       <c r="BF303" s="275"/>
       <c r="BG303" s="275"/>
       <c r="BH303" s="108"/>
-      <c r="BI303" s="300" t="s">
+      <c r="BI303" s="322" t="s">
         <v>360</v>
       </c>
-      <c r="BJ303" s="300"/>
-      <c r="BK303" s="300"/>
-      <c r="BL303" s="300"/>
-      <c r="BM303" s="300"/>
-      <c r="BN303" s="300"/>
-      <c r="BO303" s="300"/>
-      <c r="BP303" s="300"/>
-      <c r="BQ303" s="300"/>
-      <c r="BR303" s="300"/>
-      <c r="BS303" s="300"/>
-      <c r="BT303" s="300"/>
-      <c r="BU303" s="300"/>
-      <c r="BV303" s="300"/>
-      <c r="BX303" s="300" t="s">
+      <c r="BJ303" s="322"/>
+      <c r="BK303" s="322"/>
+      <c r="BL303" s="322"/>
+      <c r="BM303" s="322"/>
+      <c r="BN303" s="322"/>
+      <c r="BO303" s="322"/>
+      <c r="BP303" s="322"/>
+      <c r="BQ303" s="322"/>
+      <c r="BR303" s="322"/>
+      <c r="BS303" s="322"/>
+      <c r="BT303" s="322"/>
+      <c r="BU303" s="322"/>
+      <c r="BV303" s="322"/>
+      <c r="BX303" s="322" t="s">
         <v>288</v>
       </c>
-      <c r="BY303" s="300"/>
-      <c r="BZ303" s="300"/>
-      <c r="CA303" s="300"/>
-      <c r="CB303" s="300"/>
-      <c r="CC303" s="300"/>
-      <c r="CD303" s="300"/>
-      <c r="CE303" s="300"/>
-      <c r="CF303" s="300"/>
-      <c r="CG303" s="300"/>
-      <c r="CH303" s="300"/>
-      <c r="CI303" s="300"/>
-      <c r="CJ303" s="300"/>
-      <c r="CK303" s="300"/>
+      <c r="BY303" s="322"/>
+      <c r="BZ303" s="322"/>
+      <c r="CA303" s="322"/>
+      <c r="CB303" s="322"/>
+      <c r="CC303" s="322"/>
+      <c r="CD303" s="322"/>
+      <c r="CE303" s="322"/>
+      <c r="CF303" s="322"/>
+      <c r="CG303" s="322"/>
+      <c r="CH303" s="322"/>
+      <c r="CI303" s="322"/>
+      <c r="CJ303" s="322"/>
+      <c r="CK303" s="322"/>
     </row>
     <row r="304" spans="1:104" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AE304" s="77"/>
@@ -60185,6 +60185,113 @@
     <row r="744" ht="14.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="131">
+    <mergeCell ref="CM271:CZ271"/>
+    <mergeCell ref="BI270:CK270"/>
+    <mergeCell ref="BI302:CK302"/>
+    <mergeCell ref="BI271:BV271"/>
+    <mergeCell ref="BX271:CK271"/>
+    <mergeCell ref="BI286:CK286"/>
+    <mergeCell ref="CM287:CZ287"/>
+    <mergeCell ref="BX303:CK303"/>
+    <mergeCell ref="BI303:BV303"/>
+    <mergeCell ref="AT239:BG239"/>
+    <mergeCell ref="BI239:BV239"/>
+    <mergeCell ref="A254:N254"/>
+    <mergeCell ref="P254:AC254"/>
+    <mergeCell ref="AE254:AR254"/>
+    <mergeCell ref="AT254:BG254"/>
+    <mergeCell ref="P224:AC224"/>
+    <mergeCell ref="P239:AC239"/>
+    <mergeCell ref="A239:N239"/>
+    <mergeCell ref="BI254:BV254"/>
+    <mergeCell ref="BI287:BV287"/>
+    <mergeCell ref="BX287:CK287"/>
+    <mergeCell ref="A17:AD17"/>
+    <mergeCell ref="AT18:BG18"/>
+    <mergeCell ref="A208:AD208"/>
+    <mergeCell ref="A209:N209"/>
+    <mergeCell ref="P209:AC209"/>
+    <mergeCell ref="AE161:AR161"/>
+    <mergeCell ref="AT161:BG161"/>
+    <mergeCell ref="BI161:BV161"/>
+    <mergeCell ref="AE209:AR209"/>
+    <mergeCell ref="AT209:BG209"/>
+    <mergeCell ref="BC160:BE160"/>
+    <mergeCell ref="BF160:BH160"/>
+    <mergeCell ref="AZ160:BB160"/>
+    <mergeCell ref="Y160:AA160"/>
+    <mergeCell ref="AB160:AD160"/>
+    <mergeCell ref="AE160:AG160"/>
+    <mergeCell ref="P160:R160"/>
+    <mergeCell ref="S160:U160"/>
+    <mergeCell ref="V160:X160"/>
+    <mergeCell ref="A160:C160"/>
+    <mergeCell ref="D160:F160"/>
+    <mergeCell ref="G160:I160"/>
+    <mergeCell ref="J160:L160"/>
+    <mergeCell ref="M160:O160"/>
+    <mergeCell ref="BI70:BV70"/>
+    <mergeCell ref="BX254:CK254"/>
+    <mergeCell ref="CM254:CZ254"/>
+    <mergeCell ref="A18:N18"/>
+    <mergeCell ref="AT34:BG34"/>
+    <mergeCell ref="P18:AC18"/>
+    <mergeCell ref="AE18:AR18"/>
+    <mergeCell ref="A69:AD69"/>
+    <mergeCell ref="BI53:BV53"/>
+    <mergeCell ref="BI68:BK68"/>
+    <mergeCell ref="BL68:BN68"/>
+    <mergeCell ref="BO68:BQ68"/>
+    <mergeCell ref="BR68:BT68"/>
+    <mergeCell ref="BU68:BW68"/>
+    <mergeCell ref="AN160:AP160"/>
+    <mergeCell ref="AQ160:AS160"/>
+    <mergeCell ref="AT160:AV160"/>
+    <mergeCell ref="AW160:AY160"/>
+    <mergeCell ref="P161:AC161"/>
+    <mergeCell ref="A224:N224"/>
+    <mergeCell ref="AE224:AR224"/>
+    <mergeCell ref="AT224:BG224"/>
+    <mergeCell ref="BI224:BV224"/>
+    <mergeCell ref="AE239:AR239"/>
+    <mergeCell ref="A70:N70"/>
+    <mergeCell ref="P70:AC70"/>
+    <mergeCell ref="AE34:AR34"/>
+    <mergeCell ref="P34:AC34"/>
+    <mergeCell ref="AE85:AR85"/>
+    <mergeCell ref="A85:N85"/>
+    <mergeCell ref="P85:AC85"/>
+    <mergeCell ref="AT85:BG85"/>
+    <mergeCell ref="A52:N52"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="D67:F67"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="J67:L67"/>
+    <mergeCell ref="M67:O67"/>
+    <mergeCell ref="AE70:AR70"/>
+    <mergeCell ref="AT70:BG70"/>
+    <mergeCell ref="P51:AX51"/>
+    <mergeCell ref="AD207:AF207"/>
+    <mergeCell ref="AG207:AI207"/>
+    <mergeCell ref="AJ207:AL207"/>
+    <mergeCell ref="AM207:AO207"/>
+    <mergeCell ref="AP207:AR207"/>
+    <mergeCell ref="A161:N161"/>
+    <mergeCell ref="A193:N193"/>
+    <mergeCell ref="A100:N100"/>
+    <mergeCell ref="P100:AC100"/>
+    <mergeCell ref="AE100:AR100"/>
+    <mergeCell ref="AH160:AJ160"/>
+    <mergeCell ref="AK160:AM160"/>
+    <mergeCell ref="A145:N145"/>
+    <mergeCell ref="P145:AC145"/>
+    <mergeCell ref="AE145:AR145"/>
+    <mergeCell ref="A130:N130"/>
+    <mergeCell ref="P130:AC130"/>
+    <mergeCell ref="AE130:AR130"/>
+    <mergeCell ref="A115:N115"/>
+    <mergeCell ref="P115:AC115"/>
+    <mergeCell ref="AE115:AR115"/>
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A177:N177"/>
     <mergeCell ref="A192:C192"/>
@@ -60209,113 +60316,6 @@
     <mergeCell ref="P52:AC52"/>
     <mergeCell ref="AE52:AR52"/>
     <mergeCell ref="AT52:BG52"/>
-    <mergeCell ref="AD207:AF207"/>
-    <mergeCell ref="AG207:AI207"/>
-    <mergeCell ref="AJ207:AL207"/>
-    <mergeCell ref="AM207:AO207"/>
-    <mergeCell ref="AP207:AR207"/>
-    <mergeCell ref="A161:N161"/>
-    <mergeCell ref="A193:N193"/>
-    <mergeCell ref="A100:N100"/>
-    <mergeCell ref="P100:AC100"/>
-    <mergeCell ref="AE100:AR100"/>
-    <mergeCell ref="AH160:AJ160"/>
-    <mergeCell ref="AK160:AM160"/>
-    <mergeCell ref="A145:N145"/>
-    <mergeCell ref="P145:AC145"/>
-    <mergeCell ref="AE145:AR145"/>
-    <mergeCell ref="A130:N130"/>
-    <mergeCell ref="P130:AC130"/>
-    <mergeCell ref="AE130:AR130"/>
-    <mergeCell ref="A115:N115"/>
-    <mergeCell ref="P115:AC115"/>
-    <mergeCell ref="AE115:AR115"/>
-    <mergeCell ref="A70:N70"/>
-    <mergeCell ref="P70:AC70"/>
-    <mergeCell ref="AE34:AR34"/>
-    <mergeCell ref="P34:AC34"/>
-    <mergeCell ref="AE85:AR85"/>
-    <mergeCell ref="A85:N85"/>
-    <mergeCell ref="P85:AC85"/>
-    <mergeCell ref="AT85:BG85"/>
-    <mergeCell ref="A52:N52"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="D67:F67"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="J67:L67"/>
-    <mergeCell ref="M67:O67"/>
-    <mergeCell ref="AE70:AR70"/>
-    <mergeCell ref="AT70:BG70"/>
-    <mergeCell ref="P51:AX51"/>
-    <mergeCell ref="BI70:BV70"/>
-    <mergeCell ref="BX254:CK254"/>
-    <mergeCell ref="CM254:CZ254"/>
-    <mergeCell ref="A18:N18"/>
-    <mergeCell ref="AT34:BG34"/>
-    <mergeCell ref="P18:AC18"/>
-    <mergeCell ref="AE18:AR18"/>
-    <mergeCell ref="A69:AD69"/>
-    <mergeCell ref="BI53:BV53"/>
-    <mergeCell ref="BI68:BK68"/>
-    <mergeCell ref="BL68:BN68"/>
-    <mergeCell ref="BO68:BQ68"/>
-    <mergeCell ref="BR68:BT68"/>
-    <mergeCell ref="BU68:BW68"/>
-    <mergeCell ref="AN160:AP160"/>
-    <mergeCell ref="AQ160:AS160"/>
-    <mergeCell ref="AT160:AV160"/>
-    <mergeCell ref="AW160:AY160"/>
-    <mergeCell ref="P161:AC161"/>
-    <mergeCell ref="A224:N224"/>
-    <mergeCell ref="AE224:AR224"/>
-    <mergeCell ref="AT224:BG224"/>
-    <mergeCell ref="BI224:BV224"/>
-    <mergeCell ref="AE239:AR239"/>
-    <mergeCell ref="A17:AD17"/>
-    <mergeCell ref="AT18:BG18"/>
-    <mergeCell ref="A208:AD208"/>
-    <mergeCell ref="A209:N209"/>
-    <mergeCell ref="P209:AC209"/>
-    <mergeCell ref="AE161:AR161"/>
-    <mergeCell ref="AT161:BG161"/>
-    <mergeCell ref="BI161:BV161"/>
-    <mergeCell ref="AE209:AR209"/>
-    <mergeCell ref="AT209:BG209"/>
-    <mergeCell ref="BC160:BE160"/>
-    <mergeCell ref="BF160:BH160"/>
-    <mergeCell ref="AZ160:BB160"/>
-    <mergeCell ref="Y160:AA160"/>
-    <mergeCell ref="AB160:AD160"/>
-    <mergeCell ref="AE160:AG160"/>
-    <mergeCell ref="P160:R160"/>
-    <mergeCell ref="S160:U160"/>
-    <mergeCell ref="V160:X160"/>
-    <mergeCell ref="A160:C160"/>
-    <mergeCell ref="D160:F160"/>
-    <mergeCell ref="G160:I160"/>
-    <mergeCell ref="J160:L160"/>
-    <mergeCell ref="M160:O160"/>
-    <mergeCell ref="BX303:CK303"/>
-    <mergeCell ref="BI303:BV303"/>
-    <mergeCell ref="AT239:BG239"/>
-    <mergeCell ref="BI239:BV239"/>
-    <mergeCell ref="A254:N254"/>
-    <mergeCell ref="P254:AC254"/>
-    <mergeCell ref="AE254:AR254"/>
-    <mergeCell ref="AT254:BG254"/>
-    <mergeCell ref="P224:AC224"/>
-    <mergeCell ref="P239:AC239"/>
-    <mergeCell ref="A239:N239"/>
-    <mergeCell ref="BI254:BV254"/>
-    <mergeCell ref="BI287:BV287"/>
-    <mergeCell ref="BX287:CK287"/>
-    <mergeCell ref="CM271:CZ271"/>
-    <mergeCell ref="BI270:CK270"/>
-    <mergeCell ref="BI302:CK302"/>
-    <mergeCell ref="BI271:BV271"/>
-    <mergeCell ref="BX271:CK271"/>
-    <mergeCell ref="BI286:CK286"/>
-    <mergeCell ref="CM287:CZ287"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
-top of sb open 11-15 goes to raise from push -bug fixes
</commit_message>
<xml_diff>
--- a/pAd/bin/Debug/Data/SPINRANGES.xlsx
+++ b/pAd/bin/Debug/Data/SPINRANGES.xlsx
@@ -2726,6 +2726,15 @@
     <xf numFmtId="49" fontId="1" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2812,15 +2821,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3196,8 +3196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EE776"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B203" sqref="B203"/>
+    <sheetView tabSelected="1" topLeftCell="R77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AK93" sqref="AK93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3207,70 +3207,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="21.1" x14ac:dyDescent="0.35">
-      <c r="A1" s="327"/>
-      <c r="B1" s="327"/>
-      <c r="C1" s="327"/>
-      <c r="D1" s="327"/>
-      <c r="E1" s="327"/>
-      <c r="F1" s="327"/>
-      <c r="G1" s="327"/>
-      <c r="H1" s="327"/>
-      <c r="I1" s="327"/>
-      <c r="J1" s="327"/>
-      <c r="K1" s="327"/>
-      <c r="L1" s="327"/>
-      <c r="M1" s="327"/>
-      <c r="N1" s="327"/>
-      <c r="O1" s="327"/>
-      <c r="P1" s="327"/>
-      <c r="Q1" s="327"/>
-      <c r="R1" s="327"/>
-      <c r="S1" s="327"/>
-      <c r="T1" s="327"/>
-      <c r="U1" s="327"/>
-      <c r="V1" s="327"/>
-      <c r="W1" s="327"/>
-      <c r="X1" s="327"/>
-      <c r="Y1" s="327"/>
-      <c r="Z1" s="327"/>
-      <c r="AA1" s="327"/>
-      <c r="AB1" s="327"/>
-      <c r="AC1" s="327"/>
-      <c r="AD1" s="327"/>
+      <c r="A1" s="330"/>
+      <c r="B1" s="330"/>
+      <c r="C1" s="330"/>
+      <c r="D1" s="330"/>
+      <c r="E1" s="330"/>
+      <c r="F1" s="330"/>
+      <c r="G1" s="330"/>
+      <c r="H1" s="330"/>
+      <c r="I1" s="330"/>
+      <c r="J1" s="330"/>
+      <c r="K1" s="330"/>
+      <c r="L1" s="330"/>
+      <c r="M1" s="330"/>
+      <c r="N1" s="330"/>
+      <c r="O1" s="330"/>
+      <c r="P1" s="330"/>
+      <c r="Q1" s="330"/>
+      <c r="R1" s="330"/>
+      <c r="S1" s="330"/>
+      <c r="T1" s="330"/>
+      <c r="U1" s="330"/>
+      <c r="V1" s="330"/>
+      <c r="W1" s="330"/>
+      <c r="X1" s="330"/>
+      <c r="Y1" s="330"/>
+      <c r="Z1" s="330"/>
+      <c r="AA1" s="330"/>
+      <c r="AB1" s="330"/>
+      <c r="AC1" s="330"/>
+      <c r="AD1" s="330"/>
     </row>
     <row r="17" spans="1:94" ht="20.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="327" t="s">
+      <c r="A17" s="330" t="s">
         <v>137</v>
       </c>
-      <c r="B17" s="327"/>
-      <c r="C17" s="327"/>
-      <c r="D17" s="327"/>
-      <c r="E17" s="327"/>
-      <c r="F17" s="327"/>
-      <c r="G17" s="327"/>
-      <c r="H17" s="327"/>
-      <c r="I17" s="327"/>
-      <c r="J17" s="327"/>
-      <c r="K17" s="327"/>
-      <c r="L17" s="327"/>
-      <c r="M17" s="327"/>
-      <c r="N17" s="327"/>
-      <c r="O17" s="327"/>
-      <c r="P17" s="327"/>
-      <c r="Q17" s="327"/>
-      <c r="R17" s="327"/>
-      <c r="S17" s="327"/>
-      <c r="T17" s="327"/>
-      <c r="U17" s="327"/>
-      <c r="V17" s="327"/>
-      <c r="W17" s="327"/>
-      <c r="X17" s="327"/>
-      <c r="Y17" s="327"/>
-      <c r="Z17" s="327"/>
-      <c r="AA17" s="327"/>
-      <c r="AB17" s="327"/>
-      <c r="AC17" s="327"/>
-      <c r="AD17" s="327"/>
+      <c r="B17" s="330"/>
+      <c r="C17" s="330"/>
+      <c r="D17" s="330"/>
+      <c r="E17" s="330"/>
+      <c r="F17" s="330"/>
+      <c r="G17" s="330"/>
+      <c r="H17" s="330"/>
+      <c r="I17" s="330"/>
+      <c r="J17" s="330"/>
+      <c r="K17" s="330"/>
+      <c r="L17" s="330"/>
+      <c r="M17" s="330"/>
+      <c r="N17" s="330"/>
+      <c r="O17" s="330"/>
+      <c r="P17" s="330"/>
+      <c r="Q17" s="330"/>
+      <c r="R17" s="330"/>
+      <c r="S17" s="330"/>
+      <c r="T17" s="330"/>
+      <c r="U17" s="330"/>
+      <c r="V17" s="330"/>
+      <c r="W17" s="330"/>
+      <c r="X17" s="330"/>
+      <c r="Y17" s="330"/>
+      <c r="Z17" s="330"/>
+      <c r="AA17" s="330"/>
+      <c r="AB17" s="330"/>
+      <c r="AC17" s="330"/>
+      <c r="AD17" s="330"/>
       <c r="AE17" s="66"/>
       <c r="AF17" s="66"/>
       <c r="AG17" s="66"/>
@@ -3337,70 +3337,70 @@
       <c r="CP17" s="66"/>
     </row>
     <row r="18" spans="1:94" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="338" t="s">
+      <c r="A18" s="341" t="s">
         <v>245</v>
       </c>
-      <c r="B18" s="338"/>
-      <c r="C18" s="338"/>
-      <c r="D18" s="338"/>
-      <c r="E18" s="338"/>
-      <c r="F18" s="338"/>
-      <c r="G18" s="338"/>
-      <c r="H18" s="338"/>
-      <c r="I18" s="338"/>
-      <c r="J18" s="338"/>
-      <c r="K18" s="338"/>
-      <c r="L18" s="338"/>
-      <c r="M18" s="338"/>
-      <c r="N18" s="338"/>
-      <c r="P18" s="338" t="s">
+      <c r="B18" s="341"/>
+      <c r="C18" s="341"/>
+      <c r="D18" s="341"/>
+      <c r="E18" s="341"/>
+      <c r="F18" s="341"/>
+      <c r="G18" s="341"/>
+      <c r="H18" s="341"/>
+      <c r="I18" s="341"/>
+      <c r="J18" s="341"/>
+      <c r="K18" s="341"/>
+      <c r="L18" s="341"/>
+      <c r="M18" s="341"/>
+      <c r="N18" s="341"/>
+      <c r="P18" s="341" t="s">
         <v>246</v>
       </c>
-      <c r="Q18" s="338"/>
-      <c r="R18" s="338"/>
-      <c r="S18" s="338"/>
-      <c r="T18" s="338"/>
-      <c r="U18" s="338"/>
-      <c r="V18" s="338"/>
-      <c r="W18" s="338"/>
-      <c r="X18" s="338"/>
-      <c r="Y18" s="338"/>
-      <c r="Z18" s="338"/>
-      <c r="AA18" s="338"/>
-      <c r="AB18" s="338"/>
-      <c r="AC18" s="338"/>
-      <c r="AE18" s="339" t="s">
+      <c r="Q18" s="341"/>
+      <c r="R18" s="341"/>
+      <c r="S18" s="341"/>
+      <c r="T18" s="341"/>
+      <c r="U18" s="341"/>
+      <c r="V18" s="341"/>
+      <c r="W18" s="341"/>
+      <c r="X18" s="341"/>
+      <c r="Y18" s="341"/>
+      <c r="Z18" s="341"/>
+      <c r="AA18" s="341"/>
+      <c r="AB18" s="341"/>
+      <c r="AC18" s="341"/>
+      <c r="AE18" s="342" t="s">
         <v>247</v>
       </c>
-      <c r="AF18" s="339"/>
-      <c r="AG18" s="339"/>
-      <c r="AH18" s="339"/>
-      <c r="AI18" s="339"/>
-      <c r="AJ18" s="339"/>
-      <c r="AK18" s="339"/>
-      <c r="AL18" s="339"/>
-      <c r="AM18" s="339"/>
-      <c r="AN18" s="339"/>
-      <c r="AO18" s="339"/>
-      <c r="AP18" s="339"/>
-      <c r="AQ18" s="339"/>
-      <c r="AR18" s="339"/>
-      <c r="AT18" s="328" t="s">
+      <c r="AF18" s="342"/>
+      <c r="AG18" s="342"/>
+      <c r="AH18" s="342"/>
+      <c r="AI18" s="342"/>
+      <c r="AJ18" s="342"/>
+      <c r="AK18" s="342"/>
+      <c r="AL18" s="342"/>
+      <c r="AM18" s="342"/>
+      <c r="AN18" s="342"/>
+      <c r="AO18" s="342"/>
+      <c r="AP18" s="342"/>
+      <c r="AQ18" s="342"/>
+      <c r="AR18" s="342"/>
+      <c r="AT18" s="331" t="s">
         <v>248</v>
       </c>
-      <c r="AU18" s="328"/>
-      <c r="AV18" s="328"/>
-      <c r="AW18" s="328"/>
-      <c r="AX18" s="328"/>
-      <c r="AY18" s="328"/>
-      <c r="AZ18" s="328"/>
-      <c r="BA18" s="328"/>
-      <c r="BB18" s="328"/>
-      <c r="BC18" s="328"/>
-      <c r="BD18" s="328"/>
-      <c r="BE18" s="328"/>
-      <c r="BF18" s="328"/>
-      <c r="BG18" s="328"/>
+      <c r="AU18" s="331"/>
+      <c r="AV18" s="331"/>
+      <c r="AW18" s="331"/>
+      <c r="AX18" s="331"/>
+      <c r="AY18" s="331"/>
+      <c r="AZ18" s="331"/>
+      <c r="BA18" s="331"/>
+      <c r="BB18" s="331"/>
+      <c r="BC18" s="331"/>
+      <c r="BD18" s="331"/>
+      <c r="BE18" s="331"/>
+      <c r="BF18" s="331"/>
+      <c r="BG18" s="331"/>
     </row>
     <row r="19" spans="1:94" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
@@ -5776,54 +5776,54 @@
     </row>
     <row r="33" spans="16:59" ht="14.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="16:59" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P34" s="338" t="s">
+      <c r="P34" s="341" t="s">
         <v>250</v>
       </c>
-      <c r="Q34" s="338"/>
-      <c r="R34" s="338"/>
-      <c r="S34" s="338"/>
-      <c r="T34" s="338"/>
-      <c r="U34" s="338"/>
-      <c r="V34" s="338"/>
-      <c r="W34" s="338"/>
-      <c r="X34" s="338"/>
-      <c r="Y34" s="338"/>
-      <c r="Z34" s="338"/>
-      <c r="AA34" s="338"/>
-      <c r="AB34" s="338"/>
-      <c r="AC34" s="338"/>
-      <c r="AE34" s="339" t="s">
+      <c r="Q34" s="341"/>
+      <c r="R34" s="341"/>
+      <c r="S34" s="341"/>
+      <c r="T34" s="341"/>
+      <c r="U34" s="341"/>
+      <c r="V34" s="341"/>
+      <c r="W34" s="341"/>
+      <c r="X34" s="341"/>
+      <c r="Y34" s="341"/>
+      <c r="Z34" s="341"/>
+      <c r="AA34" s="341"/>
+      <c r="AB34" s="341"/>
+      <c r="AC34" s="341"/>
+      <c r="AE34" s="342" t="s">
         <v>249</v>
       </c>
-      <c r="AF34" s="339"/>
-      <c r="AG34" s="339"/>
-      <c r="AH34" s="339"/>
-      <c r="AI34" s="339"/>
-      <c r="AJ34" s="339"/>
-      <c r="AK34" s="339"/>
-      <c r="AL34" s="339"/>
-      <c r="AM34" s="339"/>
-      <c r="AN34" s="339"/>
-      <c r="AO34" s="339"/>
-      <c r="AP34" s="339"/>
-      <c r="AQ34" s="339"/>
-      <c r="AR34" s="339"/>
-      <c r="AT34" s="346" t="s">
+      <c r="AF34" s="342"/>
+      <c r="AG34" s="342"/>
+      <c r="AH34" s="342"/>
+      <c r="AI34" s="342"/>
+      <c r="AJ34" s="342"/>
+      <c r="AK34" s="342"/>
+      <c r="AL34" s="342"/>
+      <c r="AM34" s="342"/>
+      <c r="AN34" s="342"/>
+      <c r="AO34" s="342"/>
+      <c r="AP34" s="342"/>
+      <c r="AQ34" s="342"/>
+      <c r="AR34" s="342"/>
+      <c r="AT34" s="349" t="s">
         <v>138</v>
       </c>
-      <c r="AU34" s="346"/>
-      <c r="AV34" s="346"/>
-      <c r="AW34" s="346"/>
-      <c r="AX34" s="346"/>
-      <c r="AY34" s="346"/>
-      <c r="AZ34" s="346"/>
-      <c r="BA34" s="346"/>
-      <c r="BB34" s="346"/>
-      <c r="BC34" s="346"/>
-      <c r="BD34" s="346"/>
-      <c r="BE34" s="346"/>
-      <c r="BF34" s="346"/>
-      <c r="BG34" s="346"/>
+      <c r="AU34" s="349"/>
+      <c r="AV34" s="349"/>
+      <c r="AW34" s="349"/>
+      <c r="AX34" s="349"/>
+      <c r="AY34" s="349"/>
+      <c r="AZ34" s="349"/>
+      <c r="BA34" s="349"/>
+      <c r="BB34" s="349"/>
+      <c r="BC34" s="349"/>
+      <c r="BD34" s="349"/>
+      <c r="BE34" s="349"/>
+      <c r="BF34" s="349"/>
+      <c r="BG34" s="349"/>
     </row>
     <row r="35" spans="16:59" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P35" s="1"/>
@@ -7612,102 +7612,102 @@
       </c>
     </row>
     <row r="49" spans="16:59" ht="14.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P49" s="322" t="s">
+      <c r="P49" s="325" t="s">
         <v>363</v>
       </c>
-      <c r="Q49" s="322"/>
-      <c r="R49" s="322"/>
-      <c r="S49" s="322"/>
-      <c r="T49" s="322"/>
-      <c r="U49" s="322"/>
-      <c r="V49" s="322"/>
-      <c r="W49" s="322"/>
-      <c r="X49" s="322"/>
-      <c r="Y49" s="322"/>
-      <c r="Z49" s="322"/>
-      <c r="AA49" s="322"/>
-      <c r="AB49" s="322"/>
-      <c r="AC49" s="322"/>
-      <c r="AD49" s="322"/>
-      <c r="AE49" s="322"/>
-      <c r="AF49" s="322"/>
-      <c r="AG49" s="322"/>
-      <c r="AH49" s="322"/>
-      <c r="AI49" s="322"/>
-      <c r="AJ49" s="322"/>
-      <c r="AK49" s="322"/>
-      <c r="AL49" s="322"/>
-      <c r="AM49" s="322"/>
-      <c r="AN49" s="322"/>
-      <c r="AO49" s="322"/>
-      <c r="AP49" s="322"/>
-      <c r="AQ49" s="322"/>
-      <c r="AR49" s="322"/>
-      <c r="AS49" s="322"/>
-      <c r="AT49" s="322"/>
-      <c r="AU49" s="322"/>
-      <c r="AV49" s="322"/>
-      <c r="AW49" s="322"/>
-      <c r="AX49" s="322"/>
-      <c r="AY49" s="322"/>
-      <c r="AZ49" s="322"/>
-      <c r="BA49" s="322"/>
-      <c r="BB49" s="322"/>
-      <c r="BC49" s="322"/>
-      <c r="BD49" s="322"/>
-      <c r="BE49" s="322"/>
-      <c r="BF49" s="322"/>
-      <c r="BG49" s="322"/>
+      <c r="Q49" s="325"/>
+      <c r="R49" s="325"/>
+      <c r="S49" s="325"/>
+      <c r="T49" s="325"/>
+      <c r="U49" s="325"/>
+      <c r="V49" s="325"/>
+      <c r="W49" s="325"/>
+      <c r="X49" s="325"/>
+      <c r="Y49" s="325"/>
+      <c r="Z49" s="325"/>
+      <c r="AA49" s="325"/>
+      <c r="AB49" s="325"/>
+      <c r="AC49" s="325"/>
+      <c r="AD49" s="325"/>
+      <c r="AE49" s="325"/>
+      <c r="AF49" s="325"/>
+      <c r="AG49" s="325"/>
+      <c r="AH49" s="325"/>
+      <c r="AI49" s="325"/>
+      <c r="AJ49" s="325"/>
+      <c r="AK49" s="325"/>
+      <c r="AL49" s="325"/>
+      <c r="AM49" s="325"/>
+      <c r="AN49" s="325"/>
+      <c r="AO49" s="325"/>
+      <c r="AP49" s="325"/>
+      <c r="AQ49" s="325"/>
+      <c r="AR49" s="325"/>
+      <c r="AS49" s="325"/>
+      <c r="AT49" s="325"/>
+      <c r="AU49" s="325"/>
+      <c r="AV49" s="325"/>
+      <c r="AW49" s="325"/>
+      <c r="AX49" s="325"/>
+      <c r="AY49" s="325"/>
+      <c r="AZ49" s="325"/>
+      <c r="BA49" s="325"/>
+      <c r="BB49" s="325"/>
+      <c r="BC49" s="325"/>
+      <c r="BD49" s="325"/>
+      <c r="BE49" s="325"/>
+      <c r="BF49" s="325"/>
+      <c r="BG49" s="325"/>
     </row>
     <row r="50" spans="16:59" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P50" s="346" t="s">
+      <c r="P50" s="349" t="s">
         <v>366</v>
       </c>
-      <c r="Q50" s="346"/>
-      <c r="R50" s="346"/>
-      <c r="S50" s="346"/>
-      <c r="T50" s="346"/>
-      <c r="U50" s="346"/>
-      <c r="V50" s="346"/>
-      <c r="W50" s="346"/>
-      <c r="X50" s="346"/>
-      <c r="Y50" s="346"/>
-      <c r="Z50" s="346"/>
-      <c r="AA50" s="346"/>
-      <c r="AB50" s="346"/>
-      <c r="AC50" s="346"/>
-      <c r="AE50" s="346" t="s">
+      <c r="Q50" s="349"/>
+      <c r="R50" s="349"/>
+      <c r="S50" s="349"/>
+      <c r="T50" s="349"/>
+      <c r="U50" s="349"/>
+      <c r="V50" s="349"/>
+      <c r="W50" s="349"/>
+      <c r="X50" s="349"/>
+      <c r="Y50" s="349"/>
+      <c r="Z50" s="349"/>
+      <c r="AA50" s="349"/>
+      <c r="AB50" s="349"/>
+      <c r="AC50" s="349"/>
+      <c r="AE50" s="349" t="s">
         <v>365</v>
       </c>
-      <c r="AF50" s="346"/>
-      <c r="AG50" s="346"/>
-      <c r="AH50" s="346"/>
-      <c r="AI50" s="346"/>
-      <c r="AJ50" s="346"/>
-      <c r="AK50" s="346"/>
-      <c r="AL50" s="346"/>
-      <c r="AM50" s="346"/>
-      <c r="AN50" s="346"/>
-      <c r="AO50" s="346"/>
-      <c r="AP50" s="346"/>
-      <c r="AQ50" s="346"/>
-      <c r="AR50" s="346"/>
-      <c r="AT50" s="346" t="s">
+      <c r="AF50" s="349"/>
+      <c r="AG50" s="349"/>
+      <c r="AH50" s="349"/>
+      <c r="AI50" s="349"/>
+      <c r="AJ50" s="349"/>
+      <c r="AK50" s="349"/>
+      <c r="AL50" s="349"/>
+      <c r="AM50" s="349"/>
+      <c r="AN50" s="349"/>
+      <c r="AO50" s="349"/>
+      <c r="AP50" s="349"/>
+      <c r="AQ50" s="349"/>
+      <c r="AR50" s="349"/>
+      <c r="AT50" s="349" t="s">
         <v>364</v>
       </c>
-      <c r="AU50" s="346"/>
-      <c r="AV50" s="346"/>
-      <c r="AW50" s="346"/>
-      <c r="AX50" s="346"/>
-      <c r="AY50" s="346"/>
-      <c r="AZ50" s="346"/>
-      <c r="BA50" s="346"/>
-      <c r="BB50" s="346"/>
-      <c r="BC50" s="346"/>
-      <c r="BD50" s="346"/>
-      <c r="BE50" s="346"/>
-      <c r="BF50" s="346"/>
-      <c r="BG50" s="346"/>
+      <c r="AU50" s="349"/>
+      <c r="AV50" s="349"/>
+      <c r="AW50" s="349"/>
+      <c r="AX50" s="349"/>
+      <c r="AY50" s="349"/>
+      <c r="AZ50" s="349"/>
+      <c r="BA50" s="349"/>
+      <c r="BB50" s="349"/>
+      <c r="BC50" s="349"/>
+      <c r="BD50" s="349"/>
+      <c r="BE50" s="349"/>
+      <c r="BF50" s="349"/>
+      <c r="BG50" s="349"/>
     </row>
     <row r="51" spans="16:59" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P51" s="1"/>
@@ -9576,111 +9576,111 @@
       <c r="BW68" s="66"/>
     </row>
     <row r="69" spans="1:75" ht="14.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P69" s="345" t="s">
+      <c r="P69" s="348" t="s">
         <v>282</v>
       </c>
-      <c r="Q69" s="345"/>
-      <c r="R69" s="345"/>
-      <c r="S69" s="345"/>
-      <c r="T69" s="345"/>
-      <c r="U69" s="345"/>
-      <c r="V69" s="345"/>
-      <c r="W69" s="345"/>
-      <c r="X69" s="345"/>
-      <c r="Y69" s="345"/>
-      <c r="Z69" s="345"/>
-      <c r="AA69" s="345"/>
-      <c r="AB69" s="345"/>
-      <c r="AC69" s="345"/>
-      <c r="AD69" s="345"/>
-      <c r="AE69" s="345"/>
-      <c r="AF69" s="345"/>
-      <c r="AG69" s="345"/>
-      <c r="AH69" s="345"/>
-      <c r="AI69" s="345"/>
-      <c r="AJ69" s="345"/>
-      <c r="AK69" s="345"/>
-      <c r="AL69" s="345"/>
-      <c r="AM69" s="345"/>
-      <c r="AN69" s="345"/>
-      <c r="AO69" s="345"/>
-      <c r="AP69" s="345"/>
-      <c r="AQ69" s="345"/>
-      <c r="AR69" s="345"/>
-      <c r="AS69" s="345"/>
-      <c r="AT69" s="345"/>
-      <c r="AU69" s="345"/>
-      <c r="AV69" s="345"/>
-      <c r="AW69" s="345"/>
-      <c r="AX69" s="345"/>
+      <c r="Q69" s="348"/>
+      <c r="R69" s="348"/>
+      <c r="S69" s="348"/>
+      <c r="T69" s="348"/>
+      <c r="U69" s="348"/>
+      <c r="V69" s="348"/>
+      <c r="W69" s="348"/>
+      <c r="X69" s="348"/>
+      <c r="Y69" s="348"/>
+      <c r="Z69" s="348"/>
+      <c r="AA69" s="348"/>
+      <c r="AB69" s="348"/>
+      <c r="AC69" s="348"/>
+      <c r="AD69" s="348"/>
+      <c r="AE69" s="348"/>
+      <c r="AF69" s="348"/>
+      <c r="AG69" s="348"/>
+      <c r="AH69" s="348"/>
+      <c r="AI69" s="348"/>
+      <c r="AJ69" s="348"/>
+      <c r="AK69" s="348"/>
+      <c r="AL69" s="348"/>
+      <c r="AM69" s="348"/>
+      <c r="AN69" s="348"/>
+      <c r="AO69" s="348"/>
+      <c r="AP69" s="348"/>
+      <c r="AQ69" s="348"/>
+      <c r="AR69" s="348"/>
+      <c r="AS69" s="348"/>
+      <c r="AT69" s="348"/>
+      <c r="AU69" s="348"/>
+      <c r="AV69" s="348"/>
+      <c r="AW69" s="348"/>
+      <c r="AX69" s="348"/>
     </row>
     <row r="70" spans="1:75" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="320" t="s">
+      <c r="A70" s="323" t="s">
         <v>197</v>
       </c>
-      <c r="B70" s="320"/>
-      <c r="C70" s="320"/>
-      <c r="D70" s="320"/>
-      <c r="E70" s="320"/>
-      <c r="F70" s="320"/>
-      <c r="G70" s="320"/>
-      <c r="H70" s="320"/>
-      <c r="I70" s="320"/>
-      <c r="J70" s="320"/>
-      <c r="K70" s="320"/>
-      <c r="L70" s="320"/>
-      <c r="M70" s="320"/>
-      <c r="N70" s="320"/>
-      <c r="P70" s="348" t="s">
+      <c r="B70" s="323"/>
+      <c r="C70" s="323"/>
+      <c r="D70" s="323"/>
+      <c r="E70" s="323"/>
+      <c r="F70" s="323"/>
+      <c r="G70" s="323"/>
+      <c r="H70" s="323"/>
+      <c r="I70" s="323"/>
+      <c r="J70" s="323"/>
+      <c r="K70" s="323"/>
+      <c r="L70" s="323"/>
+      <c r="M70" s="323"/>
+      <c r="N70" s="323"/>
+      <c r="P70" s="351" t="s">
         <v>200</v>
       </c>
-      <c r="Q70" s="348"/>
-      <c r="R70" s="348"/>
-      <c r="S70" s="348"/>
-      <c r="T70" s="348"/>
-      <c r="U70" s="348"/>
-      <c r="V70" s="348"/>
-      <c r="W70" s="348"/>
-      <c r="X70" s="348"/>
-      <c r="Y70" s="348"/>
-      <c r="Z70" s="348"/>
-      <c r="AA70" s="348"/>
-      <c r="AB70" s="348"/>
-      <c r="AC70" s="348"/>
+      <c r="Q70" s="351"/>
+      <c r="R70" s="351"/>
+      <c r="S70" s="351"/>
+      <c r="T70" s="351"/>
+      <c r="U70" s="351"/>
+      <c r="V70" s="351"/>
+      <c r="W70" s="351"/>
+      <c r="X70" s="351"/>
+      <c r="Y70" s="351"/>
+      <c r="Z70" s="351"/>
+      <c r="AA70" s="351"/>
+      <c r="AB70" s="351"/>
+      <c r="AC70" s="351"/>
       <c r="AD70" s="106"/>
-      <c r="AE70" s="348" t="s">
+      <c r="AE70" s="351" t="s">
         <v>201</v>
       </c>
-      <c r="AF70" s="348"/>
-      <c r="AG70" s="348"/>
-      <c r="AH70" s="348"/>
-      <c r="AI70" s="348"/>
-      <c r="AJ70" s="348"/>
-      <c r="AK70" s="348"/>
-      <c r="AL70" s="348"/>
-      <c r="AM70" s="348"/>
-      <c r="AN70" s="348"/>
-      <c r="AO70" s="348"/>
-      <c r="AP70" s="348"/>
-      <c r="AQ70" s="348"/>
-      <c r="AR70" s="348"/>
+      <c r="AF70" s="351"/>
+      <c r="AG70" s="351"/>
+      <c r="AH70" s="351"/>
+      <c r="AI70" s="351"/>
+      <c r="AJ70" s="351"/>
+      <c r="AK70" s="351"/>
+      <c r="AL70" s="351"/>
+      <c r="AM70" s="351"/>
+      <c r="AN70" s="351"/>
+      <c r="AO70" s="351"/>
+      <c r="AP70" s="351"/>
+      <c r="AQ70" s="351"/>
+      <c r="AR70" s="351"/>
       <c r="AS70" s="107"/>
-      <c r="AT70" s="348" t="s">
+      <c r="AT70" s="351" t="s">
         <v>202</v>
       </c>
-      <c r="AU70" s="348"/>
-      <c r="AV70" s="348"/>
-      <c r="AW70" s="348"/>
-      <c r="AX70" s="348"/>
-      <c r="AY70" s="348"/>
-      <c r="AZ70" s="348"/>
-      <c r="BA70" s="348"/>
-      <c r="BB70" s="348"/>
-      <c r="BC70" s="348"/>
-      <c r="BD70" s="348"/>
-      <c r="BE70" s="348"/>
-      <c r="BF70" s="348"/>
-      <c r="BG70" s="348"/>
+      <c r="AU70" s="351"/>
+      <c r="AV70" s="351"/>
+      <c r="AW70" s="351"/>
+      <c r="AX70" s="351"/>
+      <c r="AY70" s="351"/>
+      <c r="AZ70" s="351"/>
+      <c r="BA70" s="351"/>
+      <c r="BB70" s="351"/>
+      <c r="BC70" s="351"/>
+      <c r="BD70" s="351"/>
+      <c r="BE70" s="351"/>
+      <c r="BF70" s="351"/>
+      <c r="BG70" s="351"/>
     </row>
     <row r="71" spans="1:75" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
@@ -9845,22 +9845,22 @@
       <c r="BG71" s="4">
         <v>2</v>
       </c>
-      <c r="BI71" s="328" t="s">
+      <c r="BI71" s="331" t="s">
         <v>164</v>
       </c>
-      <c r="BJ71" s="328"/>
-      <c r="BK71" s="328"/>
-      <c r="BL71" s="328"/>
-      <c r="BM71" s="328"/>
-      <c r="BN71" s="328"/>
-      <c r="BO71" s="328"/>
-      <c r="BP71" s="328"/>
-      <c r="BQ71" s="328"/>
-      <c r="BR71" s="328"/>
-      <c r="BS71" s="328"/>
-      <c r="BT71" s="328"/>
-      <c r="BU71" s="328"/>
-      <c r="BV71" s="328"/>
+      <c r="BJ71" s="331"/>
+      <c r="BK71" s="331"/>
+      <c r="BL71" s="331"/>
+      <c r="BM71" s="331"/>
+      <c r="BN71" s="331"/>
+      <c r="BO71" s="331"/>
+      <c r="BP71" s="331"/>
+      <c r="BQ71" s="331"/>
+      <c r="BR71" s="331"/>
+      <c r="BS71" s="331"/>
+      <c r="BT71" s="331"/>
+      <c r="BU71" s="331"/>
+      <c r="BV71" s="331"/>
     </row>
     <row r="72" spans="1:75" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
@@ -12638,31 +12638,31 @@
       </c>
     </row>
     <row r="85" spans="1:89" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="335" t="s">
+      <c r="A85" s="338" t="s">
         <v>192</v>
       </c>
-      <c r="B85" s="335"/>
-      <c r="C85" s="335"/>
-      <c r="D85" s="340" t="s">
+      <c r="B85" s="338"/>
+      <c r="C85" s="338"/>
+      <c r="D85" s="343" t="s">
         <v>193</v>
       </c>
-      <c r="E85" s="340"/>
-      <c r="F85" s="340"/>
-      <c r="G85" s="341" t="s">
+      <c r="E85" s="343"/>
+      <c r="F85" s="343"/>
+      <c r="G85" s="344" t="s">
         <v>194</v>
       </c>
-      <c r="H85" s="341"/>
-      <c r="I85" s="341"/>
-      <c r="J85" s="336" t="s">
+      <c r="H85" s="344"/>
+      <c r="I85" s="344"/>
+      <c r="J85" s="339" t="s">
         <v>195</v>
       </c>
-      <c r="K85" s="336"/>
-      <c r="L85" s="336"/>
-      <c r="M85" s="337" t="s">
+      <c r="K85" s="339"/>
+      <c r="L85" s="339"/>
+      <c r="M85" s="340" t="s">
         <v>196</v>
       </c>
-      <c r="N85" s="337"/>
-      <c r="O85" s="337"/>
+      <c r="N85" s="340"/>
+      <c r="O85" s="340"/>
       <c r="BI85" s="12" t="s">
         <v>92</v>
       </c>
@@ -12707,153 +12707,153 @@
       </c>
     </row>
     <row r="86" spans="1:89" ht="14.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="BI86" s="335"/>
-      <c r="BJ86" s="335"/>
-      <c r="BK86" s="335"/>
-      <c r="BL86" s="340"/>
-      <c r="BM86" s="340"/>
-      <c r="BN86" s="340"/>
-      <c r="BO86" s="341"/>
-      <c r="BP86" s="341"/>
-      <c r="BQ86" s="341"/>
-      <c r="BR86" s="336"/>
-      <c r="BS86" s="336"/>
-      <c r="BT86" s="336"/>
-      <c r="BU86" s="337"/>
-      <c r="BV86" s="337"/>
-      <c r="BW86" s="337"/>
+      <c r="BI86" s="338"/>
+      <c r="BJ86" s="338"/>
+      <c r="BK86" s="338"/>
+      <c r="BL86" s="343"/>
+      <c r="BM86" s="343"/>
+      <c r="BN86" s="343"/>
+      <c r="BO86" s="344"/>
+      <c r="BP86" s="344"/>
+      <c r="BQ86" s="344"/>
+      <c r="BR86" s="339"/>
+      <c r="BS86" s="339"/>
+      <c r="BT86" s="339"/>
+      <c r="BU86" s="340"/>
+      <c r="BV86" s="340"/>
+      <c r="BW86" s="340"/>
     </row>
     <row r="87" spans="1:89" ht="20.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="327" t="s">
+      <c r="A87" s="330" t="s">
         <v>163</v>
       </c>
-      <c r="B87" s="327"/>
-      <c r="C87" s="327"/>
-      <c r="D87" s="327"/>
-      <c r="E87" s="327"/>
-      <c r="F87" s="327"/>
-      <c r="G87" s="327"/>
-      <c r="H87" s="327"/>
-      <c r="I87" s="327"/>
-      <c r="J87" s="327"/>
-      <c r="K87" s="327"/>
-      <c r="L87" s="327"/>
-      <c r="M87" s="327"/>
-      <c r="N87" s="327"/>
-      <c r="O87" s="327"/>
-      <c r="P87" s="327"/>
-      <c r="Q87" s="327"/>
-      <c r="R87" s="327"/>
-      <c r="S87" s="327"/>
-      <c r="T87" s="327"/>
-      <c r="U87" s="327"/>
-      <c r="V87" s="327"/>
-      <c r="W87" s="327"/>
-      <c r="X87" s="327"/>
-      <c r="Y87" s="327"/>
-      <c r="Z87" s="327"/>
-      <c r="AA87" s="327"/>
-      <c r="AB87" s="327"/>
-      <c r="AC87" s="327"/>
-      <c r="AD87" s="327"/>
+      <c r="B87" s="330"/>
+      <c r="C87" s="330"/>
+      <c r="D87" s="330"/>
+      <c r="E87" s="330"/>
+      <c r="F87" s="330"/>
+      <c r="G87" s="330"/>
+      <c r="H87" s="330"/>
+      <c r="I87" s="330"/>
+      <c r="J87" s="330"/>
+      <c r="K87" s="330"/>
+      <c r="L87" s="330"/>
+      <c r="M87" s="330"/>
+      <c r="N87" s="330"/>
+      <c r="O87" s="330"/>
+      <c r="P87" s="330"/>
+      <c r="Q87" s="330"/>
+      <c r="R87" s="330"/>
+      <c r="S87" s="330"/>
+      <c r="T87" s="330"/>
+      <c r="U87" s="330"/>
+      <c r="V87" s="330"/>
+      <c r="W87" s="330"/>
+      <c r="X87" s="330"/>
+      <c r="Y87" s="330"/>
+      <c r="Z87" s="330"/>
+      <c r="AA87" s="330"/>
+      <c r="AB87" s="330"/>
+      <c r="AC87" s="330"/>
+      <c r="AD87" s="330"/>
     </row>
     <row r="88" spans="1:89" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="320" t="s">
+      <c r="A88" s="323" t="s">
         <v>257</v>
       </c>
-      <c r="B88" s="320"/>
-      <c r="C88" s="320"/>
-      <c r="D88" s="320"/>
-      <c r="E88" s="320"/>
-      <c r="F88" s="320"/>
-      <c r="G88" s="320"/>
-      <c r="H88" s="320"/>
-      <c r="I88" s="320"/>
-      <c r="J88" s="320"/>
-      <c r="K88" s="320"/>
-      <c r="L88" s="320"/>
-      <c r="M88" s="320"/>
-      <c r="N88" s="320"/>
-      <c r="P88" s="328" t="s">
+      <c r="B88" s="323"/>
+      <c r="C88" s="323"/>
+      <c r="D88" s="323"/>
+      <c r="E88" s="323"/>
+      <c r="F88" s="323"/>
+      <c r="G88" s="323"/>
+      <c r="H88" s="323"/>
+      <c r="I88" s="323"/>
+      <c r="J88" s="323"/>
+      <c r="K88" s="323"/>
+      <c r="L88" s="323"/>
+      <c r="M88" s="323"/>
+      <c r="N88" s="323"/>
+      <c r="P88" s="331" t="s">
         <v>258</v>
       </c>
-      <c r="Q88" s="328"/>
-      <c r="R88" s="328"/>
-      <c r="S88" s="328"/>
-      <c r="T88" s="328"/>
-      <c r="U88" s="328"/>
-      <c r="V88" s="328"/>
-      <c r="W88" s="328"/>
-      <c r="X88" s="328"/>
-      <c r="Y88" s="328"/>
-      <c r="Z88" s="328"/>
-      <c r="AA88" s="328"/>
-      <c r="AB88" s="328"/>
-      <c r="AC88" s="328"/>
-      <c r="AE88" s="320" t="s">
+      <c r="Q88" s="331"/>
+      <c r="R88" s="331"/>
+      <c r="S88" s="331"/>
+      <c r="T88" s="331"/>
+      <c r="U88" s="331"/>
+      <c r="V88" s="331"/>
+      <c r="W88" s="331"/>
+      <c r="X88" s="331"/>
+      <c r="Y88" s="331"/>
+      <c r="Z88" s="331"/>
+      <c r="AA88" s="331"/>
+      <c r="AB88" s="331"/>
+      <c r="AC88" s="331"/>
+      <c r="AE88" s="323" t="s">
         <v>259</v>
       </c>
-      <c r="AF88" s="320"/>
-      <c r="AG88" s="320"/>
-      <c r="AH88" s="320"/>
-      <c r="AI88" s="320"/>
-      <c r="AJ88" s="320"/>
-      <c r="AK88" s="320"/>
-      <c r="AL88" s="320"/>
-      <c r="AM88" s="320"/>
-      <c r="AN88" s="320"/>
-      <c r="AO88" s="320"/>
-      <c r="AP88" s="320"/>
-      <c r="AQ88" s="320"/>
-      <c r="AR88" s="320"/>
-      <c r="AT88" s="320" t="s">
+      <c r="AF88" s="323"/>
+      <c r="AG88" s="323"/>
+      <c r="AH88" s="323"/>
+      <c r="AI88" s="323"/>
+      <c r="AJ88" s="323"/>
+      <c r="AK88" s="323"/>
+      <c r="AL88" s="323"/>
+      <c r="AM88" s="323"/>
+      <c r="AN88" s="323"/>
+      <c r="AO88" s="323"/>
+      <c r="AP88" s="323"/>
+      <c r="AQ88" s="323"/>
+      <c r="AR88" s="323"/>
+      <c r="AT88" s="323" t="s">
         <v>260</v>
       </c>
-      <c r="AU88" s="320"/>
-      <c r="AV88" s="320"/>
-      <c r="AW88" s="320"/>
-      <c r="AX88" s="320"/>
-      <c r="AY88" s="320"/>
-      <c r="AZ88" s="320"/>
-      <c r="BA88" s="320"/>
-      <c r="BB88" s="320"/>
-      <c r="BC88" s="320"/>
-      <c r="BD88" s="320"/>
-      <c r="BE88" s="320"/>
-      <c r="BF88" s="320"/>
-      <c r="BG88" s="320"/>
-      <c r="BI88" s="320" t="s">
+      <c r="AU88" s="323"/>
+      <c r="AV88" s="323"/>
+      <c r="AW88" s="323"/>
+      <c r="AX88" s="323"/>
+      <c r="AY88" s="323"/>
+      <c r="AZ88" s="323"/>
+      <c r="BA88" s="323"/>
+      <c r="BB88" s="323"/>
+      <c r="BC88" s="323"/>
+      <c r="BD88" s="323"/>
+      <c r="BE88" s="323"/>
+      <c r="BF88" s="323"/>
+      <c r="BG88" s="323"/>
+      <c r="BI88" s="323" t="s">
         <v>261</v>
       </c>
-      <c r="BJ88" s="320"/>
-      <c r="BK88" s="320"/>
-      <c r="BL88" s="320"/>
-      <c r="BM88" s="320"/>
-      <c r="BN88" s="320"/>
-      <c r="BO88" s="320"/>
-      <c r="BP88" s="320"/>
-      <c r="BQ88" s="320"/>
-      <c r="BR88" s="320"/>
-      <c r="BS88" s="320"/>
-      <c r="BT88" s="320"/>
-      <c r="BU88" s="320"/>
-      <c r="BV88" s="320"/>
-      <c r="BX88" s="320" t="s">
+      <c r="BJ88" s="323"/>
+      <c r="BK88" s="323"/>
+      <c r="BL88" s="323"/>
+      <c r="BM88" s="323"/>
+      <c r="BN88" s="323"/>
+      <c r="BO88" s="323"/>
+      <c r="BP88" s="323"/>
+      <c r="BQ88" s="323"/>
+      <c r="BR88" s="323"/>
+      <c r="BS88" s="323"/>
+      <c r="BT88" s="323"/>
+      <c r="BU88" s="323"/>
+      <c r="BV88" s="323"/>
+      <c r="BX88" s="323" t="s">
         <v>262</v>
       </c>
-      <c r="BY88" s="320"/>
-      <c r="BZ88" s="320"/>
-      <c r="CA88" s="320"/>
-      <c r="CB88" s="320"/>
-      <c r="CC88" s="320"/>
-      <c r="CD88" s="320"/>
-      <c r="CE88" s="320"/>
-      <c r="CF88" s="320"/>
-      <c r="CG88" s="320"/>
-      <c r="CH88" s="320"/>
-      <c r="CI88" s="320"/>
-      <c r="CJ88" s="320"/>
-      <c r="CK88" s="320"/>
+      <c r="BY88" s="323"/>
+      <c r="BZ88" s="323"/>
+      <c r="CA88" s="323"/>
+      <c r="CB88" s="323"/>
+      <c r="CC88" s="323"/>
+      <c r="CD88" s="323"/>
+      <c r="CE88" s="323"/>
+      <c r="CF88" s="323"/>
+      <c r="CG88" s="323"/>
+      <c r="CH88" s="323"/>
+      <c r="CI88" s="323"/>
+      <c r="CJ88" s="323"/>
+      <c r="CK88" s="323"/>
     </row>
     <row r="89" spans="1:89" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
@@ -13439,7 +13439,7 @@
       <c r="AE91" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AF91" s="37" t="s">
+      <c r="AF91" s="8" t="s">
         <v>11</v>
       </c>
       <c r="AG91" s="9" t="s">
@@ -13481,7 +13481,7 @@
       <c r="AT91" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AU91" s="37" t="s">
+      <c r="AU91" s="8" t="s">
         <v>11</v>
       </c>
       <c r="AV91" s="9" t="s">
@@ -13693,10 +13693,10 @@
       <c r="AE92" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AF92" s="37" t="s">
+      <c r="AF92" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AG92" s="38" t="s">
+      <c r="AG92" s="9" t="s">
         <v>24</v>
       </c>
       <c r="AH92" s="9" t="s">
@@ -13735,10 +13735,10 @@
       <c r="AT92" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AU92" s="37" t="s">
+      <c r="AU92" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AV92" s="38" t="s">
+      <c r="AV92" s="9" t="s">
         <v>24</v>
       </c>
       <c r="AW92" s="9" t="s">
@@ -13947,13 +13947,13 @@
       <c r="AE93" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AF93" s="37" t="s">
+      <c r="AF93" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="AG93" s="38" t="s">
+      <c r="AG93" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AH93" s="38" t="s">
+      <c r="AH93" s="9" t="s">
         <v>36</v>
       </c>
       <c r="AI93" s="9" t="s">
@@ -13989,10 +13989,10 @@
       <c r="AT93" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AU93" s="37" t="s">
+      <c r="AU93" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="AV93" s="38" t="s">
+      <c r="AV93" s="9" t="s">
         <v>25</v>
       </c>
       <c r="AW93" s="38" t="s">
@@ -14201,10 +14201,10 @@
       <c r="AE94" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AF94" s="37" t="s">
+      <c r="AF94" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="AG94" s="38" t="s">
+      <c r="AG94" s="9" t="s">
         <v>26</v>
       </c>
       <c r="AH94" s="38" t="s">
@@ -14243,7 +14243,7 @@
       <c r="AT94" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AU94" s="37" t="s">
+      <c r="AU94" s="8" t="s">
         <v>14</v>
       </c>
       <c r="AV94" s="38" t="s">
@@ -14455,10 +14455,10 @@
       <c r="AE95" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AF95" s="37" t="s">
+      <c r="AF95" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="AG95" s="38" t="s">
+      <c r="AG95" s="9" t="s">
         <v>27</v>
       </c>
       <c r="AH95" s="9" t="s">
@@ -14497,7 +14497,7 @@
       <c r="AT95" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AU95" s="37" t="s">
+      <c r="AU95" s="8" t="s">
         <v>15</v>
       </c>
       <c r="AV95" s="38" t="s">
@@ -14709,7 +14709,7 @@
       <c r="AE96" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AF96" s="37" t="s">
+      <c r="AF96" s="8" t="s">
         <v>16</v>
       </c>
       <c r="AG96" s="38" t="s">
@@ -14727,7 +14727,7 @@
       <c r="AK96" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="AL96" s="38" t="s">
+      <c r="AL96" s="9" t="s">
         <v>70</v>
       </c>
       <c r="AM96" s="9" t="s">
@@ -14751,7 +14751,7 @@
       <c r="AT96" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AU96" s="37" t="s">
+      <c r="AU96" s="8" t="s">
         <v>16</v>
       </c>
       <c r="AV96" s="38" t="s">
@@ -14769,7 +14769,7 @@
       <c r="AZ96" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="BA96" s="38" t="s">
+      <c r="BA96" s="9" t="s">
         <v>70</v>
       </c>
       <c r="BB96" s="9" t="s">
@@ -14984,7 +14984,7 @@
       <c r="AL97" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="AM97" s="38" t="s">
+      <c r="AM97" s="9" t="s">
         <v>74</v>
       </c>
       <c r="AN97" s="9" t="s">
@@ -15026,7 +15026,7 @@
       <c r="BA97" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BB97" s="38" t="s">
+      <c r="BB97" s="9" t="s">
         <v>74</v>
       </c>
       <c r="BC97" s="9" t="s">
@@ -16400,106 +16400,106 @@
       </c>
     </row>
     <row r="103" spans="1:135" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="344" t="s">
+      <c r="A103" s="347" t="s">
         <v>270</v>
       </c>
-      <c r="B103" s="344"/>
-      <c r="C103" s="344"/>
-      <c r="D103" s="344"/>
-      <c r="E103" s="344"/>
-      <c r="F103" s="344"/>
-      <c r="G103" s="344"/>
-      <c r="H103" s="344"/>
-      <c r="I103" s="344"/>
-      <c r="J103" s="344"/>
-      <c r="K103" s="344"/>
-      <c r="L103" s="344"/>
-      <c r="M103" s="344"/>
-      <c r="N103" s="344"/>
+      <c r="B103" s="347"/>
+      <c r="C103" s="347"/>
+      <c r="D103" s="347"/>
+      <c r="E103" s="347"/>
+      <c r="F103" s="347"/>
+      <c r="G103" s="347"/>
+      <c r="H103" s="347"/>
+      <c r="I103" s="347"/>
+      <c r="J103" s="347"/>
+      <c r="K103" s="347"/>
+      <c r="L103" s="347"/>
+      <c r="M103" s="347"/>
+      <c r="N103" s="347"/>
       <c r="O103" s="207"/>
-      <c r="P103" s="344" t="s">
+      <c r="P103" s="347" t="s">
         <v>271</v>
       </c>
-      <c r="Q103" s="344"/>
-      <c r="R103" s="344"/>
-      <c r="S103" s="344"/>
-      <c r="T103" s="344"/>
-      <c r="U103" s="344"/>
-      <c r="V103" s="344"/>
-      <c r="W103" s="344"/>
-      <c r="X103" s="344"/>
-      <c r="Y103" s="344"/>
-      <c r="Z103" s="344"/>
-      <c r="AA103" s="344"/>
-      <c r="AB103" s="344"/>
-      <c r="AC103" s="344"/>
+      <c r="Q103" s="347"/>
+      <c r="R103" s="347"/>
+      <c r="S103" s="347"/>
+      <c r="T103" s="347"/>
+      <c r="U103" s="347"/>
+      <c r="V103" s="347"/>
+      <c r="W103" s="347"/>
+      <c r="X103" s="347"/>
+      <c r="Y103" s="347"/>
+      <c r="Z103" s="347"/>
+      <c r="AA103" s="347"/>
+      <c r="AB103" s="347"/>
+      <c r="AC103" s="347"/>
       <c r="AD103" s="207"/>
-      <c r="AE103" s="344" t="s">
+      <c r="AE103" s="347" t="s">
         <v>272</v>
       </c>
-      <c r="AF103" s="344"/>
-      <c r="AG103" s="344"/>
-      <c r="AH103" s="344"/>
-      <c r="AI103" s="344"/>
-      <c r="AJ103" s="344"/>
-      <c r="AK103" s="344"/>
-      <c r="AL103" s="344"/>
-      <c r="AM103" s="344"/>
-      <c r="AN103" s="344"/>
-      <c r="AO103" s="344"/>
-      <c r="AP103" s="344"/>
-      <c r="AQ103" s="344"/>
-      <c r="AR103" s="344"/>
-      <c r="AT103" s="344" t="s">
+      <c r="AF103" s="347"/>
+      <c r="AG103" s="347"/>
+      <c r="AH103" s="347"/>
+      <c r="AI103" s="347"/>
+      <c r="AJ103" s="347"/>
+      <c r="AK103" s="347"/>
+      <c r="AL103" s="347"/>
+      <c r="AM103" s="347"/>
+      <c r="AN103" s="347"/>
+      <c r="AO103" s="347"/>
+      <c r="AP103" s="347"/>
+      <c r="AQ103" s="347"/>
+      <c r="AR103" s="347"/>
+      <c r="AT103" s="347" t="s">
         <v>273</v>
       </c>
-      <c r="AU103" s="344"/>
-      <c r="AV103" s="344"/>
-      <c r="AW103" s="344"/>
-      <c r="AX103" s="344"/>
-      <c r="AY103" s="344"/>
-      <c r="AZ103" s="344"/>
-      <c r="BA103" s="344"/>
-      <c r="BB103" s="344"/>
-      <c r="BC103" s="344"/>
-      <c r="BD103" s="344"/>
-      <c r="BE103" s="344"/>
-      <c r="BF103" s="344"/>
-      <c r="BG103" s="344"/>
+      <c r="AU103" s="347"/>
+      <c r="AV103" s="347"/>
+      <c r="AW103" s="347"/>
+      <c r="AX103" s="347"/>
+      <c r="AY103" s="347"/>
+      <c r="AZ103" s="347"/>
+      <c r="BA103" s="347"/>
+      <c r="BB103" s="347"/>
+      <c r="BC103" s="347"/>
+      <c r="BD103" s="347"/>
+      <c r="BE103" s="347"/>
+      <c r="BF103" s="347"/>
+      <c r="BG103" s="347"/>
       <c r="BH103" s="207"/>
-      <c r="BI103" s="344" t="s">
+      <c r="BI103" s="347" t="s">
         <v>274</v>
       </c>
-      <c r="BJ103" s="344"/>
-      <c r="BK103" s="344"/>
-      <c r="BL103" s="344"/>
-      <c r="BM103" s="344"/>
-      <c r="BN103" s="344"/>
-      <c r="BO103" s="344"/>
-      <c r="BP103" s="344"/>
-      <c r="BQ103" s="344"/>
-      <c r="BR103" s="344"/>
-      <c r="BS103" s="344"/>
-      <c r="BT103" s="344"/>
-      <c r="BU103" s="344"/>
-      <c r="BV103" s="344"/>
+      <c r="BJ103" s="347"/>
+      <c r="BK103" s="347"/>
+      <c r="BL103" s="347"/>
+      <c r="BM103" s="347"/>
+      <c r="BN103" s="347"/>
+      <c r="BO103" s="347"/>
+      <c r="BP103" s="347"/>
+      <c r="BQ103" s="347"/>
+      <c r="BR103" s="347"/>
+      <c r="BS103" s="347"/>
+      <c r="BT103" s="347"/>
+      <c r="BU103" s="347"/>
+      <c r="BV103" s="347"/>
       <c r="BW103" s="207"/>
-      <c r="BX103" s="344" t="s">
+      <c r="BX103" s="347" t="s">
         <v>275</v>
       </c>
-      <c r="BY103" s="344"/>
-      <c r="BZ103" s="344"/>
-      <c r="CA103" s="344"/>
-      <c r="CB103" s="344"/>
-      <c r="CC103" s="344"/>
-      <c r="CD103" s="344"/>
-      <c r="CE103" s="344"/>
-      <c r="CF103" s="344"/>
-      <c r="CG103" s="344"/>
-      <c r="CH103" s="344"/>
-      <c r="CI103" s="344"/>
-      <c r="CJ103" s="344"/>
-      <c r="CK103" s="344"/>
+      <c r="BY103" s="347"/>
+      <c r="BZ103" s="347"/>
+      <c r="CA103" s="347"/>
+      <c r="CB103" s="347"/>
+      <c r="CC103" s="347"/>
+      <c r="CD103" s="347"/>
+      <c r="CE103" s="347"/>
+      <c r="CF103" s="347"/>
+      <c r="CG103" s="347"/>
+      <c r="CH103" s="347"/>
+      <c r="CI103" s="347"/>
+      <c r="CJ103" s="347"/>
+      <c r="CK103" s="347"/>
       <c r="CL103" s="210"/>
       <c r="CM103" s="76"/>
       <c r="CN103" s="76"/>
@@ -17042,55 +17042,55 @@
       </c>
       <c r="CL105" s="210"/>
       <c r="CM105" s="76"/>
-      <c r="CN105" s="320" t="s">
+      <c r="CN105" s="323" t="s">
         <v>367</v>
       </c>
-      <c r="CO105" s="320"/>
-      <c r="CP105" s="320"/>
-      <c r="CQ105" s="320"/>
-      <c r="CR105" s="320"/>
-      <c r="CS105" s="320"/>
-      <c r="CT105" s="320"/>
-      <c r="CU105" s="320"/>
-      <c r="CV105" s="320"/>
-      <c r="CW105" s="320"/>
-      <c r="CX105" s="320"/>
-      <c r="CY105" s="320"/>
-      <c r="CZ105" s="320"/>
-      <c r="DA105" s="320"/>
+      <c r="CO105" s="323"/>
+      <c r="CP105" s="323"/>
+      <c r="CQ105" s="323"/>
+      <c r="CR105" s="323"/>
+      <c r="CS105" s="323"/>
+      <c r="CT105" s="323"/>
+      <c r="CU105" s="323"/>
+      <c r="CV105" s="323"/>
+      <c r="CW105" s="323"/>
+      <c r="CX105" s="323"/>
+      <c r="CY105" s="323"/>
+      <c r="CZ105" s="323"/>
+      <c r="DA105" s="323"/>
       <c r="DB105" s="76"/>
-      <c r="DC105" s="320" t="s">
+      <c r="DC105" s="323" t="s">
         <v>368</v>
       </c>
-      <c r="DD105" s="320"/>
-      <c r="DE105" s="320"/>
-      <c r="DF105" s="320"/>
-      <c r="DG105" s="320"/>
-      <c r="DH105" s="320"/>
-      <c r="DI105" s="320"/>
-      <c r="DJ105" s="320"/>
-      <c r="DK105" s="320"/>
-      <c r="DL105" s="320"/>
-      <c r="DM105" s="320"/>
-      <c r="DN105" s="320"/>
-      <c r="DO105" s="320"/>
-      <c r="DP105" s="320"/>
-      <c r="DR105" s="320" t="s">
+      <c r="DD105" s="323"/>
+      <c r="DE105" s="323"/>
+      <c r="DF105" s="323"/>
+      <c r="DG105" s="323"/>
+      <c r="DH105" s="323"/>
+      <c r="DI105" s="323"/>
+      <c r="DJ105" s="323"/>
+      <c r="DK105" s="323"/>
+      <c r="DL105" s="323"/>
+      <c r="DM105" s="323"/>
+      <c r="DN105" s="323"/>
+      <c r="DO105" s="323"/>
+      <c r="DP105" s="323"/>
+      <c r="DR105" s="323" t="s">
         <v>371</v>
       </c>
-      <c r="DS105" s="320"/>
-      <c r="DT105" s="320"/>
-      <c r="DU105" s="320"/>
-      <c r="DV105" s="320"/>
-      <c r="DW105" s="320"/>
-      <c r="DX105" s="320"/>
-      <c r="DY105" s="320"/>
-      <c r="DZ105" s="320"/>
-      <c r="EA105" s="320"/>
-      <c r="EB105" s="320"/>
-      <c r="EC105" s="320"/>
-      <c r="ED105" s="320"/>
-      <c r="EE105" s="320"/>
+      <c r="DS105" s="323"/>
+      <c r="DT105" s="323"/>
+      <c r="DU105" s="323"/>
+      <c r="DV105" s="323"/>
+      <c r="DW105" s="323"/>
+      <c r="DX105" s="323"/>
+      <c r="DY105" s="323"/>
+      <c r="DZ105" s="323"/>
+      <c r="EA105" s="323"/>
+      <c r="EB105" s="323"/>
+      <c r="EC105" s="323"/>
+      <c r="ED105" s="323"/>
+      <c r="EE105" s="323"/>
     </row>
     <row r="106" spans="1:135" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
@@ -21743,107 +21743,107 @@
       </c>
     </row>
     <row r="118" spans="1:135" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="339" t="s">
+      <c r="A118" s="342" t="s">
         <v>251</v>
       </c>
-      <c r="B118" s="339"/>
-      <c r="C118" s="339"/>
-      <c r="D118" s="339"/>
-      <c r="E118" s="339"/>
-      <c r="F118" s="339"/>
-      <c r="G118" s="339"/>
-      <c r="H118" s="339"/>
-      <c r="I118" s="339"/>
-      <c r="J118" s="339"/>
-      <c r="K118" s="339"/>
-      <c r="L118" s="339"/>
-      <c r="M118" s="339"/>
-      <c r="N118" s="339"/>
+      <c r="B118" s="342"/>
+      <c r="C118" s="342"/>
+      <c r="D118" s="342"/>
+      <c r="E118" s="342"/>
+      <c r="F118" s="342"/>
+      <c r="G118" s="342"/>
+      <c r="H118" s="342"/>
+      <c r="I118" s="342"/>
+      <c r="J118" s="342"/>
+      <c r="K118" s="342"/>
+      <c r="L118" s="342"/>
+      <c r="M118" s="342"/>
+      <c r="N118" s="342"/>
       <c r="O118" s="205"/>
-      <c r="P118" s="339" t="s">
+      <c r="P118" s="342" t="s">
         <v>252</v>
       </c>
-      <c r="Q118" s="339"/>
-      <c r="R118" s="339"/>
-      <c r="S118" s="339"/>
-      <c r="T118" s="339"/>
-      <c r="U118" s="339"/>
-      <c r="V118" s="339"/>
-      <c r="W118" s="339"/>
-      <c r="X118" s="339"/>
-      <c r="Y118" s="339"/>
-      <c r="Z118" s="339"/>
-      <c r="AA118" s="339"/>
-      <c r="AB118" s="339"/>
-      <c r="AC118" s="339"/>
+      <c r="Q118" s="342"/>
+      <c r="R118" s="342"/>
+      <c r="S118" s="342"/>
+      <c r="T118" s="342"/>
+      <c r="U118" s="342"/>
+      <c r="V118" s="342"/>
+      <c r="W118" s="342"/>
+      <c r="X118" s="342"/>
+      <c r="Y118" s="342"/>
+      <c r="Z118" s="342"/>
+      <c r="AA118" s="342"/>
+      <c r="AB118" s="342"/>
+      <c r="AC118" s="342"/>
       <c r="AD118" s="205"/>
-      <c r="AE118" s="339" t="s">
+      <c r="AE118" s="342" t="s">
         <v>253</v>
       </c>
-      <c r="AF118" s="339"/>
-      <c r="AG118" s="339"/>
-      <c r="AH118" s="339"/>
-      <c r="AI118" s="339"/>
-      <c r="AJ118" s="339"/>
-      <c r="AK118" s="339"/>
-      <c r="AL118" s="339"/>
-      <c r="AM118" s="339"/>
-      <c r="AN118" s="339"/>
-      <c r="AO118" s="339"/>
-      <c r="AP118" s="339"/>
-      <c r="AQ118" s="339"/>
-      <c r="AR118" s="339"/>
+      <c r="AF118" s="342"/>
+      <c r="AG118" s="342"/>
+      <c r="AH118" s="342"/>
+      <c r="AI118" s="342"/>
+      <c r="AJ118" s="342"/>
+      <c r="AK118" s="342"/>
+      <c r="AL118" s="342"/>
+      <c r="AM118" s="342"/>
+      <c r="AN118" s="342"/>
+      <c r="AO118" s="342"/>
+      <c r="AP118" s="342"/>
+      <c r="AQ118" s="342"/>
+      <c r="AR118" s="342"/>
       <c r="AS118" s="205"/>
-      <c r="AT118" s="339" t="s">
+      <c r="AT118" s="342" t="s">
         <v>254</v>
       </c>
-      <c r="AU118" s="339"/>
-      <c r="AV118" s="339"/>
-      <c r="AW118" s="339"/>
-      <c r="AX118" s="339"/>
-      <c r="AY118" s="339"/>
-      <c r="AZ118" s="339"/>
-      <c r="BA118" s="339"/>
-      <c r="BB118" s="339"/>
-      <c r="BC118" s="339"/>
-      <c r="BD118" s="339"/>
-      <c r="BE118" s="339"/>
-      <c r="BF118" s="339"/>
-      <c r="BG118" s="339"/>
+      <c r="AU118" s="342"/>
+      <c r="AV118" s="342"/>
+      <c r="AW118" s="342"/>
+      <c r="AX118" s="342"/>
+      <c r="AY118" s="342"/>
+      <c r="AZ118" s="342"/>
+      <c r="BA118" s="342"/>
+      <c r="BB118" s="342"/>
+      <c r="BC118" s="342"/>
+      <c r="BD118" s="342"/>
+      <c r="BE118" s="342"/>
+      <c r="BF118" s="342"/>
+      <c r="BG118" s="342"/>
       <c r="BH118" s="205"/>
-      <c r="BI118" s="339" t="s">
+      <c r="BI118" s="342" t="s">
         <v>255</v>
       </c>
-      <c r="BJ118" s="339"/>
-      <c r="BK118" s="339"/>
-      <c r="BL118" s="339"/>
-      <c r="BM118" s="339"/>
-      <c r="BN118" s="339"/>
-      <c r="BO118" s="339"/>
-      <c r="BP118" s="339"/>
-      <c r="BQ118" s="339"/>
-      <c r="BR118" s="339"/>
-      <c r="BS118" s="339"/>
-      <c r="BT118" s="339"/>
-      <c r="BU118" s="339"/>
-      <c r="BV118" s="339"/>
+      <c r="BJ118" s="342"/>
+      <c r="BK118" s="342"/>
+      <c r="BL118" s="342"/>
+      <c r="BM118" s="342"/>
+      <c r="BN118" s="342"/>
+      <c r="BO118" s="342"/>
+      <c r="BP118" s="342"/>
+      <c r="BQ118" s="342"/>
+      <c r="BR118" s="342"/>
+      <c r="BS118" s="342"/>
+      <c r="BT118" s="342"/>
+      <c r="BU118" s="342"/>
+      <c r="BV118" s="342"/>
       <c r="BW118" s="205"/>
-      <c r="BX118" s="339" t="s">
+      <c r="BX118" s="342" t="s">
         <v>256</v>
       </c>
-      <c r="BY118" s="339"/>
-      <c r="BZ118" s="339"/>
-      <c r="CA118" s="339"/>
-      <c r="CB118" s="339"/>
-      <c r="CC118" s="339"/>
-      <c r="CD118" s="339"/>
-      <c r="CE118" s="339"/>
-      <c r="CF118" s="339"/>
-      <c r="CG118" s="339"/>
-      <c r="CH118" s="339"/>
-      <c r="CI118" s="339"/>
-      <c r="CJ118" s="339"/>
-      <c r="CK118" s="339"/>
+      <c r="BY118" s="342"/>
+      <c r="BZ118" s="342"/>
+      <c r="CA118" s="342"/>
+      <c r="CB118" s="342"/>
+      <c r="CC118" s="342"/>
+      <c r="CD118" s="342"/>
+      <c r="CE118" s="342"/>
+      <c r="CF118" s="342"/>
+      <c r="CG118" s="342"/>
+      <c r="CH118" s="342"/>
+      <c r="CI118" s="342"/>
+      <c r="CJ118" s="342"/>
+      <c r="CK118" s="342"/>
       <c r="CL118" s="210"/>
       <c r="CM118" s="76"/>
       <c r="CN118" s="5" t="s">
@@ -22905,39 +22905,39 @@
       </c>
       <c r="CL121" s="205"/>
       <c r="CM121" s="205"/>
-      <c r="CN121" s="320" t="s">
+      <c r="CN121" s="323" t="s">
         <v>369</v>
       </c>
-      <c r="CO121" s="320"/>
-      <c r="CP121" s="320"/>
-      <c r="CQ121" s="320"/>
-      <c r="CR121" s="320"/>
-      <c r="CS121" s="320"/>
-      <c r="CT121" s="320"/>
-      <c r="CU121" s="320"/>
-      <c r="CV121" s="320"/>
-      <c r="CW121" s="320"/>
-      <c r="CX121" s="320"/>
-      <c r="CY121" s="320"/>
-      <c r="CZ121" s="320"/>
-      <c r="DA121" s="320"/>
+      <c r="CO121" s="323"/>
+      <c r="CP121" s="323"/>
+      <c r="CQ121" s="323"/>
+      <c r="CR121" s="323"/>
+      <c r="CS121" s="323"/>
+      <c r="CT121" s="323"/>
+      <c r="CU121" s="323"/>
+      <c r="CV121" s="323"/>
+      <c r="CW121" s="323"/>
+      <c r="CX121" s="323"/>
+      <c r="CY121" s="323"/>
+      <c r="CZ121" s="323"/>
+      <c r="DA121" s="323"/>
       <c r="DB121" s="205"/>
-      <c r="DC121" s="320" t="s">
+      <c r="DC121" s="323" t="s">
         <v>370</v>
       </c>
-      <c r="DD121" s="320"/>
-      <c r="DE121" s="320"/>
-      <c r="DF121" s="320"/>
-      <c r="DG121" s="320"/>
-      <c r="DH121" s="320"/>
-      <c r="DI121" s="320"/>
-      <c r="DJ121" s="320"/>
-      <c r="DK121" s="320"/>
-      <c r="DL121" s="320"/>
-      <c r="DM121" s="320"/>
-      <c r="DN121" s="320"/>
-      <c r="DO121" s="320"/>
-      <c r="DP121" s="320"/>
+      <c r="DD121" s="323"/>
+      <c r="DE121" s="323"/>
+      <c r="DF121" s="323"/>
+      <c r="DG121" s="323"/>
+      <c r="DH121" s="323"/>
+      <c r="DI121" s="323"/>
+      <c r="DJ121" s="323"/>
+      <c r="DK121" s="323"/>
+      <c r="DL121" s="323"/>
+      <c r="DM121" s="323"/>
+      <c r="DN121" s="323"/>
+      <c r="DO121" s="323"/>
+      <c r="DP121" s="323"/>
       <c r="DQ121" s="205"/>
       <c r="DR121" s="205"/>
       <c r="DS121" s="205"/>
@@ -26778,107 +26778,107 @@
       <c r="DS132" s="205"/>
     </row>
     <row r="133" spans="1:123" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="339" t="s">
+      <c r="A133" s="342" t="s">
         <v>265</v>
       </c>
-      <c r="B133" s="339"/>
-      <c r="C133" s="339"/>
-      <c r="D133" s="339"/>
-      <c r="E133" s="339"/>
-      <c r="F133" s="339"/>
-      <c r="G133" s="339"/>
-      <c r="H133" s="339"/>
-      <c r="I133" s="339"/>
-      <c r="J133" s="339"/>
-      <c r="K133" s="339"/>
-      <c r="L133" s="339"/>
-      <c r="M133" s="339"/>
-      <c r="N133" s="339"/>
+      <c r="B133" s="342"/>
+      <c r="C133" s="342"/>
+      <c r="D133" s="342"/>
+      <c r="E133" s="342"/>
+      <c r="F133" s="342"/>
+      <c r="G133" s="342"/>
+      <c r="H133" s="342"/>
+      <c r="I133" s="342"/>
+      <c r="J133" s="342"/>
+      <c r="K133" s="342"/>
+      <c r="L133" s="342"/>
+      <c r="M133" s="342"/>
+      <c r="N133" s="342"/>
       <c r="O133" s="205"/>
-      <c r="P133" s="339" t="s">
+      <c r="P133" s="342" t="s">
         <v>266</v>
       </c>
-      <c r="Q133" s="339"/>
-      <c r="R133" s="339"/>
-      <c r="S133" s="339"/>
-      <c r="T133" s="339"/>
-      <c r="U133" s="339"/>
-      <c r="V133" s="339"/>
-      <c r="W133" s="339"/>
-      <c r="X133" s="339"/>
-      <c r="Y133" s="339"/>
-      <c r="Z133" s="339"/>
-      <c r="AA133" s="339"/>
-      <c r="AB133" s="339"/>
-      <c r="AC133" s="339"/>
+      <c r="Q133" s="342"/>
+      <c r="R133" s="342"/>
+      <c r="S133" s="342"/>
+      <c r="T133" s="342"/>
+      <c r="U133" s="342"/>
+      <c r="V133" s="342"/>
+      <c r="W133" s="342"/>
+      <c r="X133" s="342"/>
+      <c r="Y133" s="342"/>
+      <c r="Z133" s="342"/>
+      <c r="AA133" s="342"/>
+      <c r="AB133" s="342"/>
+      <c r="AC133" s="342"/>
       <c r="AD133" s="205"/>
-      <c r="AE133" s="339" t="s">
+      <c r="AE133" s="342" t="s">
         <v>267</v>
       </c>
-      <c r="AF133" s="339"/>
-      <c r="AG133" s="339"/>
-      <c r="AH133" s="339"/>
-      <c r="AI133" s="339"/>
-      <c r="AJ133" s="339"/>
-      <c r="AK133" s="339"/>
-      <c r="AL133" s="339"/>
-      <c r="AM133" s="339"/>
-      <c r="AN133" s="339"/>
-      <c r="AO133" s="339"/>
-      <c r="AP133" s="339"/>
-      <c r="AQ133" s="339"/>
-      <c r="AR133" s="339"/>
+      <c r="AF133" s="342"/>
+      <c r="AG133" s="342"/>
+      <c r="AH133" s="342"/>
+      <c r="AI133" s="342"/>
+      <c r="AJ133" s="342"/>
+      <c r="AK133" s="342"/>
+      <c r="AL133" s="342"/>
+      <c r="AM133" s="342"/>
+      <c r="AN133" s="342"/>
+      <c r="AO133" s="342"/>
+      <c r="AP133" s="342"/>
+      <c r="AQ133" s="342"/>
+      <c r="AR133" s="342"/>
       <c r="AS133" s="205"/>
-      <c r="AT133" s="339" t="s">
+      <c r="AT133" s="342" t="s">
         <v>268</v>
       </c>
-      <c r="AU133" s="339"/>
-      <c r="AV133" s="339"/>
-      <c r="AW133" s="339"/>
-      <c r="AX133" s="339"/>
-      <c r="AY133" s="339"/>
-      <c r="AZ133" s="339"/>
-      <c r="BA133" s="339"/>
-      <c r="BB133" s="339"/>
-      <c r="BC133" s="339"/>
-      <c r="BD133" s="339"/>
-      <c r="BE133" s="339"/>
-      <c r="BF133" s="339"/>
-      <c r="BG133" s="339"/>
+      <c r="AU133" s="342"/>
+      <c r="AV133" s="342"/>
+      <c r="AW133" s="342"/>
+      <c r="AX133" s="342"/>
+      <c r="AY133" s="342"/>
+      <c r="AZ133" s="342"/>
+      <c r="BA133" s="342"/>
+      <c r="BB133" s="342"/>
+      <c r="BC133" s="342"/>
+      <c r="BD133" s="342"/>
+      <c r="BE133" s="342"/>
+      <c r="BF133" s="342"/>
+      <c r="BG133" s="342"/>
       <c r="BH133" s="205"/>
-      <c r="BI133" s="339" t="s">
+      <c r="BI133" s="342" t="s">
         <v>269</v>
       </c>
-      <c r="BJ133" s="339"/>
-      <c r="BK133" s="339"/>
-      <c r="BL133" s="339"/>
-      <c r="BM133" s="339"/>
-      <c r="BN133" s="339"/>
-      <c r="BO133" s="339"/>
-      <c r="BP133" s="339"/>
-      <c r="BQ133" s="339"/>
-      <c r="BR133" s="339"/>
-      <c r="BS133" s="339"/>
-      <c r="BT133" s="339"/>
-      <c r="BU133" s="339"/>
-      <c r="BV133" s="339"/>
+      <c r="BJ133" s="342"/>
+      <c r="BK133" s="342"/>
+      <c r="BL133" s="342"/>
+      <c r="BM133" s="342"/>
+      <c r="BN133" s="342"/>
+      <c r="BO133" s="342"/>
+      <c r="BP133" s="342"/>
+      <c r="BQ133" s="342"/>
+      <c r="BR133" s="342"/>
+      <c r="BS133" s="342"/>
+      <c r="BT133" s="342"/>
+      <c r="BU133" s="342"/>
+      <c r="BV133" s="342"/>
       <c r="BW133" s="205"/>
-      <c r="BX133" s="339" t="s">
+      <c r="BX133" s="342" t="s">
         <v>264</v>
       </c>
-      <c r="BY133" s="339"/>
-      <c r="BZ133" s="339"/>
-      <c r="CA133" s="339"/>
-      <c r="CB133" s="339"/>
-      <c r="CC133" s="339"/>
-      <c r="CD133" s="339"/>
-      <c r="CE133" s="339"/>
-      <c r="CF133" s="339"/>
-      <c r="CG133" s="339"/>
-      <c r="CH133" s="339"/>
-      <c r="CI133" s="339"/>
-      <c r="CJ133" s="339"/>
-      <c r="CK133" s="339"/>
+      <c r="BY133" s="342"/>
+      <c r="BZ133" s="342"/>
+      <c r="CA133" s="342"/>
+      <c r="CB133" s="342"/>
+      <c r="CC133" s="342"/>
+      <c r="CD133" s="342"/>
+      <c r="CE133" s="342"/>
+      <c r="CF133" s="342"/>
+      <c r="CG133" s="342"/>
+      <c r="CH133" s="342"/>
+      <c r="CI133" s="342"/>
+      <c r="CJ133" s="342"/>
+      <c r="CK133" s="342"/>
       <c r="CL133" s="205"/>
       <c r="CM133" s="205"/>
       <c r="CN133" s="5" t="s">
@@ -31173,102 +31173,102 @@
       <c r="DS147" s="205"/>
     </row>
     <row r="148" spans="1:123" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="320" t="s">
+      <c r="A148" s="323" t="s">
         <v>276</v>
       </c>
-      <c r="B148" s="320"/>
-      <c r="C148" s="320"/>
-      <c r="D148" s="320"/>
-      <c r="E148" s="320"/>
-      <c r="F148" s="320"/>
-      <c r="G148" s="320"/>
-      <c r="H148" s="320"/>
-      <c r="I148" s="320"/>
-      <c r="J148" s="320"/>
-      <c r="K148" s="320"/>
-      <c r="L148" s="320"/>
-      <c r="M148" s="320"/>
-      <c r="N148" s="320"/>
-      <c r="P148" s="328" t="s">
+      <c r="B148" s="323"/>
+      <c r="C148" s="323"/>
+      <c r="D148" s="323"/>
+      <c r="E148" s="323"/>
+      <c r="F148" s="323"/>
+      <c r="G148" s="323"/>
+      <c r="H148" s="323"/>
+      <c r="I148" s="323"/>
+      <c r="J148" s="323"/>
+      <c r="K148" s="323"/>
+      <c r="L148" s="323"/>
+      <c r="M148" s="323"/>
+      <c r="N148" s="323"/>
+      <c r="P148" s="331" t="s">
         <v>277</v>
       </c>
-      <c r="Q148" s="328"/>
-      <c r="R148" s="328"/>
-      <c r="S148" s="328"/>
-      <c r="T148" s="328"/>
-      <c r="U148" s="328"/>
-      <c r="V148" s="328"/>
-      <c r="W148" s="328"/>
-      <c r="X148" s="328"/>
-      <c r="Y148" s="328"/>
-      <c r="Z148" s="328"/>
-      <c r="AA148" s="328"/>
-      <c r="AB148" s="328"/>
-      <c r="AC148" s="328"/>
-      <c r="AE148" s="320" t="s">
+      <c r="Q148" s="331"/>
+      <c r="R148" s="331"/>
+      <c r="S148" s="331"/>
+      <c r="T148" s="331"/>
+      <c r="U148" s="331"/>
+      <c r="V148" s="331"/>
+      <c r="W148" s="331"/>
+      <c r="X148" s="331"/>
+      <c r="Y148" s="331"/>
+      <c r="Z148" s="331"/>
+      <c r="AA148" s="331"/>
+      <c r="AB148" s="331"/>
+      <c r="AC148" s="331"/>
+      <c r="AE148" s="323" t="s">
         <v>278</v>
       </c>
-      <c r="AF148" s="320"/>
-      <c r="AG148" s="320"/>
-      <c r="AH148" s="320"/>
-      <c r="AI148" s="320"/>
-      <c r="AJ148" s="320"/>
-      <c r="AK148" s="320"/>
-      <c r="AL148" s="320"/>
-      <c r="AM148" s="320"/>
-      <c r="AN148" s="320"/>
-      <c r="AO148" s="320"/>
-      <c r="AP148" s="320"/>
-      <c r="AQ148" s="320"/>
-      <c r="AR148" s="320"/>
-      <c r="AT148" s="320" t="s">
+      <c r="AF148" s="323"/>
+      <c r="AG148" s="323"/>
+      <c r="AH148" s="323"/>
+      <c r="AI148" s="323"/>
+      <c r="AJ148" s="323"/>
+      <c r="AK148" s="323"/>
+      <c r="AL148" s="323"/>
+      <c r="AM148" s="323"/>
+      <c r="AN148" s="323"/>
+      <c r="AO148" s="323"/>
+      <c r="AP148" s="323"/>
+      <c r="AQ148" s="323"/>
+      <c r="AR148" s="323"/>
+      <c r="AT148" s="323" t="s">
         <v>279</v>
       </c>
-      <c r="AU148" s="320"/>
-      <c r="AV148" s="320"/>
-      <c r="AW148" s="320"/>
-      <c r="AX148" s="320"/>
-      <c r="AY148" s="320"/>
-      <c r="AZ148" s="320"/>
-      <c r="BA148" s="320"/>
-      <c r="BB148" s="320"/>
-      <c r="BC148" s="320"/>
-      <c r="BD148" s="320"/>
-      <c r="BE148" s="320"/>
-      <c r="BF148" s="320"/>
-      <c r="BG148" s="320"/>
-      <c r="BI148" s="320" t="s">
+      <c r="AU148" s="323"/>
+      <c r="AV148" s="323"/>
+      <c r="AW148" s="323"/>
+      <c r="AX148" s="323"/>
+      <c r="AY148" s="323"/>
+      <c r="AZ148" s="323"/>
+      <c r="BA148" s="323"/>
+      <c r="BB148" s="323"/>
+      <c r="BC148" s="323"/>
+      <c r="BD148" s="323"/>
+      <c r="BE148" s="323"/>
+      <c r="BF148" s="323"/>
+      <c r="BG148" s="323"/>
+      <c r="BI148" s="323" t="s">
         <v>280</v>
       </c>
-      <c r="BJ148" s="320"/>
-      <c r="BK148" s="320"/>
-      <c r="BL148" s="320"/>
-      <c r="BM148" s="320"/>
-      <c r="BN148" s="320"/>
-      <c r="BO148" s="320"/>
-      <c r="BP148" s="320"/>
-      <c r="BQ148" s="320"/>
-      <c r="BR148" s="320"/>
-      <c r="BS148" s="320"/>
-      <c r="BT148" s="320"/>
-      <c r="BU148" s="320"/>
-      <c r="BV148" s="320"/>
-      <c r="BX148" s="320" t="s">
+      <c r="BJ148" s="323"/>
+      <c r="BK148" s="323"/>
+      <c r="BL148" s="323"/>
+      <c r="BM148" s="323"/>
+      <c r="BN148" s="323"/>
+      <c r="BO148" s="323"/>
+      <c r="BP148" s="323"/>
+      <c r="BQ148" s="323"/>
+      <c r="BR148" s="323"/>
+      <c r="BS148" s="323"/>
+      <c r="BT148" s="323"/>
+      <c r="BU148" s="323"/>
+      <c r="BV148" s="323"/>
+      <c r="BX148" s="323" t="s">
         <v>281</v>
       </c>
-      <c r="BY148" s="320"/>
-      <c r="BZ148" s="320"/>
-      <c r="CA148" s="320"/>
-      <c r="CB148" s="320"/>
-      <c r="CC148" s="320"/>
-      <c r="CD148" s="320"/>
-      <c r="CE148" s="320"/>
-      <c r="CF148" s="320"/>
-      <c r="CG148" s="320"/>
-      <c r="CH148" s="320"/>
-      <c r="CI148" s="320"/>
-      <c r="CJ148" s="320"/>
-      <c r="CK148" s="320"/>
+      <c r="BY148" s="323"/>
+      <c r="BZ148" s="323"/>
+      <c r="CA148" s="323"/>
+      <c r="CB148" s="323"/>
+      <c r="CC148" s="323"/>
+      <c r="CD148" s="323"/>
+      <c r="CE148" s="323"/>
+      <c r="CF148" s="323"/>
+      <c r="CG148" s="323"/>
+      <c r="CH148" s="323"/>
+      <c r="CI148" s="323"/>
+      <c r="CJ148" s="323"/>
+      <c r="CK148" s="323"/>
       <c r="CL148" s="205"/>
       <c r="CM148" s="205"/>
       <c r="CN148" s="205"/>
@@ -35325,71 +35325,71 @@
       <c r="DS162" s="205"/>
     </row>
     <row r="163" spans="1:123" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="328" t="s">
+      <c r="A163" s="331" t="s">
         <v>198</v>
       </c>
-      <c r="B163" s="328"/>
-      <c r="C163" s="328"/>
-      <c r="D163" s="328"/>
-      <c r="E163" s="328"/>
-      <c r="F163" s="328"/>
-      <c r="G163" s="328"/>
-      <c r="H163" s="328"/>
-      <c r="I163" s="328"/>
-      <c r="J163" s="328"/>
-      <c r="K163" s="328"/>
-      <c r="L163" s="328"/>
-      <c r="M163" s="328"/>
-      <c r="N163" s="328"/>
-      <c r="P163" s="347" t="s">
+      <c r="B163" s="331"/>
+      <c r="C163" s="331"/>
+      <c r="D163" s="331"/>
+      <c r="E163" s="331"/>
+      <c r="F163" s="331"/>
+      <c r="G163" s="331"/>
+      <c r="H163" s="331"/>
+      <c r="I163" s="331"/>
+      <c r="J163" s="331"/>
+      <c r="K163" s="331"/>
+      <c r="L163" s="331"/>
+      <c r="M163" s="331"/>
+      <c r="N163" s="331"/>
+      <c r="P163" s="350" t="s">
         <v>236</v>
       </c>
-      <c r="Q163" s="347"/>
-      <c r="R163" s="347"/>
-      <c r="S163" s="347"/>
-      <c r="T163" s="347"/>
-      <c r="U163" s="347"/>
-      <c r="V163" s="347"/>
-      <c r="W163" s="347"/>
-      <c r="X163" s="347"/>
-      <c r="Y163" s="347"/>
-      <c r="Z163" s="347"/>
-      <c r="AA163" s="347"/>
-      <c r="AB163" s="347"/>
-      <c r="AC163" s="347"/>
+      <c r="Q163" s="350"/>
+      <c r="R163" s="350"/>
+      <c r="S163" s="350"/>
+      <c r="T163" s="350"/>
+      <c r="U163" s="350"/>
+      <c r="V163" s="350"/>
+      <c r="W163" s="350"/>
+      <c r="X163" s="350"/>
+      <c r="Y163" s="350"/>
+      <c r="Z163" s="350"/>
+      <c r="AA163" s="350"/>
+      <c r="AB163" s="350"/>
+      <c r="AC163" s="350"/>
       <c r="AD163"/>
-      <c r="AE163" s="347" t="s">
+      <c r="AE163" s="350" t="s">
         <v>237</v>
       </c>
-      <c r="AF163" s="347"/>
-      <c r="AG163" s="347"/>
-      <c r="AH163" s="347"/>
-      <c r="AI163" s="347"/>
-      <c r="AJ163" s="347"/>
-      <c r="AK163" s="347"/>
-      <c r="AL163" s="347"/>
-      <c r="AM163" s="347"/>
-      <c r="AN163" s="347"/>
-      <c r="AO163" s="347"/>
-      <c r="AP163" s="347"/>
-      <c r="AQ163" s="347"/>
-      <c r="AR163" s="347"/>
-      <c r="AT163" s="347" t="s">
+      <c r="AF163" s="350"/>
+      <c r="AG163" s="350"/>
+      <c r="AH163" s="350"/>
+      <c r="AI163" s="350"/>
+      <c r="AJ163" s="350"/>
+      <c r="AK163" s="350"/>
+      <c r="AL163" s="350"/>
+      <c r="AM163" s="350"/>
+      <c r="AN163" s="350"/>
+      <c r="AO163" s="350"/>
+      <c r="AP163" s="350"/>
+      <c r="AQ163" s="350"/>
+      <c r="AR163" s="350"/>
+      <c r="AT163" s="350" t="s">
         <v>238</v>
       </c>
-      <c r="AU163" s="347"/>
-      <c r="AV163" s="347"/>
-      <c r="AW163" s="347"/>
-      <c r="AX163" s="347"/>
-      <c r="AY163" s="347"/>
-      <c r="AZ163" s="347"/>
-      <c r="BA163" s="347"/>
-      <c r="BB163" s="347"/>
-      <c r="BC163" s="347"/>
-      <c r="BD163" s="347"/>
-      <c r="BE163" s="347"/>
-      <c r="BF163" s="347"/>
-      <c r="BG163" s="347"/>
+      <c r="AU163" s="350"/>
+      <c r="AV163" s="350"/>
+      <c r="AW163" s="350"/>
+      <c r="AX163" s="350"/>
+      <c r="AY163" s="350"/>
+      <c r="AZ163" s="350"/>
+      <c r="BA163" s="350"/>
+      <c r="BB163" s="350"/>
+      <c r="BC163" s="350"/>
+      <c r="BD163" s="350"/>
+      <c r="BE163" s="350"/>
+      <c r="BF163" s="350"/>
+      <c r="BG163" s="350"/>
     </row>
     <row r="164" spans="1:123" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1"/>
@@ -37783,191 +37783,191 @@
       </c>
     </row>
     <row r="178" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="335" t="s">
+      <c r="A178" s="338" t="s">
         <v>199</v>
       </c>
-      <c r="B178" s="335"/>
-      <c r="C178" s="335"/>
-      <c r="D178" s="340" t="s">
+      <c r="B178" s="338"/>
+      <c r="C178" s="338"/>
+      <c r="D178" s="343" t="s">
         <v>193</v>
       </c>
-      <c r="E178" s="340"/>
-      <c r="F178" s="340"/>
-      <c r="G178" s="341" t="s">
+      <c r="E178" s="343"/>
+      <c r="F178" s="343"/>
+      <c r="G178" s="344" t="s">
         <v>194</v>
       </c>
-      <c r="H178" s="341"/>
-      <c r="I178" s="341"/>
-      <c r="J178" s="336" t="s">
+      <c r="H178" s="344"/>
+      <c r="I178" s="344"/>
+      <c r="J178" s="339" t="s">
         <v>195</v>
       </c>
-      <c r="K178" s="336"/>
-      <c r="L178" s="336"/>
-      <c r="M178" s="337" t="s">
+      <c r="K178" s="339"/>
+      <c r="L178" s="339"/>
+      <c r="M178" s="340" t="s">
         <v>196</v>
       </c>
-      <c r="N178" s="337"/>
-      <c r="O178" s="337"/>
-      <c r="P178" s="333" t="s">
+      <c r="N178" s="340"/>
+      <c r="O178" s="340"/>
+      <c r="P178" s="336" t="s">
         <v>187</v>
       </c>
-      <c r="Q178" s="333"/>
-      <c r="R178" s="333"/>
-      <c r="S178" s="334" t="s">
+      <c r="Q178" s="336"/>
+      <c r="R178" s="336"/>
+      <c r="S178" s="337" t="s">
         <v>188</v>
       </c>
-      <c r="T178" s="334"/>
-      <c r="U178" s="334"/>
-      <c r="V178" s="332" t="s">
+      <c r="T178" s="337"/>
+      <c r="U178" s="337"/>
+      <c r="V178" s="335" t="s">
         <v>189</v>
       </c>
-      <c r="W178" s="332"/>
-      <c r="X178" s="332"/>
-      <c r="Y178" s="330" t="s">
+      <c r="W178" s="335"/>
+      <c r="X178" s="335"/>
+      <c r="Y178" s="333" t="s">
         <v>190</v>
       </c>
-      <c r="Z178" s="330"/>
-      <c r="AA178" s="330"/>
-      <c r="AB178" s="331" t="s">
+      <c r="Z178" s="333"/>
+      <c r="AA178" s="333"/>
+      <c r="AB178" s="334" t="s">
         <v>191</v>
       </c>
-      <c r="AC178" s="331"/>
-      <c r="AD178" s="331"/>
-      <c r="AE178" s="333" t="s">
+      <c r="AC178" s="334"/>
+      <c r="AD178" s="334"/>
+      <c r="AE178" s="336" t="s">
         <v>187</v>
       </c>
-      <c r="AF178" s="333"/>
-      <c r="AG178" s="333"/>
-      <c r="AH178" s="334" t="s">
+      <c r="AF178" s="336"/>
+      <c r="AG178" s="336"/>
+      <c r="AH178" s="337" t="s">
         <v>188</v>
       </c>
-      <c r="AI178" s="334"/>
-      <c r="AJ178" s="334"/>
-      <c r="AK178" s="332" t="s">
+      <c r="AI178" s="337"/>
+      <c r="AJ178" s="337"/>
+      <c r="AK178" s="335" t="s">
         <v>189</v>
       </c>
-      <c r="AL178" s="332"/>
-      <c r="AM178" s="332"/>
-      <c r="AN178" s="330" t="s">
+      <c r="AL178" s="335"/>
+      <c r="AM178" s="335"/>
+      <c r="AN178" s="333" t="s">
         <v>190</v>
       </c>
-      <c r="AO178" s="330"/>
-      <c r="AP178" s="330"/>
-      <c r="AQ178" s="331" t="s">
+      <c r="AO178" s="333"/>
+      <c r="AP178" s="333"/>
+      <c r="AQ178" s="334" t="s">
         <v>191</v>
       </c>
-      <c r="AR178" s="331"/>
-      <c r="AS178" s="331"/>
-      <c r="AT178" s="333" t="s">
+      <c r="AR178" s="334"/>
+      <c r="AS178" s="334"/>
+      <c r="AT178" s="336" t="s">
         <v>187</v>
       </c>
-      <c r="AU178" s="333"/>
-      <c r="AV178" s="333"/>
-      <c r="AW178" s="334" t="s">
+      <c r="AU178" s="336"/>
+      <c r="AV178" s="336"/>
+      <c r="AW178" s="337" t="s">
         <v>188</v>
       </c>
-      <c r="AX178" s="334"/>
-      <c r="AY178" s="334"/>
-      <c r="AZ178" s="332" t="s">
+      <c r="AX178" s="337"/>
+      <c r="AY178" s="337"/>
+      <c r="AZ178" s="335" t="s">
         <v>189</v>
       </c>
-      <c r="BA178" s="332"/>
-      <c r="BB178" s="332"/>
-      <c r="BC178" s="330" t="s">
+      <c r="BA178" s="335"/>
+      <c r="BB178" s="335"/>
+      <c r="BC178" s="333" t="s">
         <v>190</v>
       </c>
-      <c r="BD178" s="330"/>
-      <c r="BE178" s="330"/>
-      <c r="BF178" s="331" t="s">
+      <c r="BD178" s="333"/>
+      <c r="BE178" s="333"/>
+      <c r="BF178" s="334" t="s">
         <v>191</v>
       </c>
-      <c r="BG178" s="331"/>
-      <c r="BH178" s="331"/>
+      <c r="BG178" s="334"/>
+      <c r="BH178" s="334"/>
     </row>
     <row r="179" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="343" t="s">
+      <c r="A179" s="346" t="s">
         <v>284</v>
       </c>
-      <c r="B179" s="343"/>
-      <c r="C179" s="343"/>
-      <c r="D179" s="343"/>
-      <c r="E179" s="343"/>
-      <c r="F179" s="343"/>
-      <c r="G179" s="343"/>
-      <c r="H179" s="343"/>
-      <c r="I179" s="343"/>
-      <c r="J179" s="343"/>
-      <c r="K179" s="343"/>
-      <c r="L179" s="343"/>
-      <c r="M179" s="343"/>
-      <c r="N179" s="343"/>
+      <c r="B179" s="346"/>
+      <c r="C179" s="346"/>
+      <c r="D179" s="346"/>
+      <c r="E179" s="346"/>
+      <c r="F179" s="346"/>
+      <c r="G179" s="346"/>
+      <c r="H179" s="346"/>
+      <c r="I179" s="346"/>
+      <c r="J179" s="346"/>
+      <c r="K179" s="346"/>
+      <c r="L179" s="346"/>
+      <c r="M179" s="346"/>
+      <c r="N179" s="346"/>
       <c r="O179"/>
-      <c r="P179" s="323" t="s">
+      <c r="P179" s="326" t="s">
         <v>283</v>
       </c>
-      <c r="Q179" s="323"/>
-      <c r="R179" s="323"/>
-      <c r="S179" s="323"/>
-      <c r="T179" s="323"/>
-      <c r="U179" s="323"/>
-      <c r="V179" s="323"/>
-      <c r="W179" s="323"/>
-      <c r="X179" s="323"/>
-      <c r="Y179" s="323"/>
-      <c r="Z179" s="323"/>
-      <c r="AA179" s="323"/>
-      <c r="AB179" s="323"/>
-      <c r="AC179" s="323"/>
-      <c r="AE179" s="323" t="s">
+      <c r="Q179" s="326"/>
+      <c r="R179" s="326"/>
+      <c r="S179" s="326"/>
+      <c r="T179" s="326"/>
+      <c r="U179" s="326"/>
+      <c r="V179" s="326"/>
+      <c r="W179" s="326"/>
+      <c r="X179" s="326"/>
+      <c r="Y179" s="326"/>
+      <c r="Z179" s="326"/>
+      <c r="AA179" s="326"/>
+      <c r="AB179" s="326"/>
+      <c r="AC179" s="326"/>
+      <c r="AE179" s="326" t="s">
         <v>285</v>
       </c>
-      <c r="AF179" s="323"/>
-      <c r="AG179" s="323"/>
-      <c r="AH179" s="323"/>
-      <c r="AI179" s="323"/>
-      <c r="AJ179" s="323"/>
-      <c r="AK179" s="323"/>
-      <c r="AL179" s="323"/>
-      <c r="AM179" s="323"/>
-      <c r="AN179" s="323"/>
-      <c r="AO179" s="323"/>
-      <c r="AP179" s="323"/>
-      <c r="AQ179" s="323"/>
-      <c r="AR179" s="323"/>
+      <c r="AF179" s="326"/>
+      <c r="AG179" s="326"/>
+      <c r="AH179" s="326"/>
+      <c r="AI179" s="326"/>
+      <c r="AJ179" s="326"/>
+      <c r="AK179" s="326"/>
+      <c r="AL179" s="326"/>
+      <c r="AM179" s="326"/>
+      <c r="AN179" s="326"/>
+      <c r="AO179" s="326"/>
+      <c r="AP179" s="326"/>
+      <c r="AQ179" s="326"/>
+      <c r="AR179" s="326"/>
       <c r="AS179"/>
-      <c r="AT179" s="323" t="s">
+      <c r="AT179" s="326" t="s">
         <v>263</v>
       </c>
-      <c r="AU179" s="323"/>
-      <c r="AV179" s="323"/>
-      <c r="AW179" s="323"/>
-      <c r="AX179" s="323"/>
-      <c r="AY179" s="323"/>
-      <c r="AZ179" s="323"/>
-      <c r="BA179" s="323"/>
-      <c r="BB179" s="323"/>
-      <c r="BC179" s="323"/>
-      <c r="BD179" s="323"/>
-      <c r="BE179" s="323"/>
-      <c r="BF179" s="323"/>
-      <c r="BG179" s="323"/>
+      <c r="AU179" s="326"/>
+      <c r="AV179" s="326"/>
+      <c r="AW179" s="326"/>
+      <c r="AX179" s="326"/>
+      <c r="AY179" s="326"/>
+      <c r="AZ179" s="326"/>
+      <c r="BA179" s="326"/>
+      <c r="BB179" s="326"/>
+      <c r="BC179" s="326"/>
+      <c r="BD179" s="326"/>
+      <c r="BE179" s="326"/>
+      <c r="BF179" s="326"/>
+      <c r="BG179" s="326"/>
       <c r="BH179"/>
-      <c r="BI179" s="323" t="s">
+      <c r="BI179" s="326" t="s">
         <v>286</v>
       </c>
-      <c r="BJ179" s="323"/>
-      <c r="BK179" s="323"/>
-      <c r="BL179" s="323"/>
-      <c r="BM179" s="323"/>
-      <c r="BN179" s="323"/>
-      <c r="BO179" s="323"/>
-      <c r="BP179" s="323"/>
-      <c r="BQ179" s="323"/>
-      <c r="BR179" s="323"/>
-      <c r="BS179" s="323"/>
-      <c r="BT179" s="323"/>
-      <c r="BU179" s="323"/>
-      <c r="BV179" s="323"/>
+      <c r="BJ179" s="326"/>
+      <c r="BK179" s="326"/>
+      <c r="BL179" s="326"/>
+      <c r="BM179" s="326"/>
+      <c r="BN179" s="326"/>
+      <c r="BO179" s="326"/>
+      <c r="BP179" s="326"/>
+      <c r="BQ179" s="326"/>
+      <c r="BR179" s="326"/>
+      <c r="BS179" s="326"/>
+      <c r="BT179" s="326"/>
+      <c r="BU179" s="326"/>
+      <c r="BV179" s="326"/>
     </row>
     <row r="180" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="1"/>
@@ -41045,22 +41045,22 @@
       <c r="BV194" s="218"/>
     </row>
     <row r="195" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="343" t="s">
+      <c r="A195" s="346" t="s">
         <v>374</v>
       </c>
-      <c r="B195" s="343"/>
-      <c r="C195" s="343"/>
-      <c r="D195" s="343"/>
-      <c r="E195" s="343"/>
-      <c r="F195" s="343"/>
-      <c r="G195" s="343"/>
-      <c r="H195" s="343"/>
-      <c r="I195" s="343"/>
-      <c r="J195" s="343"/>
-      <c r="K195" s="343"/>
-      <c r="L195" s="343"/>
-      <c r="M195" s="343"/>
-      <c r="N195" s="343"/>
+      <c r="B195" s="346"/>
+      <c r="C195" s="346"/>
+      <c r="D195" s="346"/>
+      <c r="E195" s="346"/>
+      <c r="F195" s="346"/>
+      <c r="G195" s="346"/>
+      <c r="H195" s="346"/>
+      <c r="I195" s="346"/>
+      <c r="J195" s="346"/>
+      <c r="K195" s="346"/>
+      <c r="L195" s="346"/>
+      <c r="M195" s="346"/>
+      <c r="N195" s="346"/>
       <c r="O195"/>
       <c r="P195" s="307"/>
       <c r="Q195" s="217"/>
@@ -41359,7 +41359,7 @@
       <c r="K198" s="298" t="s">
         <v>31</v>
       </c>
-      <c r="L198" s="349" t="s">
+      <c r="L198" s="320" t="s">
         <v>32</v>
       </c>
       <c r="M198" s="86" t="s">
@@ -41762,7 +41762,7 @@
       <c r="H202" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="I202" s="350" t="s">
+      <c r="I202" s="321" t="s">
         <v>67</v>
       </c>
       <c r="J202" s="69" t="s">
@@ -42183,7 +42183,7 @@
       <c r="K206" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="L206" s="349">
+      <c r="L206" s="320">
         <v>54</v>
       </c>
       <c r="M206" s="86">
@@ -42498,7 +42498,7 @@
       <c r="M209" s="16">
         <v>32</v>
       </c>
-      <c r="N209" s="351">
+      <c r="N209" s="322">
         <v>22</v>
       </c>
       <c r="O209" s="205"/>
@@ -44018,31 +44018,31 @@
       <c r="BW223" s="205"/>
     </row>
     <row r="224" spans="1:75" ht="14.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A224" s="335" t="s">
+      <c r="A224" s="338" t="s">
         <v>199</v>
       </c>
-      <c r="B224" s="335"/>
-      <c r="C224" s="335"/>
-      <c r="D224" s="340" t="s">
+      <c r="B224" s="338"/>
+      <c r="C224" s="338"/>
+      <c r="D224" s="343" t="s">
         <v>193</v>
       </c>
-      <c r="E224" s="340"/>
-      <c r="F224" s="340"/>
-      <c r="G224" s="341" t="s">
+      <c r="E224" s="343"/>
+      <c r="F224" s="343"/>
+      <c r="G224" s="344" t="s">
         <v>194</v>
       </c>
-      <c r="H224" s="341"/>
-      <c r="I224" s="341"/>
-      <c r="J224" s="336" t="s">
+      <c r="H224" s="344"/>
+      <c r="I224" s="344"/>
+      <c r="J224" s="339" t="s">
         <v>195</v>
       </c>
-      <c r="K224" s="336"/>
-      <c r="L224" s="336"/>
-      <c r="M224" s="337" t="s">
+      <c r="K224" s="339"/>
+      <c r="L224" s="339"/>
+      <c r="M224" s="340" t="s">
         <v>196</v>
       </c>
-      <c r="N224" s="337"/>
-      <c r="O224" s="337"/>
+      <c r="N224" s="340"/>
+      <c r="O224" s="340"/>
       <c r="P224" s="205"/>
       <c r="Q224" s="205"/>
       <c r="R224" s="205"/>
@@ -44105,38 +44105,38 @@
       <c r="BW224" s="205"/>
     </row>
     <row r="225" spans="1:44" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="320" t="s">
+      <c r="A225" s="323" t="s">
         <v>165</v>
       </c>
-      <c r="B225" s="320"/>
-      <c r="C225" s="320"/>
-      <c r="D225" s="320"/>
-      <c r="E225" s="320"/>
-      <c r="F225" s="320"/>
-      <c r="G225" s="320"/>
-      <c r="H225" s="320"/>
-      <c r="I225" s="320"/>
-      <c r="J225" s="320"/>
-      <c r="K225" s="320"/>
-      <c r="L225" s="320"/>
-      <c r="M225" s="320"/>
-      <c r="N225" s="320"/>
-      <c r="P225" s="320" t="s">
+      <c r="B225" s="323"/>
+      <c r="C225" s="323"/>
+      <c r="D225" s="323"/>
+      <c r="E225" s="323"/>
+      <c r="F225" s="323"/>
+      <c r="G225" s="323"/>
+      <c r="H225" s="323"/>
+      <c r="I225" s="323"/>
+      <c r="J225" s="323"/>
+      <c r="K225" s="323"/>
+      <c r="L225" s="323"/>
+      <c r="M225" s="323"/>
+      <c r="N225" s="323"/>
+      <c r="P225" s="323" t="s">
         <v>197</v>
       </c>
-      <c r="Q225" s="320"/>
-      <c r="R225" s="320"/>
-      <c r="S225" s="320"/>
-      <c r="T225" s="320"/>
-      <c r="U225" s="320"/>
-      <c r="V225" s="320"/>
-      <c r="W225" s="320"/>
-      <c r="X225" s="320"/>
-      <c r="Y225" s="320"/>
-      <c r="Z225" s="320"/>
-      <c r="AA225" s="320"/>
-      <c r="AB225" s="320"/>
-      <c r="AC225" s="320"/>
+      <c r="Q225" s="323"/>
+      <c r="R225" s="323"/>
+      <c r="S225" s="323"/>
+      <c r="T225" s="323"/>
+      <c r="U225" s="323"/>
+      <c r="V225" s="323"/>
+      <c r="W225" s="323"/>
+      <c r="X225" s="323"/>
+      <c r="Y225" s="323"/>
+      <c r="Z225" s="323"/>
+      <c r="AA225" s="323"/>
+      <c r="AB225" s="323"/>
+      <c r="AC225" s="323"/>
     </row>
     <row r="226" spans="1:44" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="1"/>
@@ -45337,133 +45337,133 @@
       <c r="AC239" s="145">
         <v>22</v>
       </c>
-      <c r="AD239" s="335" t="s">
+      <c r="AD239" s="338" t="s">
         <v>192</v>
       </c>
-      <c r="AE239" s="335"/>
-      <c r="AF239" s="335"/>
-      <c r="AG239" s="340" t="s">
+      <c r="AE239" s="338"/>
+      <c r="AF239" s="338"/>
+      <c r="AG239" s="343" t="s">
         <v>193</v>
       </c>
-      <c r="AH239" s="340"/>
-      <c r="AI239" s="340"/>
-      <c r="AJ239" s="341" t="s">
+      <c r="AH239" s="343"/>
+      <c r="AI239" s="343"/>
+      <c r="AJ239" s="344" t="s">
         <v>194</v>
       </c>
-      <c r="AK239" s="341"/>
-      <c r="AL239" s="341"/>
-      <c r="AM239" s="336" t="s">
+      <c r="AK239" s="344"/>
+      <c r="AL239" s="344"/>
+      <c r="AM239" s="339" t="s">
         <v>195</v>
       </c>
-      <c r="AN239" s="336"/>
-      <c r="AO239" s="336"/>
-      <c r="AP239" s="337" t="s">
+      <c r="AN239" s="339"/>
+      <c r="AO239" s="339"/>
+      <c r="AP239" s="340" t="s">
         <v>196</v>
       </c>
-      <c r="AQ239" s="337"/>
-      <c r="AR239" s="337"/>
+      <c r="AQ239" s="340"/>
+      <c r="AR239" s="340"/>
     </row>
     <row r="240" spans="1:44" ht="20.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A240" s="327" t="s">
+      <c r="A240" s="330" t="s">
         <v>166</v>
       </c>
-      <c r="B240" s="327"/>
-      <c r="C240" s="327"/>
-      <c r="D240" s="327"/>
-      <c r="E240" s="327"/>
-      <c r="F240" s="327"/>
-      <c r="G240" s="327"/>
-      <c r="H240" s="327"/>
-      <c r="I240" s="327"/>
-      <c r="J240" s="327"/>
-      <c r="K240" s="327"/>
-      <c r="L240" s="327"/>
-      <c r="M240" s="327"/>
-      <c r="N240" s="327"/>
-      <c r="O240" s="327"/>
-      <c r="P240" s="327"/>
-      <c r="Q240" s="327"/>
-      <c r="R240" s="327"/>
-      <c r="S240" s="327"/>
-      <c r="T240" s="327"/>
-      <c r="U240" s="327"/>
-      <c r="V240" s="327"/>
-      <c r="W240" s="327"/>
-      <c r="X240" s="327"/>
-      <c r="Y240" s="327"/>
-      <c r="Z240" s="327"/>
-      <c r="AA240" s="327"/>
-      <c r="AB240" s="327"/>
-      <c r="AC240" s="327"/>
-      <c r="AD240" s="327"/>
+      <c r="B240" s="330"/>
+      <c r="C240" s="330"/>
+      <c r="D240" s="330"/>
+      <c r="E240" s="330"/>
+      <c r="F240" s="330"/>
+      <c r="G240" s="330"/>
+      <c r="H240" s="330"/>
+      <c r="I240" s="330"/>
+      <c r="J240" s="330"/>
+      <c r="K240" s="330"/>
+      <c r="L240" s="330"/>
+      <c r="M240" s="330"/>
+      <c r="N240" s="330"/>
+      <c r="O240" s="330"/>
+      <c r="P240" s="330"/>
+      <c r="Q240" s="330"/>
+      <c r="R240" s="330"/>
+      <c r="S240" s="330"/>
+      <c r="T240" s="330"/>
+      <c r="U240" s="330"/>
+      <c r="V240" s="330"/>
+      <c r="W240" s="330"/>
+      <c r="X240" s="330"/>
+      <c r="Y240" s="330"/>
+      <c r="Z240" s="330"/>
+      <c r="AA240" s="330"/>
+      <c r="AB240" s="330"/>
+      <c r="AC240" s="330"/>
+      <c r="AD240" s="330"/>
     </row>
     <row r="241" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A241" s="323" t="s">
+      <c r="A241" s="326" t="s">
         <v>167</v>
       </c>
-      <c r="B241" s="323"/>
-      <c r="C241" s="323"/>
-      <c r="D241" s="323"/>
-      <c r="E241" s="323"/>
-      <c r="F241" s="323"/>
-      <c r="G241" s="323"/>
-      <c r="H241" s="323"/>
-      <c r="I241" s="323"/>
-      <c r="J241" s="323"/>
-      <c r="K241" s="323"/>
-      <c r="L241" s="323"/>
-      <c r="M241" s="323"/>
-      <c r="N241" s="323"/>
+      <c r="B241" s="326"/>
+      <c r="C241" s="326"/>
+      <c r="D241" s="326"/>
+      <c r="E241" s="326"/>
+      <c r="F241" s="326"/>
+      <c r="G241" s="326"/>
+      <c r="H241" s="326"/>
+      <c r="I241" s="326"/>
+      <c r="J241" s="326"/>
+      <c r="K241" s="326"/>
+      <c r="L241" s="326"/>
+      <c r="M241" s="326"/>
+      <c r="N241" s="326"/>
       <c r="O241"/>
-      <c r="P241" s="323" t="s">
+      <c r="P241" s="326" t="s">
         <v>168</v>
       </c>
-      <c r="Q241" s="323"/>
-      <c r="R241" s="323"/>
-      <c r="S241" s="323"/>
-      <c r="T241" s="323"/>
-      <c r="U241" s="323"/>
-      <c r="V241" s="323"/>
-      <c r="W241" s="323"/>
-      <c r="X241" s="323"/>
-      <c r="Y241" s="323"/>
-      <c r="Z241" s="323"/>
-      <c r="AA241" s="323"/>
-      <c r="AB241" s="323"/>
-      <c r="AC241" s="323"/>
-      <c r="AE241" s="324" t="s">
+      <c r="Q241" s="326"/>
+      <c r="R241" s="326"/>
+      <c r="S241" s="326"/>
+      <c r="T241" s="326"/>
+      <c r="U241" s="326"/>
+      <c r="V241" s="326"/>
+      <c r="W241" s="326"/>
+      <c r="X241" s="326"/>
+      <c r="Y241" s="326"/>
+      <c r="Z241" s="326"/>
+      <c r="AA241" s="326"/>
+      <c r="AB241" s="326"/>
+      <c r="AC241" s="326"/>
+      <c r="AE241" s="327" t="s">
         <v>169</v>
       </c>
-      <c r="AF241" s="324"/>
-      <c r="AG241" s="324"/>
-      <c r="AH241" s="324"/>
-      <c r="AI241" s="324"/>
-      <c r="AJ241" s="324"/>
-      <c r="AK241" s="324"/>
-      <c r="AL241" s="324"/>
-      <c r="AM241" s="324"/>
-      <c r="AN241" s="324"/>
-      <c r="AO241" s="324"/>
-      <c r="AP241" s="324"/>
-      <c r="AQ241" s="324"/>
-      <c r="AR241" s="324"/>
+      <c r="AF241" s="327"/>
+      <c r="AG241" s="327"/>
+      <c r="AH241" s="327"/>
+      <c r="AI241" s="327"/>
+      <c r="AJ241" s="327"/>
+      <c r="AK241" s="327"/>
+      <c r="AL241" s="327"/>
+      <c r="AM241" s="327"/>
+      <c r="AN241" s="327"/>
+      <c r="AO241" s="327"/>
+      <c r="AP241" s="327"/>
+      <c r="AQ241" s="327"/>
+      <c r="AR241" s="327"/>
       <c r="AS241"/>
-      <c r="AT241" s="329" t="s">
+      <c r="AT241" s="332" t="s">
         <v>170</v>
       </c>
-      <c r="AU241" s="329"/>
-      <c r="AV241" s="329"/>
-      <c r="AW241" s="329"/>
-      <c r="AX241" s="329"/>
-      <c r="AY241" s="329"/>
-      <c r="AZ241" s="329"/>
-      <c r="BA241" s="329"/>
-      <c r="BB241" s="329"/>
-      <c r="BC241" s="329"/>
-      <c r="BD241" s="329"/>
-      <c r="BE241" s="329"/>
-      <c r="BF241" s="329"/>
-      <c r="BG241" s="329"/>
+      <c r="AU241" s="332"/>
+      <c r="AV241" s="332"/>
+      <c r="AW241" s="332"/>
+      <c r="AX241" s="332"/>
+      <c r="AY241" s="332"/>
+      <c r="AZ241" s="332"/>
+      <c r="BA241" s="332"/>
+      <c r="BB241" s="332"/>
+      <c r="BC241" s="332"/>
+      <c r="BD241" s="332"/>
+      <c r="BE241" s="332"/>
+      <c r="BF241" s="332"/>
+      <c r="BG241" s="332"/>
     </row>
     <row r="242" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="1"/>
@@ -47870,90 +47870,90 @@
       </c>
     </row>
     <row r="256" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A256" s="321" t="s">
+      <c r="A256" s="324" t="s">
         <v>171</v>
       </c>
-      <c r="B256" s="321"/>
-      <c r="C256" s="321"/>
-      <c r="D256" s="321"/>
-      <c r="E256" s="321"/>
-      <c r="F256" s="321"/>
-      <c r="G256" s="321"/>
-      <c r="H256" s="321"/>
-      <c r="I256" s="321"/>
-      <c r="J256" s="321"/>
-      <c r="K256" s="321"/>
-      <c r="L256" s="321"/>
-      <c r="M256" s="321"/>
-      <c r="N256" s="321"/>
+      <c r="B256" s="324"/>
+      <c r="C256" s="324"/>
+      <c r="D256" s="324"/>
+      <c r="E256" s="324"/>
+      <c r="F256" s="324"/>
+      <c r="G256" s="324"/>
+      <c r="H256" s="324"/>
+      <c r="I256" s="324"/>
+      <c r="J256" s="324"/>
+      <c r="K256" s="324"/>
+      <c r="L256" s="324"/>
+      <c r="M256" s="324"/>
+      <c r="N256" s="324"/>
       <c r="O256" s="119"/>
-      <c r="P256" s="329" t="s">
+      <c r="P256" s="332" t="s">
         <v>172</v>
       </c>
-      <c r="Q256" s="329"/>
-      <c r="R256" s="329"/>
-      <c r="S256" s="329"/>
-      <c r="T256" s="329"/>
-      <c r="U256" s="329"/>
-      <c r="V256" s="329"/>
-      <c r="W256" s="329"/>
-      <c r="X256" s="329"/>
-      <c r="Y256" s="329"/>
-      <c r="Z256" s="329"/>
-      <c r="AA256" s="329"/>
-      <c r="AB256" s="329"/>
-      <c r="AC256" s="329"/>
+      <c r="Q256" s="332"/>
+      <c r="R256" s="332"/>
+      <c r="S256" s="332"/>
+      <c r="T256" s="332"/>
+      <c r="U256" s="332"/>
+      <c r="V256" s="332"/>
+      <c r="W256" s="332"/>
+      <c r="X256" s="332"/>
+      <c r="Y256" s="332"/>
+      <c r="Z256" s="332"/>
+      <c r="AA256" s="332"/>
+      <c r="AB256" s="332"/>
+      <c r="AC256" s="332"/>
       <c r="AD256" s="120"/>
-      <c r="AE256" s="329" t="s">
+      <c r="AE256" s="332" t="s">
         <v>173</v>
       </c>
-      <c r="AF256" s="329"/>
-      <c r="AG256" s="329"/>
-      <c r="AH256" s="329"/>
-      <c r="AI256" s="329"/>
-      <c r="AJ256" s="329"/>
-      <c r="AK256" s="329"/>
-      <c r="AL256" s="329"/>
-      <c r="AM256" s="329"/>
-      <c r="AN256" s="329"/>
-      <c r="AO256" s="329"/>
-      <c r="AP256" s="329"/>
-      <c r="AQ256" s="329"/>
-      <c r="AR256" s="329"/>
+      <c r="AF256" s="332"/>
+      <c r="AG256" s="332"/>
+      <c r="AH256" s="332"/>
+      <c r="AI256" s="332"/>
+      <c r="AJ256" s="332"/>
+      <c r="AK256" s="332"/>
+      <c r="AL256" s="332"/>
+      <c r="AM256" s="332"/>
+      <c r="AN256" s="332"/>
+      <c r="AO256" s="332"/>
+      <c r="AP256" s="332"/>
+      <c r="AQ256" s="332"/>
+      <c r="AR256" s="332"/>
       <c r="AS256" s="119"/>
-      <c r="AT256" s="342" t="s">
+      <c r="AT256" s="345" t="s">
         <v>174</v>
       </c>
-      <c r="AU256" s="342"/>
-      <c r="AV256" s="342"/>
-      <c r="AW256" s="342"/>
-      <c r="AX256" s="342"/>
-      <c r="AY256" s="342"/>
-      <c r="AZ256" s="342"/>
-      <c r="BA256" s="342"/>
-      <c r="BB256" s="342"/>
-      <c r="BC256" s="342"/>
-      <c r="BD256" s="342"/>
-      <c r="BE256" s="342"/>
-      <c r="BF256" s="342"/>
-      <c r="BG256" s="342"/>
+      <c r="AU256" s="345"/>
+      <c r="AV256" s="345"/>
+      <c r="AW256" s="345"/>
+      <c r="AX256" s="345"/>
+      <c r="AY256" s="345"/>
+      <c r="AZ256" s="345"/>
+      <c r="BA256" s="345"/>
+      <c r="BB256" s="345"/>
+      <c r="BC256" s="345"/>
+      <c r="BD256" s="345"/>
+      <c r="BE256" s="345"/>
+      <c r="BF256" s="345"/>
+      <c r="BG256" s="345"/>
       <c r="BH256" s="119"/>
-      <c r="BI256" s="325" t="s">
+      <c r="BI256" s="328" t="s">
         <v>175</v>
       </c>
-      <c r="BJ256" s="325"/>
-      <c r="BK256" s="325"/>
-      <c r="BL256" s="325"/>
-      <c r="BM256" s="325"/>
-      <c r="BN256" s="325"/>
-      <c r="BO256" s="325"/>
-      <c r="BP256" s="325"/>
-      <c r="BQ256" s="325"/>
-      <c r="BR256" s="325"/>
-      <c r="BS256" s="325"/>
-      <c r="BT256" s="325"/>
-      <c r="BU256" s="325"/>
-      <c r="BV256" s="325"/>
+      <c r="BJ256" s="328"/>
+      <c r="BK256" s="328"/>
+      <c r="BL256" s="328"/>
+      <c r="BM256" s="328"/>
+      <c r="BN256" s="328"/>
+      <c r="BO256" s="328"/>
+      <c r="BP256" s="328"/>
+      <c r="BQ256" s="328"/>
+      <c r="BR256" s="328"/>
+      <c r="BS256" s="328"/>
+      <c r="BT256" s="328"/>
+      <c r="BU256" s="328"/>
+      <c r="BV256" s="328"/>
     </row>
     <row r="257" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="1"/>
@@ -50970,90 +50970,90 @@
       </c>
     </row>
     <row r="271" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A271" s="321" t="s">
+      <c r="A271" s="324" t="s">
         <v>176</v>
       </c>
-      <c r="B271" s="321"/>
-      <c r="C271" s="321"/>
-      <c r="D271" s="321"/>
-      <c r="E271" s="321"/>
-      <c r="F271" s="321"/>
-      <c r="G271" s="321"/>
-      <c r="H271" s="321"/>
-      <c r="I271" s="321"/>
-      <c r="J271" s="321"/>
-      <c r="K271" s="321"/>
-      <c r="L271" s="321"/>
-      <c r="M271" s="321"/>
-      <c r="N271" s="321"/>
+      <c r="B271" s="324"/>
+      <c r="C271" s="324"/>
+      <c r="D271" s="324"/>
+      <c r="E271" s="324"/>
+      <c r="F271" s="324"/>
+      <c r="G271" s="324"/>
+      <c r="H271" s="324"/>
+      <c r="I271" s="324"/>
+      <c r="J271" s="324"/>
+      <c r="K271" s="324"/>
+      <c r="L271" s="324"/>
+      <c r="M271" s="324"/>
+      <c r="N271" s="324"/>
       <c r="O271" s="119"/>
-      <c r="P271" s="321" t="s">
+      <c r="P271" s="324" t="s">
         <v>177</v>
       </c>
-      <c r="Q271" s="321"/>
-      <c r="R271" s="321"/>
-      <c r="S271" s="321"/>
-      <c r="T271" s="321"/>
-      <c r="U271" s="321"/>
-      <c r="V271" s="321"/>
-      <c r="W271" s="321"/>
-      <c r="X271" s="321"/>
-      <c r="Y271" s="321"/>
-      <c r="Z271" s="321"/>
-      <c r="AA271" s="321"/>
-      <c r="AB271" s="321"/>
-      <c r="AC271" s="321"/>
+      <c r="Q271" s="324"/>
+      <c r="R271" s="324"/>
+      <c r="S271" s="324"/>
+      <c r="T271" s="324"/>
+      <c r="U271" s="324"/>
+      <c r="V271" s="324"/>
+      <c r="W271" s="324"/>
+      <c r="X271" s="324"/>
+      <c r="Y271" s="324"/>
+      <c r="Z271" s="324"/>
+      <c r="AA271" s="324"/>
+      <c r="AB271" s="324"/>
+      <c r="AC271" s="324"/>
       <c r="AD271" s="120"/>
-      <c r="AE271" s="321" t="s">
+      <c r="AE271" s="324" t="s">
         <v>178</v>
       </c>
-      <c r="AF271" s="321"/>
-      <c r="AG271" s="321"/>
-      <c r="AH271" s="321"/>
-      <c r="AI271" s="321"/>
-      <c r="AJ271" s="321"/>
-      <c r="AK271" s="321"/>
-      <c r="AL271" s="321"/>
-      <c r="AM271" s="321"/>
-      <c r="AN271" s="321"/>
-      <c r="AO271" s="321"/>
-      <c r="AP271" s="321"/>
-      <c r="AQ271" s="321"/>
-      <c r="AR271" s="321"/>
+      <c r="AF271" s="324"/>
+      <c r="AG271" s="324"/>
+      <c r="AH271" s="324"/>
+      <c r="AI271" s="324"/>
+      <c r="AJ271" s="324"/>
+      <c r="AK271" s="324"/>
+      <c r="AL271" s="324"/>
+      <c r="AM271" s="324"/>
+      <c r="AN271" s="324"/>
+      <c r="AO271" s="324"/>
+      <c r="AP271" s="324"/>
+      <c r="AQ271" s="324"/>
+      <c r="AR271" s="324"/>
       <c r="AS271" s="119"/>
-      <c r="AT271" s="321" t="s">
+      <c r="AT271" s="324" t="s">
         <v>179</v>
       </c>
-      <c r="AU271" s="321"/>
-      <c r="AV271" s="321"/>
-      <c r="AW271" s="321"/>
-      <c r="AX271" s="321"/>
-      <c r="AY271" s="321"/>
-      <c r="AZ271" s="321"/>
-      <c r="BA271" s="321"/>
-      <c r="BB271" s="321"/>
-      <c r="BC271" s="321"/>
-      <c r="BD271" s="321"/>
-      <c r="BE271" s="321"/>
-      <c r="BF271" s="321"/>
-      <c r="BG271" s="321"/>
+      <c r="AU271" s="324"/>
+      <c r="AV271" s="324"/>
+      <c r="AW271" s="324"/>
+      <c r="AX271" s="324"/>
+      <c r="AY271" s="324"/>
+      <c r="AZ271" s="324"/>
+      <c r="BA271" s="324"/>
+      <c r="BB271" s="324"/>
+      <c r="BC271" s="324"/>
+      <c r="BD271" s="324"/>
+      <c r="BE271" s="324"/>
+      <c r="BF271" s="324"/>
+      <c r="BG271" s="324"/>
       <c r="BH271"/>
-      <c r="BI271" s="321" t="s">
+      <c r="BI271" s="324" t="s">
         <v>180</v>
       </c>
-      <c r="BJ271" s="321"/>
-      <c r="BK271" s="321"/>
-      <c r="BL271" s="321"/>
-      <c r="BM271" s="321"/>
-      <c r="BN271" s="321"/>
-      <c r="BO271" s="321"/>
-      <c r="BP271" s="321"/>
-      <c r="BQ271" s="321"/>
-      <c r="BR271" s="321"/>
-      <c r="BS271" s="321"/>
-      <c r="BT271" s="321"/>
-      <c r="BU271" s="321"/>
-      <c r="BV271" s="321"/>
+      <c r="BJ271" s="324"/>
+      <c r="BK271" s="324"/>
+      <c r="BL271" s="324"/>
+      <c r="BM271" s="324"/>
+      <c r="BN271" s="324"/>
+      <c r="BO271" s="324"/>
+      <c r="BP271" s="324"/>
+      <c r="BQ271" s="324"/>
+      <c r="BR271" s="324"/>
+      <c r="BS271" s="324"/>
+      <c r="BT271" s="324"/>
+      <c r="BU271" s="324"/>
+      <c r="BV271" s="324"/>
     </row>
     <row r="272" spans="1:74" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="1"/>
@@ -54099,124 +54099,124 @@
       <c r="CZ285" s="296"/>
     </row>
     <row r="286" spans="1:104" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A286" s="321" t="s">
+      <c r="A286" s="324" t="s">
         <v>181</v>
       </c>
-      <c r="B286" s="321"/>
-      <c r="C286" s="321"/>
-      <c r="D286" s="321"/>
-      <c r="E286" s="321"/>
-      <c r="F286" s="321"/>
-      <c r="G286" s="321"/>
-      <c r="H286" s="321"/>
-      <c r="I286" s="321"/>
-      <c r="J286" s="321"/>
-      <c r="K286" s="321"/>
-      <c r="L286" s="321"/>
-      <c r="M286" s="321"/>
-      <c r="N286" s="321"/>
+      <c r="B286" s="324"/>
+      <c r="C286" s="324"/>
+      <c r="D286" s="324"/>
+      <c r="E286" s="324"/>
+      <c r="F286" s="324"/>
+      <c r="G286" s="324"/>
+      <c r="H286" s="324"/>
+      <c r="I286" s="324"/>
+      <c r="J286" s="324"/>
+      <c r="K286" s="324"/>
+      <c r="L286" s="324"/>
+      <c r="M286" s="324"/>
+      <c r="N286" s="324"/>
       <c r="O286" s="119"/>
-      <c r="P286" s="321" t="s">
+      <c r="P286" s="324" t="s">
         <v>182</v>
       </c>
-      <c r="Q286" s="321"/>
-      <c r="R286" s="321"/>
-      <c r="S286" s="321"/>
-      <c r="T286" s="321"/>
-      <c r="U286" s="321"/>
-      <c r="V286" s="321"/>
-      <c r="W286" s="321"/>
-      <c r="X286" s="321"/>
-      <c r="Y286" s="321"/>
-      <c r="Z286" s="321"/>
-      <c r="AA286" s="321"/>
-      <c r="AB286" s="321"/>
-      <c r="AC286" s="321"/>
+      <c r="Q286" s="324"/>
+      <c r="R286" s="324"/>
+      <c r="S286" s="324"/>
+      <c r="T286" s="324"/>
+      <c r="U286" s="324"/>
+      <c r="V286" s="324"/>
+      <c r="W286" s="324"/>
+      <c r="X286" s="324"/>
+      <c r="Y286" s="324"/>
+      <c r="Z286" s="324"/>
+      <c r="AA286" s="324"/>
+      <c r="AB286" s="324"/>
+      <c r="AC286" s="324"/>
       <c r="AD286" s="120"/>
-      <c r="AE286" s="321" t="s">
+      <c r="AE286" s="324" t="s">
         <v>183</v>
       </c>
-      <c r="AF286" s="321"/>
-      <c r="AG286" s="321"/>
-      <c r="AH286" s="321"/>
-      <c r="AI286" s="321"/>
-      <c r="AJ286" s="321"/>
-      <c r="AK286" s="321"/>
-      <c r="AL286" s="321"/>
-      <c r="AM286" s="321"/>
-      <c r="AN286" s="321"/>
-      <c r="AO286" s="321"/>
-      <c r="AP286" s="321"/>
-      <c r="AQ286" s="321"/>
-      <c r="AR286" s="321"/>
+      <c r="AF286" s="324"/>
+      <c r="AG286" s="324"/>
+      <c r="AH286" s="324"/>
+      <c r="AI286" s="324"/>
+      <c r="AJ286" s="324"/>
+      <c r="AK286" s="324"/>
+      <c r="AL286" s="324"/>
+      <c r="AM286" s="324"/>
+      <c r="AN286" s="324"/>
+      <c r="AO286" s="324"/>
+      <c r="AP286" s="324"/>
+      <c r="AQ286" s="324"/>
+      <c r="AR286" s="324"/>
       <c r="AS286"/>
-      <c r="AT286" s="326" t="s">
+      <c r="AT286" s="329" t="s">
         <v>184</v>
       </c>
-      <c r="AU286" s="326"/>
-      <c r="AV286" s="326"/>
-      <c r="AW286" s="326"/>
-      <c r="AX286" s="326"/>
-      <c r="AY286" s="326"/>
-      <c r="AZ286" s="326"/>
-      <c r="BA286" s="326"/>
-      <c r="BB286" s="326"/>
-      <c r="BC286" s="326"/>
-      <c r="BD286" s="326"/>
-      <c r="BE286" s="326"/>
-      <c r="BF286" s="326"/>
-      <c r="BG286" s="326"/>
+      <c r="AU286" s="329"/>
+      <c r="AV286" s="329"/>
+      <c r="AW286" s="329"/>
+      <c r="AX286" s="329"/>
+      <c r="AY286" s="329"/>
+      <c r="AZ286" s="329"/>
+      <c r="BA286" s="329"/>
+      <c r="BB286" s="329"/>
+      <c r="BC286" s="329"/>
+      <c r="BD286" s="329"/>
+      <c r="BE286" s="329"/>
+      <c r="BF286" s="329"/>
+      <c r="BG286" s="329"/>
       <c r="BH286" s="119"/>
-      <c r="BI286" s="321" t="s">
+      <c r="BI286" s="324" t="s">
         <v>185</v>
       </c>
-      <c r="BJ286" s="321"/>
-      <c r="BK286" s="321"/>
-      <c r="BL286" s="321"/>
-      <c r="BM286" s="321"/>
-      <c r="BN286" s="321"/>
-      <c r="BO286" s="321"/>
-      <c r="BP286" s="321"/>
-      <c r="BQ286" s="321"/>
-      <c r="BR286" s="321"/>
-      <c r="BS286" s="321"/>
-      <c r="BT286" s="321"/>
-      <c r="BU286" s="321"/>
-      <c r="BV286" s="321"/>
+      <c r="BJ286" s="324"/>
+      <c r="BK286" s="324"/>
+      <c r="BL286" s="324"/>
+      <c r="BM286" s="324"/>
+      <c r="BN286" s="324"/>
+      <c r="BO286" s="324"/>
+      <c r="BP286" s="324"/>
+      <c r="BQ286" s="324"/>
+      <c r="BR286" s="324"/>
+      <c r="BS286" s="324"/>
+      <c r="BT286" s="324"/>
+      <c r="BU286" s="324"/>
+      <c r="BV286" s="324"/>
       <c r="BW286"/>
-      <c r="BX286" s="321" t="s">
+      <c r="BX286" s="324" t="s">
         <v>358</v>
       </c>
-      <c r="BY286" s="321"/>
-      <c r="BZ286" s="321"/>
-      <c r="CA286" s="321"/>
-      <c r="CB286" s="321"/>
-      <c r="CC286" s="321"/>
-      <c r="CD286" s="321"/>
-      <c r="CE286" s="321"/>
-      <c r="CF286" s="321"/>
-      <c r="CG286" s="321"/>
-      <c r="CH286" s="321"/>
-      <c r="CI286" s="321"/>
-      <c r="CJ286" s="321"/>
-      <c r="CK286" s="321"/>
+      <c r="BY286" s="324"/>
+      <c r="BZ286" s="324"/>
+      <c r="CA286" s="324"/>
+      <c r="CB286" s="324"/>
+      <c r="CC286" s="324"/>
+      <c r="CD286" s="324"/>
+      <c r="CE286" s="324"/>
+      <c r="CF286" s="324"/>
+      <c r="CG286" s="324"/>
+      <c r="CH286" s="324"/>
+      <c r="CI286" s="324"/>
+      <c r="CJ286" s="324"/>
+      <c r="CK286" s="324"/>
       <c r="CL286"/>
-      <c r="CM286" s="324" t="s">
+      <c r="CM286" s="327" t="s">
         <v>186</v>
       </c>
-      <c r="CN286" s="324"/>
-      <c r="CO286" s="324"/>
-      <c r="CP286" s="324"/>
-      <c r="CQ286" s="324"/>
-      <c r="CR286" s="324"/>
-      <c r="CS286" s="324"/>
-      <c r="CT286" s="324"/>
-      <c r="CU286" s="324"/>
-      <c r="CV286" s="324"/>
-      <c r="CW286" s="324"/>
-      <c r="CX286" s="324"/>
-      <c r="CY286" s="324"/>
-      <c r="CZ286" s="324"/>
+      <c r="CN286" s="327"/>
+      <c r="CO286" s="327"/>
+      <c r="CP286" s="327"/>
+      <c r="CQ286" s="327"/>
+      <c r="CR286" s="327"/>
+      <c r="CS286" s="327"/>
+      <c r="CT286" s="327"/>
+      <c r="CU286" s="327"/>
+      <c r="CV286" s="327"/>
+      <c r="CW286" s="327"/>
+      <c r="CX286" s="327"/>
+      <c r="CY286" s="327"/>
+      <c r="CZ286" s="327"/>
     </row>
     <row r="287" spans="1:104" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="1"/>
@@ -58480,37 +58480,37 @@
       <c r="BF302" s="288"/>
       <c r="BG302" s="288"/>
       <c r="BH302" s="66"/>
-      <c r="BI302" s="322" t="s">
+      <c r="BI302" s="325" t="s">
         <v>360</v>
       </c>
-      <c r="BJ302" s="322"/>
-      <c r="BK302" s="322"/>
-      <c r="BL302" s="322"/>
-      <c r="BM302" s="322"/>
-      <c r="BN302" s="322"/>
-      <c r="BO302" s="322"/>
-      <c r="BP302" s="322"/>
-      <c r="BQ302" s="322"/>
-      <c r="BR302" s="322"/>
-      <c r="BS302" s="322"/>
-      <c r="BT302" s="322"/>
-      <c r="BU302" s="322"/>
-      <c r="BV302" s="322"/>
-      <c r="BW302" s="322"/>
-      <c r="BX302" s="322"/>
-      <c r="BY302" s="322"/>
-      <c r="BZ302" s="322"/>
-      <c r="CA302" s="322"/>
-      <c r="CB302" s="322"/>
-      <c r="CC302" s="322"/>
-      <c r="CD302" s="322"/>
-      <c r="CE302" s="322"/>
-      <c r="CF302" s="322"/>
-      <c r="CG302" s="322"/>
-      <c r="CH302" s="322"/>
-      <c r="CI302" s="322"/>
-      <c r="CJ302" s="322"/>
-      <c r="CK302" s="322"/>
+      <c r="BJ302" s="325"/>
+      <c r="BK302" s="325"/>
+      <c r="BL302" s="325"/>
+      <c r="BM302" s="325"/>
+      <c r="BN302" s="325"/>
+      <c r="BO302" s="325"/>
+      <c r="BP302" s="325"/>
+      <c r="BQ302" s="325"/>
+      <c r="BR302" s="325"/>
+      <c r="BS302" s="325"/>
+      <c r="BT302" s="325"/>
+      <c r="BU302" s="325"/>
+      <c r="BV302" s="325"/>
+      <c r="BW302" s="325"/>
+      <c r="BX302" s="325"/>
+      <c r="BY302" s="325"/>
+      <c r="BZ302" s="325"/>
+      <c r="CA302" s="325"/>
+      <c r="CB302" s="325"/>
+      <c r="CC302" s="325"/>
+      <c r="CD302" s="325"/>
+      <c r="CE302" s="325"/>
+      <c r="CF302" s="325"/>
+      <c r="CG302" s="325"/>
+      <c r="CH302" s="325"/>
+      <c r="CI302" s="325"/>
+      <c r="CJ302" s="325"/>
+      <c r="CK302" s="325"/>
       <c r="CL302" s="66"/>
     </row>
     <row r="303" spans="1:104" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -58557,55 +58557,55 @@
       <c r="BF303" s="274"/>
       <c r="BG303" s="274"/>
       <c r="BH303" s="107"/>
-      <c r="BI303" s="321" t="s">
+      <c r="BI303" s="324" t="s">
         <v>359</v>
       </c>
-      <c r="BJ303" s="321"/>
-      <c r="BK303" s="321"/>
-      <c r="BL303" s="321"/>
-      <c r="BM303" s="321"/>
-      <c r="BN303" s="321"/>
-      <c r="BO303" s="321"/>
-      <c r="BP303" s="321"/>
-      <c r="BQ303" s="321"/>
-      <c r="BR303" s="321"/>
-      <c r="BS303" s="321"/>
-      <c r="BT303" s="321"/>
-      <c r="BU303" s="321"/>
-      <c r="BV303" s="321"/>
-      <c r="BX303" s="321" t="s">
+      <c r="BJ303" s="324"/>
+      <c r="BK303" s="324"/>
+      <c r="BL303" s="324"/>
+      <c r="BM303" s="324"/>
+      <c r="BN303" s="324"/>
+      <c r="BO303" s="324"/>
+      <c r="BP303" s="324"/>
+      <c r="BQ303" s="324"/>
+      <c r="BR303" s="324"/>
+      <c r="BS303" s="324"/>
+      <c r="BT303" s="324"/>
+      <c r="BU303" s="324"/>
+      <c r="BV303" s="324"/>
+      <c r="BX303" s="324" t="s">
         <v>287</v>
       </c>
-      <c r="BY303" s="321"/>
-      <c r="BZ303" s="321"/>
-      <c r="CA303" s="321"/>
-      <c r="CB303" s="321"/>
-      <c r="CC303" s="321"/>
-      <c r="CD303" s="321"/>
-      <c r="CE303" s="321"/>
-      <c r="CF303" s="321"/>
-      <c r="CG303" s="321"/>
-      <c r="CH303" s="321"/>
-      <c r="CI303" s="321"/>
-      <c r="CJ303" s="321"/>
-      <c r="CK303" s="321"/>
+      <c r="BY303" s="324"/>
+      <c r="BZ303" s="324"/>
+      <c r="CA303" s="324"/>
+      <c r="CB303" s="324"/>
+      <c r="CC303" s="324"/>
+      <c r="CD303" s="324"/>
+      <c r="CE303" s="324"/>
+      <c r="CF303" s="324"/>
+      <c r="CG303" s="324"/>
+      <c r="CH303" s="324"/>
+      <c r="CI303" s="324"/>
+      <c r="CJ303" s="324"/>
+      <c r="CK303" s="324"/>
       <c r="CL303" s="294"/>
-      <c r="CM303" s="321" t="s">
+      <c r="CM303" s="324" t="s">
         <v>293</v>
       </c>
-      <c r="CN303" s="321"/>
-      <c r="CO303" s="321"/>
-      <c r="CP303" s="321"/>
-      <c r="CQ303" s="321"/>
-      <c r="CR303" s="321"/>
-      <c r="CS303" s="321"/>
-      <c r="CT303" s="321"/>
-      <c r="CU303" s="321"/>
-      <c r="CV303" s="321"/>
-      <c r="CW303" s="321"/>
-      <c r="CX303" s="321"/>
-      <c r="CY303" s="321"/>
-      <c r="CZ303" s="321"/>
+      <c r="CN303" s="324"/>
+      <c r="CO303" s="324"/>
+      <c r="CP303" s="324"/>
+      <c r="CQ303" s="324"/>
+      <c r="CR303" s="324"/>
+      <c r="CS303" s="324"/>
+      <c r="CT303" s="324"/>
+      <c r="CU303" s="324"/>
+      <c r="CV303" s="324"/>
+      <c r="CW303" s="324"/>
+      <c r="CX303" s="324"/>
+      <c r="CY303" s="324"/>
+      <c r="CZ303" s="324"/>
     </row>
     <row r="304" spans="1:104" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" s="77"/>
@@ -60909,37 +60909,37 @@
       <c r="BF318" s="288"/>
       <c r="BG318" s="288"/>
       <c r="BH318" s="66"/>
-      <c r="BI318" s="322" t="s">
+      <c r="BI318" s="325" t="s">
         <v>361</v>
       </c>
-      <c r="BJ318" s="322"/>
-      <c r="BK318" s="322"/>
-      <c r="BL318" s="322"/>
-      <c r="BM318" s="322"/>
-      <c r="BN318" s="322"/>
-      <c r="BO318" s="322"/>
-      <c r="BP318" s="322"/>
-      <c r="BQ318" s="322"/>
-      <c r="BR318" s="322"/>
-      <c r="BS318" s="322"/>
-      <c r="BT318" s="322"/>
-      <c r="BU318" s="322"/>
-      <c r="BV318" s="322"/>
-      <c r="BW318" s="322"/>
-      <c r="BX318" s="322"/>
-      <c r="BY318" s="322"/>
-      <c r="BZ318" s="322"/>
-      <c r="CA318" s="322"/>
-      <c r="CB318" s="322"/>
-      <c r="CC318" s="322"/>
-      <c r="CD318" s="322"/>
-      <c r="CE318" s="322"/>
-      <c r="CF318" s="322"/>
-      <c r="CG318" s="322"/>
-      <c r="CH318" s="322"/>
-      <c r="CI318" s="322"/>
-      <c r="CJ318" s="322"/>
-      <c r="CK318" s="322"/>
+      <c r="BJ318" s="325"/>
+      <c r="BK318" s="325"/>
+      <c r="BL318" s="325"/>
+      <c r="BM318" s="325"/>
+      <c r="BN318" s="325"/>
+      <c r="BO318" s="325"/>
+      <c r="BP318" s="325"/>
+      <c r="BQ318" s="325"/>
+      <c r="BR318" s="325"/>
+      <c r="BS318" s="325"/>
+      <c r="BT318" s="325"/>
+      <c r="BU318" s="325"/>
+      <c r="BV318" s="325"/>
+      <c r="BW318" s="325"/>
+      <c r="BX318" s="325"/>
+      <c r="BY318" s="325"/>
+      <c r="BZ318" s="325"/>
+      <c r="CA318" s="325"/>
+      <c r="CB318" s="325"/>
+      <c r="CC318" s="325"/>
+      <c r="CD318" s="325"/>
+      <c r="CE318" s="325"/>
+      <c r="CF318" s="325"/>
+      <c r="CG318" s="325"/>
+      <c r="CH318" s="325"/>
+      <c r="CI318" s="325"/>
+      <c r="CJ318" s="325"/>
+      <c r="CK318" s="325"/>
       <c r="CL318" s="295"/>
       <c r="CM318" s="293"/>
       <c r="CN318" s="293"/>
@@ -60985,55 +60985,55 @@
       <c r="BE319" s="274"/>
       <c r="BF319" s="274"/>
       <c r="BG319" s="274"/>
-      <c r="BI319" s="321" t="s">
+      <c r="BI319" s="324" t="s">
         <v>359</v>
       </c>
-      <c r="BJ319" s="321"/>
-      <c r="BK319" s="321"/>
-      <c r="BL319" s="321"/>
-      <c r="BM319" s="321"/>
-      <c r="BN319" s="321"/>
-      <c r="BO319" s="321"/>
-      <c r="BP319" s="321"/>
-      <c r="BQ319" s="321"/>
-      <c r="BR319" s="321"/>
-      <c r="BS319" s="321"/>
-      <c r="BT319" s="321"/>
-      <c r="BU319" s="321"/>
-      <c r="BV319" s="321"/>
-      <c r="BX319" s="321" t="s">
+      <c r="BJ319" s="324"/>
+      <c r="BK319" s="324"/>
+      <c r="BL319" s="324"/>
+      <c r="BM319" s="324"/>
+      <c r="BN319" s="324"/>
+      <c r="BO319" s="324"/>
+      <c r="BP319" s="324"/>
+      <c r="BQ319" s="324"/>
+      <c r="BR319" s="324"/>
+      <c r="BS319" s="324"/>
+      <c r="BT319" s="324"/>
+      <c r="BU319" s="324"/>
+      <c r="BV319" s="324"/>
+      <c r="BX319" s="324" t="s">
         <v>287</v>
       </c>
-      <c r="BY319" s="321"/>
-      <c r="BZ319" s="321"/>
-      <c r="CA319" s="321"/>
-      <c r="CB319" s="321"/>
-      <c r="CC319" s="321"/>
-      <c r="CD319" s="321"/>
-      <c r="CE319" s="321"/>
-      <c r="CF319" s="321"/>
-      <c r="CG319" s="321"/>
-      <c r="CH319" s="321"/>
-      <c r="CI319" s="321"/>
-      <c r="CJ319" s="321"/>
-      <c r="CK319" s="321"/>
+      <c r="BY319" s="324"/>
+      <c r="BZ319" s="324"/>
+      <c r="CA319" s="324"/>
+      <c r="CB319" s="324"/>
+      <c r="CC319" s="324"/>
+      <c r="CD319" s="324"/>
+      <c r="CE319" s="324"/>
+      <c r="CF319" s="324"/>
+      <c r="CG319" s="324"/>
+      <c r="CH319" s="324"/>
+      <c r="CI319" s="324"/>
+      <c r="CJ319" s="324"/>
+      <c r="CK319" s="324"/>
       <c r="CL319" s="294"/>
-      <c r="CM319" s="323" t="s">
+      <c r="CM319" s="326" t="s">
         <v>291</v>
       </c>
-      <c r="CN319" s="323"/>
-      <c r="CO319" s="323"/>
-      <c r="CP319" s="323"/>
-      <c r="CQ319" s="323"/>
-      <c r="CR319" s="323"/>
-      <c r="CS319" s="323"/>
-      <c r="CT319" s="323"/>
-      <c r="CU319" s="323"/>
-      <c r="CV319" s="323"/>
-      <c r="CW319" s="323"/>
-      <c r="CX319" s="323"/>
-      <c r="CY319" s="323"/>
-      <c r="CZ319" s="323"/>
+      <c r="CN319" s="326"/>
+      <c r="CO319" s="326"/>
+      <c r="CP319" s="326"/>
+      <c r="CQ319" s="326"/>
+      <c r="CR319" s="326"/>
+      <c r="CS319" s="326"/>
+      <c r="CT319" s="326"/>
+      <c r="CU319" s="326"/>
+      <c r="CV319" s="326"/>
+      <c r="CW319" s="326"/>
+      <c r="CX319" s="326"/>
+      <c r="CY319" s="326"/>
+      <c r="CZ319" s="326"/>
     </row>
     <row r="320" spans="1:104" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" s="77"/>
@@ -63216,37 +63216,37 @@
       <c r="BF334" s="66"/>
       <c r="BG334" s="66"/>
       <c r="BH334" s="66"/>
-      <c r="BI334" s="322" t="s">
+      <c r="BI334" s="325" t="s">
         <v>362</v>
       </c>
-      <c r="BJ334" s="322"/>
-      <c r="BK334" s="322"/>
-      <c r="BL334" s="322"/>
-      <c r="BM334" s="322"/>
-      <c r="BN334" s="322"/>
-      <c r="BO334" s="322"/>
-      <c r="BP334" s="322"/>
-      <c r="BQ334" s="322"/>
-      <c r="BR334" s="322"/>
-      <c r="BS334" s="322"/>
-      <c r="BT334" s="322"/>
-      <c r="BU334" s="322"/>
-      <c r="BV334" s="322"/>
-      <c r="BW334" s="322"/>
-      <c r="BX334" s="322"/>
-      <c r="BY334" s="322"/>
-      <c r="BZ334" s="322"/>
-      <c r="CA334" s="322"/>
-      <c r="CB334" s="322"/>
-      <c r="CC334" s="322"/>
-      <c r="CD334" s="322"/>
-      <c r="CE334" s="322"/>
-      <c r="CF334" s="322"/>
-      <c r="CG334" s="322"/>
-      <c r="CH334" s="322"/>
-      <c r="CI334" s="322"/>
-      <c r="CJ334" s="322"/>
-      <c r="CK334" s="322"/>
+      <c r="BJ334" s="325"/>
+      <c r="BK334" s="325"/>
+      <c r="BL334" s="325"/>
+      <c r="BM334" s="325"/>
+      <c r="BN334" s="325"/>
+      <c r="BO334" s="325"/>
+      <c r="BP334" s="325"/>
+      <c r="BQ334" s="325"/>
+      <c r="BR334" s="325"/>
+      <c r="BS334" s="325"/>
+      <c r="BT334" s="325"/>
+      <c r="BU334" s="325"/>
+      <c r="BV334" s="325"/>
+      <c r="BW334" s="325"/>
+      <c r="BX334" s="325"/>
+      <c r="BY334" s="325"/>
+      <c r="BZ334" s="325"/>
+      <c r="CA334" s="325"/>
+      <c r="CB334" s="325"/>
+      <c r="CC334" s="325"/>
+      <c r="CD334" s="325"/>
+      <c r="CE334" s="325"/>
+      <c r="CF334" s="325"/>
+      <c r="CG334" s="325"/>
+      <c r="CH334" s="325"/>
+      <c r="CI334" s="325"/>
+      <c r="CJ334" s="325"/>
+      <c r="CK334" s="325"/>
       <c r="CL334" s="294"/>
     </row>
     <row r="335" spans="1:104" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -63280,38 +63280,38 @@
       <c r="BF335" s="274"/>
       <c r="BG335" s="274"/>
       <c r="BH335" s="107"/>
-      <c r="BI335" s="323" t="s">
+      <c r="BI335" s="326" t="s">
         <v>359</v>
       </c>
-      <c r="BJ335" s="323"/>
-      <c r="BK335" s="323"/>
-      <c r="BL335" s="323"/>
-      <c r="BM335" s="323"/>
-      <c r="BN335" s="323"/>
-      <c r="BO335" s="323"/>
-      <c r="BP335" s="323"/>
-      <c r="BQ335" s="323"/>
-      <c r="BR335" s="323"/>
-      <c r="BS335" s="323"/>
-      <c r="BT335" s="323"/>
-      <c r="BU335" s="323"/>
-      <c r="BV335" s="323"/>
-      <c r="BX335" s="323" t="s">
+      <c r="BJ335" s="326"/>
+      <c r="BK335" s="326"/>
+      <c r="BL335" s="326"/>
+      <c r="BM335" s="326"/>
+      <c r="BN335" s="326"/>
+      <c r="BO335" s="326"/>
+      <c r="BP335" s="326"/>
+      <c r="BQ335" s="326"/>
+      <c r="BR335" s="326"/>
+      <c r="BS335" s="326"/>
+      <c r="BT335" s="326"/>
+      <c r="BU335" s="326"/>
+      <c r="BV335" s="326"/>
+      <c r="BX335" s="326" t="s">
         <v>287</v>
       </c>
-      <c r="BY335" s="323"/>
-      <c r="BZ335" s="323"/>
-      <c r="CA335" s="323"/>
-      <c r="CB335" s="323"/>
-      <c r="CC335" s="323"/>
-      <c r="CD335" s="323"/>
-      <c r="CE335" s="323"/>
-      <c r="CF335" s="323"/>
-      <c r="CG335" s="323"/>
-      <c r="CH335" s="323"/>
-      <c r="CI335" s="323"/>
-      <c r="CJ335" s="323"/>
-      <c r="CK335" s="323"/>
+      <c r="BY335" s="326"/>
+      <c r="BZ335" s="326"/>
+      <c r="CA335" s="326"/>
+      <c r="CB335" s="326"/>
+      <c r="CC335" s="326"/>
+      <c r="CD335" s="326"/>
+      <c r="CE335" s="326"/>
+      <c r="CF335" s="326"/>
+      <c r="CG335" s="326"/>
+      <c r="CH335" s="326"/>
+      <c r="CI335" s="326"/>
+      <c r="CJ335" s="326"/>
+      <c r="CK335" s="326"/>
     </row>
     <row r="336" spans="1:104" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AE336" s="77"/>

</xml_diff>